<commit_message>
Set versions on CT
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC99F7B2-78B5-E645-B9B7-969098745501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA59329F-BA33-834F-A3EE-C20C20D80FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31720" yWindow="5760" windowWidth="37320" windowHeight="20560" activeTab="7" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="31720" yWindow="5760" windowWidth="37320" windowHeight="20560" firstSheet="2" activeTab="13" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="318">
   <si>
     <t>Epoch</t>
   </si>
@@ -1017,6 +1017,12 @@
   </si>
   <si>
     <t>ICD-10-CM: G30.9=Alzheimer's disease; unspecified</t>
+  </si>
+  <si>
+    <t>ICD-10=1</t>
+  </si>
+  <si>
+    <t>ICD-10-CM=1</t>
   </si>
 </sst>
 </file>
@@ -1258,13 +1264,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2436,11 +2442,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2448,7 +2452,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="29" t="s">
         <v>91</v>
       </c>
       <c r="B1" t="s">
@@ -2456,11 +2460,27 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="29" t="s">
         <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2576,36 +2596,36 @@
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="53" t="s">
         <v>276</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -2622,7 +2642,7 @@
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="52" t="s">
         <v>165</v>
       </c>
       <c r="C7" s="50"/>
@@ -2749,16 +2769,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5895,7 +5915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2F56-38DA-1440-8447-6C36029D01F5}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add initial narrative content for LZZT
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6D0C9C-3862-684A-8FE7-5980D765FBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A7CF4A-A203-9A49-9A68-96DA52E13DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31720" yWindow="5760" windowWidth="37320" windowHeight="20560" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="44780" yWindow="500" windowWidth="44440" windowHeight="25820" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
-    <sheet name="studyIdentifiers" sheetId="3" r:id="rId2"/>
-    <sheet name="studyDesign" sheetId="4" r:id="rId3"/>
-    <sheet name="studyDesignArms" sheetId="14" r:id="rId4"/>
-    <sheet name="studyDesignEpochs" sheetId="15" r:id="rId5"/>
-    <sheet name="mainTimeline" sheetId="1" r:id="rId6"/>
-    <sheet name="studyDesignII" sheetId="6" r:id="rId7"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId8"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId9"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId10"/>
-    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId11"/>
-    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId12"/>
-    <sheet name="studyDesignElements" sheetId="13" r:id="rId13"/>
-    <sheet name="configuration" sheetId="10" r:id="rId14"/>
+    <sheet name="studyDesignContent" sheetId="16" r:id="rId2"/>
+    <sheet name="studyIdentifiers" sheetId="3" r:id="rId3"/>
+    <sheet name="studyDesign" sheetId="4" r:id="rId4"/>
+    <sheet name="studyDesignArms" sheetId="14" r:id="rId5"/>
+    <sheet name="studyDesignEpochs" sheetId="15" r:id="rId6"/>
+    <sheet name="mainTimeline" sheetId="1" r:id="rId7"/>
+    <sheet name="studyDesignII" sheetId="6" r:id="rId8"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId9"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId10"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId11"/>
+    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId12"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId13"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId14"/>
+    <sheet name="configuration" sheetId="10" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="586">
   <si>
     <t>Epoch</t>
   </si>
@@ -1026,6 +1027,815 @@
   </si>
   <si>
     <t>None set</t>
+  </si>
+  <si>
+    <t>sectionNumber</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sectionTitle</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>PROTOCOL SUMMARY</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Protocol Synopsis</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Trial Schema</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Schedule of Activities</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>INTRODUCTION</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Purpose of Trial</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>Summary of Benefits and Risks</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TRIAL OBJECTIVES, ENDPOINTS AND ESTIMANDS</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>TRIAL DESIGN</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>Description of Trial Design</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>Participant Input into Design</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>Rationale for Trial Design</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>Rationale for Comparator</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>Rationale for Adaptive or Novel Trial Design</t>
+  </si>
+  <si>
+    <t>4.2.3</t>
+  </si>
+  <si>
+    <t>Other Trial Design Considerations</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>Access to Trial Intervention After End of Trial</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>Start of Trial and End of Trial</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>TRIAL POPULATION</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>Selection of Trial Population</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>Rationale for Trial Population</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>Inclusion Criteria</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Inclusion criteria are:&lt;/p&gt;
+&lt;ul&gt;
+  &lt;li&gt;1. Something&lt;/li&gt;
+  &lt;li&gt;2. Something else&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>Exclusion Criteria</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Exclusion criteria are:&lt;/p&gt;
+&lt;ul&gt;
+  &lt;li&gt;1. Dont do this&lt;/li&gt;
+  &lt;li&gt;2. And don't do that&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>Lifestyle Considerations</t>
+  </si>
+  <si>
+    <t>5.5.1</t>
+  </si>
+  <si>
+    <t>Meals and Dietary Restrictions</t>
+  </si>
+  <si>
+    <t>5.5.2</t>
+  </si>
+  <si>
+    <t>Caffeine, Alcohol, Tobacco, and Other Habits</t>
+  </si>
+  <si>
+    <t>5.5.3</t>
+  </si>
+  <si>
+    <t>Physical Activity</t>
+  </si>
+  <si>
+    <t>5.5.4</t>
+  </si>
+  <si>
+    <t>Other Activity</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>Screen Failures</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>TRIAL INTERVENTION AND CONCOMITANT THERAPY</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>Description of Trial Intervention</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>Rationale for Trial Intervention</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>Dosing and Administration</t>
+  </si>
+  <si>
+    <t>6.3.1</t>
+  </si>
+  <si>
+    <t>Trial Intervention Dose Modification</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>Treatment of Overdose</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>Preparation, Handling, Storage and Accountability</t>
+  </si>
+  <si>
+    <t>6.5.1</t>
+  </si>
+  <si>
+    <t>Preparation of Trial Intervention</t>
+  </si>
+  <si>
+    <t>6.5.2</t>
+  </si>
+  <si>
+    <t>Handling and Storage of Trial Intervention</t>
+  </si>
+  <si>
+    <t>6.5.3</t>
+  </si>
+  <si>
+    <t>Accountability of Trial Intervention</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>Participant Assignment, Randomisation and Blinding</t>
+  </si>
+  <si>
+    <t>6.6.1</t>
+  </si>
+  <si>
+    <t>Participant Assignment</t>
+  </si>
+  <si>
+    <t>6.6.2</t>
+  </si>
+  <si>
+    <t>Randomisation</t>
+  </si>
+  <si>
+    <t>6.6.3</t>
+  </si>
+  <si>
+    <t>Blinding and Unblinding</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Blinding and unblinding text here please&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <t>Trial Intervention Compliance</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>Concomitant Therapy</t>
+  </si>
+  <si>
+    <t>6.8.1</t>
+  </si>
+  <si>
+    <t>Prohibited Concomitant Therapy</t>
+  </si>
+  <si>
+    <t>6.8.2</t>
+  </si>
+  <si>
+    <t>Permitted Concomitant Therapy</t>
+  </si>
+  <si>
+    <t>6.8.3</t>
+  </si>
+  <si>
+    <t>Rescue Therapy</t>
+  </si>
+  <si>
+    <t>6.8.4</t>
+  </si>
+  <si>
+    <t>Other Therapy</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>DISCONTINUATION OF TRIAL INTERVENTION AND PARTICIPANT WITHDRAWAL FROM TRIAL</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>Discontinuation of Trial Intervention</t>
+  </si>
+  <si>
+    <t>7.1.1</t>
+  </si>
+  <si>
+    <t>Criteria for Permanent Discontinuation of Trial Intervention</t>
+  </si>
+  <si>
+    <t>7.1.2</t>
+  </si>
+  <si>
+    <t>Temporary Discontinuation or Interruption of Trial Intervention</t>
+  </si>
+  <si>
+    <t>7.1.3</t>
+  </si>
+  <si>
+    <t>Rechallenge</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>Participant Withdrawal from the Trial</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>Lost to Follow-Up</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>Trial Stopping Rules</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>TRIAL ASSESSMENTS AND PROCEDURES</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>Screening/Baseline Assessments and Procedures</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>Efficacy Assessments and Procedures</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>Safety Assessments and Procedures</t>
+  </si>
+  <si>
+    <t>8.3.1</t>
+  </si>
+  <si>
+    <t>Physical Examination</t>
+  </si>
+  <si>
+    <t>8.3.2</t>
+  </si>
+  <si>
+    <t>Vital Signs</t>
+  </si>
+  <si>
+    <t>8.3.3</t>
+  </si>
+  <si>
+    <t>Electrocardiograms</t>
+  </si>
+  <si>
+    <t>8.3.4</t>
+  </si>
+  <si>
+    <t>Clinical Laboratory Assessments</t>
+  </si>
+  <si>
+    <t>8.3.5</t>
+  </si>
+  <si>
+    <t>Suicidal Ideation and Behaviour Risk Monitoring</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>Adverse Events and Serious Adverse Events</t>
+  </si>
+  <si>
+    <t>8.4.1</t>
+  </si>
+  <si>
+    <t>Definitions of AE and SAE</t>
+  </si>
+  <si>
+    <t>8.4.2</t>
+  </si>
+  <si>
+    <t>Time Period and Frequency for Collecting AE and SAE Information</t>
+  </si>
+  <si>
+    <t>8.4.3</t>
+  </si>
+  <si>
+    <t>Identifying AEs and SAEs</t>
+  </si>
+  <si>
+    <t>8.4.4</t>
+  </si>
+  <si>
+    <t>Recording of AEs and SAEs</t>
+  </si>
+  <si>
+    <t>8.4.5</t>
+  </si>
+  <si>
+    <t>Follow-up of AEs and SAEs</t>
+  </si>
+  <si>
+    <t>8.4.6</t>
+  </si>
+  <si>
+    <t>Reporting of SAEs</t>
+  </si>
+  <si>
+    <t>8.4.7</t>
+  </si>
+  <si>
+    <t>Regulatory Reporting Requirements for SAEs</t>
+  </si>
+  <si>
+    <t>8.4.8</t>
+  </si>
+  <si>
+    <t>Serious and Unexpected Adverse Reaction Reporting</t>
+  </si>
+  <si>
+    <t>8.4.9</t>
+  </si>
+  <si>
+    <t>Adverse Events of Special Interest</t>
+  </si>
+  <si>
+    <t>8.4.10</t>
+  </si>
+  <si>
+    <t>Disease-related Events or Outcomes Not Qualifying as AEs or SAEs</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>Pregnancy and Postpartum Information</t>
+  </si>
+  <si>
+    <t>8.5.1</t>
+  </si>
+  <si>
+    <t>Participants Who Become Pregnant During the Trial</t>
+  </si>
+  <si>
+    <t>8.5.2</t>
+  </si>
+  <si>
+    <t>Participants Whose Partners Become Pregnant</t>
+  </si>
+  <si>
+    <t>8.6</t>
+  </si>
+  <si>
+    <t>Medical Device Product Complaints for Drug/Device Combination Products</t>
+  </si>
+  <si>
+    <t>8.6.1</t>
+  </si>
+  <si>
+    <t>Definition of Medical Device Product Complaints</t>
+  </si>
+  <si>
+    <t>8.6.2</t>
+  </si>
+  <si>
+    <t>Recording of Medical Device Product Complaints</t>
+  </si>
+  <si>
+    <t>8.6.3</t>
+  </si>
+  <si>
+    <t>Time Period and Frequency for Collecting Medical Device Product Complaints .</t>
+  </si>
+  <si>
+    <t>8.6.4</t>
+  </si>
+  <si>
+    <t>Follow-Up of Medical Device Product Complaints</t>
+  </si>
+  <si>
+    <t>8.6.5</t>
+  </si>
+  <si>
+    <t>Regulatory Reporting Requirements for Medical Device Product Complaints</t>
+  </si>
+  <si>
+    <t>8.7</t>
+  </si>
+  <si>
+    <t>Pharmacokinetics</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>Genetics</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>Biomarkers</t>
+  </si>
+  <si>
+    <t>Immunogenicity Assessments</t>
+  </si>
+  <si>
+    <t>8.1.1</t>
+  </si>
+  <si>
+    <t>Medical Resource Utilisation and Health Economics</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>STATISTICAL CONSIDERATIONS</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>Analysis Sets</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>Analyses Supporting Primary Objective(s)</t>
+  </si>
+  <si>
+    <t>9.2.1</t>
+  </si>
+  <si>
+    <t>Statistical Model, Hypothesis, and Method of Analysis</t>
+  </si>
+  <si>
+    <t>9.2.2</t>
+  </si>
+  <si>
+    <t>Handling of Intercurrent Events of Primary Estimand(s)</t>
+  </si>
+  <si>
+    <t>9.2.3</t>
+  </si>
+  <si>
+    <t>Handling of Missing Data</t>
+  </si>
+  <si>
+    <t>9.2.4</t>
+  </si>
+  <si>
+    <t>Sensitivity Analysis</t>
+  </si>
+  <si>
+    <t>9.2.5</t>
+  </si>
+  <si>
+    <t>Supplementary Analysis</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>Analysis Supporting Secondary Objective(s)</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>Analysis of Exploratory Objective(s)</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>Safety Analyses</t>
+  </si>
+  <si>
+    <t>9.6</t>
+  </si>
+  <si>
+    <t>Other Analyses</t>
+  </si>
+  <si>
+    <t>9.7</t>
+  </si>
+  <si>
+    <t>Interim Analyses</t>
+  </si>
+  <si>
+    <t>9.8</t>
+  </si>
+  <si>
+    <t>Sample Size Determination</t>
+  </si>
+  <si>
+    <t>9.9</t>
+  </si>
+  <si>
+    <t>Protocol Deviations</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>GENERAL CONSIDERATIONS: REGULATORY, ETHICAL, AND TRIAL OVERSIGHT</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>Regulatory and Ethical Considerations</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>Committees</t>
+  </si>
+  <si>
+    <t>10.3</t>
+  </si>
+  <si>
+    <t>Informed Consent Process</t>
+  </si>
+  <si>
+    <t>10.4</t>
+  </si>
+  <si>
+    <t>Data Protection</t>
+  </si>
+  <si>
+    <t>10.5</t>
+  </si>
+  <si>
+    <t>Early Site Closure or Trial Termination</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>GENERAL CONSIDERATIONS: RISK MANAGEMENT AND QUALITY ASSURANCE</t>
+  </si>
+  <si>
+    <t>11.1</t>
+  </si>
+  <si>
+    <t>Quality Tolerance Limits</t>
+  </si>
+  <si>
+    <t>11.2</t>
+  </si>
+  <si>
+    <t>Data Quality Assurance</t>
+  </si>
+  <si>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t>Source Data</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>APPENDIX: ADVERSE EVENTS AND SERIOUS ADVERSE EVENTS - DEFINITIONS, SEVERITY, AND CAUSALITY</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>Further Details and Clarifications on the AE Definition</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t>Further Details and Clarifications on the SAE Definition</t>
+  </si>
+  <si>
+    <t>12.3</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>12.4</t>
+  </si>
+  <si>
+    <t>Causality</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>APPENDIX: DEFINITIONS AND SUPPORTING OPERATIONAL DETAILS</t>
+  </si>
+  <si>
+    <t>13.1</t>
+  </si>
+  <si>
+    <t>Contraception and Pregnancy Testing</t>
+  </si>
+  <si>
+    <t>13.1.1</t>
+  </si>
+  <si>
+    <t>Definitions Related to Childbearing Potential</t>
+  </si>
+  <si>
+    <t>13.1.2</t>
+  </si>
+  <si>
+    <t>Contraception</t>
+  </si>
+  <si>
+    <t>13.1.3</t>
+  </si>
+  <si>
+    <t>Pregnancy Testing</t>
+  </si>
+  <si>
+    <t>13.2</t>
+  </si>
+  <si>
+    <t>Clinical Laboratory Tests</t>
+  </si>
+  <si>
+    <t>13.3</t>
+  </si>
+  <si>
+    <t>Country/Region-Specific Differences</t>
+  </si>
+  <si>
+    <t>13.4</t>
+  </si>
+  <si>
+    <t>Prior Protocol Amendments</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>APPENDIX: GLOSSARY OF TERMS</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>APPENDIX: REFERENCES</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1096,7 +1906,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1115,6 +1925,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1128,7 +1944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1267,16 +2083,22 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1594,7 +2416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1722,6 +2544,334 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="3" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="59.5" customWidth="1"/>
+    <col min="6" max="7" width="31.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" t="s">
+        <v>255</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>286</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>257</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="G8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E9" t="s">
+        <v>235</v>
+      </c>
+      <c r="G9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D036654E-7FF8-D440-BC0A-D74BC57BB3C9}">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -1771,7 +2921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E6393-3A18-464C-A40D-B41879707264}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -1842,7 +2992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4E9D5-B601-284A-9651-0AA604C2B9D1}">
   <dimension ref="A1:AF36"/>
   <sheetViews>
@@ -2301,7 +3451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FA5DC6-70BE-E845-A085-20526138A835}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -2445,7 +3595,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2495,6 +3645,1241 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
+  <dimension ref="A1:D137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="16" style="3" customWidth="1"/>
+    <col min="3" max="3" width="49.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="81.33203125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="55" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" s="56"/>
+      <c r="C2" s="6" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="B13" s="56"/>
+      <c r="C13" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="B14" s="56"/>
+      <c r="C14" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="B15" s="56"/>
+      <c r="C15" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="B16" s="56"/>
+      <c r="C16" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="B17" s="56"/>
+      <c r="C17" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="B18" s="56"/>
+      <c r="C18" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="B19" s="56"/>
+      <c r="C19" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="B20" s="56"/>
+      <c r="C20" s="6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>361</v>
+      </c>
+      <c r="B21" s="56"/>
+      <c r="C21" s="6" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="B22" s="56"/>
+      <c r="C22" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="B23" s="56"/>
+      <c r="C23" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="B24" s="56"/>
+      <c r="C24" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="B25" s="56"/>
+      <c r="C25" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="B26" s="56"/>
+      <c r="C26" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="B27" s="56"/>
+      <c r="C27" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="B28" s="56"/>
+      <c r="C28" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="B29" s="56"/>
+      <c r="C29" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="B30" s="56"/>
+      <c r="C30" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="B31" s="56"/>
+      <c r="C31" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="B32" s="56"/>
+      <c r="C32" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="B33" s="56"/>
+      <c r="C33" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="B34" s="56"/>
+      <c r="C34" s="6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="B35" s="56"/>
+      <c r="C35" s="6" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="B36" s="56"/>
+      <c r="C36" s="6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="B37" s="56"/>
+      <c r="C37" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
+        <v>397</v>
+      </c>
+      <c r="B38" s="56"/>
+      <c r="C38" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="B39" s="56"/>
+      <c r="C39" s="6" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="B40" s="56"/>
+      <c r="C40" s="6" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="B41" s="56"/>
+      <c r="C41" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="B42" s="56"/>
+      <c r="C42" s="6" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
+        <v>407</v>
+      </c>
+      <c r="B43" s="56"/>
+      <c r="C43" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
+        <v>410</v>
+      </c>
+      <c r="B44" s="56"/>
+      <c r="C44" s="6" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="15" t="s">
+        <v>412</v>
+      </c>
+      <c r="B45" s="56"/>
+      <c r="C45" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="B46" s="56"/>
+      <c r="C46" s="6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="B47" s="56"/>
+      <c r="C47" s="6" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="B48" s="56"/>
+      <c r="C48" s="6" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="15" t="s">
+        <v>420</v>
+      </c>
+      <c r="B49" s="56"/>
+      <c r="C49" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="B50" s="56"/>
+      <c r="C50" s="6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="B51" s="56"/>
+      <c r="C51" s="6" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="B52" s="56"/>
+      <c r="C52" s="6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="B53" s="56"/>
+      <c r="C53" s="6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="B54" s="56"/>
+      <c r="C54" s="6" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="B55" s="56"/>
+      <c r="C55" s="6" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="B56" s="56"/>
+      <c r="C56" s="6" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
+        <v>436</v>
+      </c>
+      <c r="B57" s="56"/>
+      <c r="C57" s="6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="B58" s="56"/>
+      <c r="C58" s="6" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="B59" s="56"/>
+      <c r="C59" s="6" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="B60" s="56"/>
+      <c r="C60" s="6" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="B61" s="56"/>
+      <c r="C61" s="6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="B62" s="56"/>
+      <c r="C62" s="6" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="B63" s="56"/>
+      <c r="C63" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="B64" s="56"/>
+      <c r="C64" s="6" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="15" t="s">
+        <v>452</v>
+      </c>
+      <c r="B65" s="56"/>
+      <c r="C65" s="6" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="B66" s="56"/>
+      <c r="C66" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="B67" s="56"/>
+      <c r="C67" s="6" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="15" t="s">
+        <v>458</v>
+      </c>
+      <c r="B68" s="56"/>
+      <c r="C68" s="6" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A69" s="15" t="s">
+        <v>460</v>
+      </c>
+      <c r="B69" s="56"/>
+      <c r="C69" s="6" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="B70" s="56"/>
+      <c r="C70" s="6" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="B71" s="56"/>
+      <c r="C71" s="6" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="B72" s="56"/>
+      <c r="C72" s="6" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="B73" s="56"/>
+      <c r="C73" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="15" t="s">
+        <v>470</v>
+      </c>
+      <c r="B74" s="56"/>
+      <c r="C74" s="6" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="15" t="s">
+        <v>472</v>
+      </c>
+      <c r="B75" s="56"/>
+      <c r="C75" s="6" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="15" t="s">
+        <v>474</v>
+      </c>
+      <c r="B76" s="56"/>
+      <c r="C76" s="6" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" s="15" t="s">
+        <v>476</v>
+      </c>
+      <c r="B77" s="56"/>
+      <c r="C77" s="6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="15" t="s">
+        <v>478</v>
+      </c>
+      <c r="B78" s="56"/>
+      <c r="C78" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="B79" s="56"/>
+      <c r="C79" s="6" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="15" t="s">
+        <v>482</v>
+      </c>
+      <c r="B80" s="56"/>
+      <c r="C80" s="6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A81" s="15" t="s">
+        <v>484</v>
+      </c>
+      <c r="B81" s="56"/>
+      <c r="C81" s="6" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="15" t="s">
+        <v>486</v>
+      </c>
+      <c r="B82" s="56"/>
+      <c r="C82" s="6" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="B83" s="56"/>
+      <c r="C83" s="6" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" s="15" t="s">
+        <v>490</v>
+      </c>
+      <c r="B84" s="56"/>
+      <c r="C84" s="6" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="15" t="s">
+        <v>492</v>
+      </c>
+      <c r="B85" s="56"/>
+      <c r="C85" s="6" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B86" s="56"/>
+      <c r="C86" s="6" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="B87" s="56"/>
+      <c r="C87" s="6" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="B88" s="56"/>
+      <c r="C88" s="6" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="B89" s="56"/>
+      <c r="C89" s="6" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="B90" s="56"/>
+      <c r="C90" s="6" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="B91" s="56"/>
+      <c r="C91" s="6" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="15" t="s">
+        <v>505</v>
+      </c>
+      <c r="B92" s="56"/>
+      <c r="C92" s="6" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="B93" s="56"/>
+      <c r="C93" s="6" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="15" t="s">
+        <v>509</v>
+      </c>
+      <c r="B94" s="56"/>
+      <c r="C94" s="6" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="15" t="s">
+        <v>511</v>
+      </c>
+      <c r="B95" s="56"/>
+      <c r="C95" s="6" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="15" t="s">
+        <v>513</v>
+      </c>
+      <c r="B96" s="56"/>
+      <c r="C96" s="6" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="15" t="s">
+        <v>515</v>
+      </c>
+      <c r="B97" s="56"/>
+      <c r="C97" s="6" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="15" t="s">
+        <v>517</v>
+      </c>
+      <c r="B98" s="56"/>
+      <c r="C98" s="6" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="B99" s="56"/>
+      <c r="C99" s="6" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="15" t="s">
+        <v>521</v>
+      </c>
+      <c r="B100" s="56"/>
+      <c r="C100" s="6" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B101" s="56"/>
+      <c r="C101" s="6" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="15" t="s">
+        <v>525</v>
+      </c>
+      <c r="B102" s="56"/>
+      <c r="C102" s="6" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="B103" s="56"/>
+      <c r="C103" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="15" t="s">
+        <v>529</v>
+      </c>
+      <c r="B104" s="56"/>
+      <c r="C104" s="6" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="15" t="s">
+        <v>531</v>
+      </c>
+      <c r="B105" s="56"/>
+      <c r="C105" s="6" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="15" t="s">
+        <v>533</v>
+      </c>
+      <c r="B106" s="56"/>
+      <c r="C106" s="6" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A107" s="15" t="s">
+        <v>535</v>
+      </c>
+      <c r="B107" s="56"/>
+      <c r="C107" s="6" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="15" t="s">
+        <v>537</v>
+      </c>
+      <c r="B108" s="56"/>
+      <c r="C108" s="6" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="15" t="s">
+        <v>539</v>
+      </c>
+      <c r="B109" s="56"/>
+      <c r="C109" s="6" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="15" t="s">
+        <v>541</v>
+      </c>
+      <c r="B110" s="56"/>
+      <c r="C110" s="6" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B111" s="56"/>
+      <c r="C111" s="6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="15" t="s">
+        <v>545</v>
+      </c>
+      <c r="B112" s="56"/>
+      <c r="C112" s="6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A113" s="15" t="s">
+        <v>547</v>
+      </c>
+      <c r="B113" s="56"/>
+      <c r="C113" s="6" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="B114" s="56"/>
+      <c r="C114" s="6" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="15" t="s">
+        <v>551</v>
+      </c>
+      <c r="B115" s="56"/>
+      <c r="C115" s="6" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="15" t="s">
+        <v>553</v>
+      </c>
+      <c r="B116" s="56"/>
+      <c r="C116" s="6" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A117" s="15" t="s">
+        <v>555</v>
+      </c>
+      <c r="B117" s="56"/>
+      <c r="C117" s="6" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="15" t="s">
+        <v>557</v>
+      </c>
+      <c r="B118" s="56"/>
+      <c r="C118" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="B119" s="56"/>
+      <c r="C119" s="6" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="B120" s="56"/>
+      <c r="C120" s="6" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="15" t="s">
+        <v>563</v>
+      </c>
+      <c r="B121" s="56"/>
+      <c r="C121" s="6" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A122" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="B122" s="56"/>
+      <c r="C122" s="6" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="15" t="s">
+        <v>567</v>
+      </c>
+      <c r="B123" s="56"/>
+      <c r="C123" s="6" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="15" t="s">
+        <v>569</v>
+      </c>
+      <c r="B124" s="56"/>
+      <c r="C124" s="6" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="15" t="s">
+        <v>571</v>
+      </c>
+      <c r="B125" s="56"/>
+      <c r="C125" s="6" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="15" t="s">
+        <v>573</v>
+      </c>
+      <c r="B126" s="56"/>
+      <c r="C126" s="6" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" s="15" t="s">
+        <v>575</v>
+      </c>
+      <c r="B127" s="56"/>
+      <c r="C127" s="6" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="15" t="s">
+        <v>577</v>
+      </c>
+      <c r="B128" s="56"/>
+      <c r="C128" s="6" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="15" t="s">
+        <v>579</v>
+      </c>
+      <c r="B129" s="56"/>
+      <c r="C129" s="6" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A130" s="15" t="s">
+        <v>581</v>
+      </c>
+      <c r="B130" s="56"/>
+      <c r="C130" s="6" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="15" t="s">
+        <v>583</v>
+      </c>
+      <c r="B131" s="56"/>
+      <c r="C131" s="6" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="15" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="15" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="15" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="15" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="15" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="15" t="s">
+        <v>585</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A054F5-5F55-D04A-9603-B97FC15141C8}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -2557,7 +4942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AA03AF-8646-874D-935F-A73550A0FA0C}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -2601,36 +4986,36 @@
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="53" t="s">
         <v>276</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -2647,7 +5032,7 @@
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="52" t="s">
         <v>165</v>
       </c>
       <c r="C7" s="50"/>
@@ -2774,16 +5159,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2791,7 +5176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB09339-52DA-2A44-9E81-01CB7197E815}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2881,7 +5266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740737DA-2EE9-3B48-882B-C915DB285C6C}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -2967,7 +5352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:X69"/>
   <sheetViews>
@@ -5853,7 +8238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46FA45D-9570-C643-AC7B-6310BD62121C}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -5916,7 +8301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2F56-38DA-1440-8447-6C36029D01F5}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -5971,332 +8356,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
-  <dimension ref="A1:K22"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="59.5" customWidth="1"/>
-    <col min="6" max="7" width="31.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>259</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>273</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="41" t="s">
-        <v>254</v>
-      </c>
-      <c r="G3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" t="s">
-        <v>255</v>
-      </c>
-      <c r="G5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" ht="119" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" t="s">
-        <v>286</v>
-      </c>
-      <c r="F6" s="41" t="s">
-        <v>287</v>
-      </c>
-      <c r="G6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>234</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>260</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="s">
-        <v>256</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>279</v>
-      </c>
-      <c r="G7" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
-        <v>257</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>280</v>
-      </c>
-      <c r="G8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
-        <v>258</v>
-      </c>
-      <c r="E9" t="s">
-        <v>235</v>
-      </c>
-      <c r="G9" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add LZZt Inclusion and Blinding info
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A7CF4A-A203-9A49-9A68-96DA52E13DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9376223-8EAB-1F40-954A-CE38577AFBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44780" yWindow="500" windowWidth="44440" windowHeight="25820" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="585">
   <si>
     <t>Epoch</t>
   </si>
@@ -1167,26 +1167,12 @@
     <t>Inclusion Criteria</t>
   </si>
   <si>
-    <t>&lt;p&gt;Inclusion criteria are:&lt;/p&gt;
-&lt;ul&gt;
-  &lt;li&gt;1. Something&lt;/li&gt;
-  &lt;li&gt;2. Something else&lt;/li&gt;
-&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>5.4</t>
   </si>
   <si>
     <t>Exclusion Criteria</t>
   </si>
   <si>
-    <t>&lt;p&gt;Exclusion criteria are:&lt;/p&gt;
-&lt;ul&gt;
-  &lt;li&gt;1. Dont do this&lt;/li&gt;
-  &lt;li&gt;2. And don't do that&lt;/li&gt;
-&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>5.5</t>
   </si>
   <si>
@@ -1307,9 +1293,6 @@
     <t>Blinding and Unblinding</t>
   </si>
   <si>
-    <t>&lt;p&gt;Blinding and unblinding text here please&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>6.7</t>
   </si>
   <si>
@@ -1836,6 +1819,88 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>&lt;p&gt;The study will be double-blind. To further preserve the blinding of the study, only a minimum number of Lilly and CRO personnel will see the randomization table and codes before the study is complete.&lt;/p&gt;
+&lt;p&gt;Emergency codes generated by a computer drug-labeling system will be available to the investigator. These codes, which reveal the patients treatment group, may be opened during the study only if the choice of follow-up treatment depends on the patient’s therapy assignment.&lt;/p&gt;
+&lt;p&gt;The investigator should make every effort to contact the clinical research physician prior to unblinding a patient’s therapy assignment. If a patient’s therapy assignment is unblinded, Lilly must be notified immediately by telephone. After the study, the investigator must return all sealed and any opened codes.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Patients may be included in the study only if they meet &lt;strong&gt;all&lt;/strong&gt; the following criteria:&lt;/p&gt;
+&lt;table&gt;
+  &lt;tr&gt;
+    &lt;td&gt;[1]&lt;/td&gt;
+    &lt;td&gt;
+      Males and postmenopausal females at least 50 years of age.
+    &lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;td&gt;[2]&lt;/td&gt;
+    &lt;td&gt;Diagnosis of probable AD as defined by National Institute of Neurological and Communicative Disorders and Stroke
+      (NINCDS) and the Alzheimer’s Disease and Related Disorders Association (ADRDA) guidelines (Attachment LZZT.7).
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;td&gt;[3]&lt;/td&gt;
+    &lt;td&gt;MMSE score of 10 to 23.&lt;/td&gt; 
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;td&gt;[4]&lt;/td&gt;
+    &lt;td&gt;Hachinski Ischemic Scale score of ≤4 (Attachment LZZT.8).&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;td&gt;[5]&lt;/td&gt;
+    &lt;td&gt;CNS imaging (CT scan or MRI of brain) compatible with AD within past 1 year.
+      The following findings are incompatible with AD:
+      &lt;ol type="a"&gt;
+        &lt;li&gt;Large vessel strokes
+          &lt;ol type="1"&gt;
+            &lt;li&gt;Any definite area of encephalomalacia consistent with ischemic necrosis in any cerebral artery
+              territory.&lt;/li&gt;
+            &lt;li&gt;Large, confluent areas of encephalomalacia in parieto-occipital or frontal regions consistent with
+              watershed infarcts. The above are exclusionary. Exceptions are made for small areas of cortical asymmetry
+              which may represent a small cortical stroke or a focal area of atrophy provided there is no abnormal
+              signal intensity in the immediately underlying parenchyma. Only one such questionable area allowed per
+              scan, and size is restricted to ≤1cm in frontal/parietal/temporal cortices and ≤2 cm in occipital cortex.
+            &lt;/li&gt;
+          &lt;/ol&gt;
+        &lt;/li&gt;
+        &lt;li&gt;Small vessel ischemia
+          &lt;ol type="1"&gt;
+            &lt;li&gt;Lacunar infarct is defined as an area of abnormal intensity seen on CT scan or on both T1 and T2
+              weighted MRI images in the basal ganglia, thalamus or deep white matter which is ≤1 cm in maximal
+              diameter. A maximum of one lacune is allowed per scan.&lt;/li&gt;
+            &lt;li&gt;Leukoariosis or leukoencephalopathy is regarded as an abnormality seen on T2 but not T1 weighted MRIs,
+              or on CT. This is accepted if mild or moderate in extent, meaning involvement of less than 25% of cortical
+              white matter.&lt;/li&gt;
+          &lt;/ol&gt;
+        &lt;/li&gt;
+        &lt;li&gt;Miscellaneous
+          &lt;ol type="1"&gt;
+            &lt;li&gt;Benign small extra-axial tumors (ie, meningiomas) are accepted if they do not contact or indent the
+              brain parenchyma.&lt;/li&gt;
+            &lt;li&gt;extra-axial arachnoid cysts are accepted if they do not indent or deform the brain parenchyma.&lt;/li&gt;
+          &lt;/ol&gt;
+        &lt;/li&gt;
+      &lt;/ol&gt;
+    &lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;td&gt;[6]&lt;/td&gt;
+    &lt;td&gt;Investigator has obtained informed consent signed by the patient (and/or legal representative) and by the
+      caregiver.&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;td&gt;[7]&lt;/td&gt;
+    &lt;td&gt;Geographic proximity to investigator’s site that allows adequate follow-up.&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;td&gt;[8]&lt;/td&gt;
+    &lt;td&gt;A reliable caregiver who is in frequent or daily contact with the patient and who will accompany the patient to
+      the office and/or be available by telephone at designated times, will monitor administration of prescribed
+      medications, and will be responsible for the overall care of the patient at home. The caregiver and the patient
+      must be able to communicate in English and willing to comply with 26 weeks of transdermal therapy.&lt;/td&gt;
+  &lt;/tr&gt;
+&lt;table&gt;</t>
   </si>
 </sst>
 </file>
@@ -2079,8 +2144,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2089,16 +2163,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3648,8 +3713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3661,10 +3726,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="50" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="50" t="s">
         <v>320</v>
       </c>
       <c r="C1" s="35" t="s">
@@ -3678,7 +3743,7 @@
       <c r="A2" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="56"/>
+      <c r="B2" s="51"/>
       <c r="C2" s="6" t="s">
         <v>324</v>
       </c>
@@ -3759,7 +3824,7 @@
       <c r="A12" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="B12" s="56"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="6" t="s">
         <v>344</v>
       </c>
@@ -3768,7 +3833,7 @@
       <c r="A13" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="B13" s="56"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="6" t="s">
         <v>346</v>
       </c>
@@ -3777,7 +3842,7 @@
       <c r="A14" s="15" t="s">
         <v>347</v>
       </c>
-      <c r="B14" s="56"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="6" t="s">
         <v>348</v>
       </c>
@@ -3786,7 +3851,7 @@
       <c r="A15" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="B15" s="56"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="6" t="s">
         <v>350</v>
       </c>
@@ -3795,7 +3860,7 @@
       <c r="A16" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="B16" s="56"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="6" t="s">
         <v>352</v>
       </c>
@@ -3804,7 +3869,7 @@
       <c r="A17" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="6" t="s">
         <v>354</v>
       </c>
@@ -3813,7 +3878,7 @@
       <c r="A18" s="15" t="s">
         <v>355</v>
       </c>
-      <c r="B18" s="56"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="6" t="s">
         <v>356</v>
       </c>
@@ -3822,7 +3887,7 @@
       <c r="A19" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="B19" s="56"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="6" t="s">
         <v>358</v>
       </c>
@@ -3831,7 +3896,7 @@
       <c r="A20" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="6" t="s">
         <v>360</v>
       </c>
@@ -3840,1038 +3905,1035 @@
       <c r="A21" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="B21" s="56"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="6" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="B22" s="56"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="6" t="s">
         <v>364</v>
       </c>
       <c r="D22" s="6" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
+      <c r="B23" s="51"/>
+      <c r="C23" s="6" t="s">
         <v>366</v>
-      </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>369</v>
-      </c>
-      <c r="B24" s="56"/>
+        <v>367</v>
+      </c>
+      <c r="B24" s="51"/>
       <c r="C24" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>371</v>
-      </c>
-      <c r="B25" s="56"/>
+        <v>369</v>
+      </c>
+      <c r="B25" s="51"/>
       <c r="C25" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>373</v>
-      </c>
-      <c r="B26" s="56"/>
+        <v>371</v>
+      </c>
+      <c r="B26" s="51"/>
       <c r="C26" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>375</v>
-      </c>
-      <c r="B27" s="56"/>
+        <v>373</v>
+      </c>
+      <c r="B27" s="51"/>
       <c r="C27" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="B28" s="56"/>
+        <v>375</v>
+      </c>
+      <c r="B28" s="51"/>
       <c r="C28" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="B29" s="56"/>
+        <v>377</v>
+      </c>
+      <c r="B29" s="51"/>
       <c r="C29" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="B30" s="56"/>
+        <v>379</v>
+      </c>
+      <c r="B30" s="51"/>
       <c r="C30" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="B31" s="56"/>
+        <v>381</v>
+      </c>
+      <c r="B31" s="51"/>
       <c r="C31" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>385</v>
-      </c>
-      <c r="B32" s="56"/>
+        <v>383</v>
+      </c>
+      <c r="B32" s="51"/>
       <c r="C32" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>387</v>
-      </c>
-      <c r="B33" s="56"/>
+        <v>385</v>
+      </c>
+      <c r="B33" s="51"/>
       <c r="C33" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>389</v>
-      </c>
-      <c r="B34" s="56"/>
+        <v>387</v>
+      </c>
+      <c r="B34" s="51"/>
       <c r="C34" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>391</v>
-      </c>
-      <c r="B35" s="56"/>
+        <v>389</v>
+      </c>
+      <c r="B35" s="51"/>
       <c r="C35" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>393</v>
-      </c>
-      <c r="B36" s="56"/>
+        <v>391</v>
+      </c>
+      <c r="B36" s="51"/>
       <c r="C36" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="B37" s="56"/>
+        <v>393</v>
+      </c>
+      <c r="B37" s="51"/>
       <c r="C37" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>397</v>
-      </c>
-      <c r="B38" s="56"/>
+        <v>395</v>
+      </c>
+      <c r="B38" s="51"/>
       <c r="C38" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>399</v>
-      </c>
-      <c r="B39" s="56"/>
+        <v>397</v>
+      </c>
+      <c r="B39" s="51"/>
       <c r="C39" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>401</v>
-      </c>
-      <c r="B40" s="56"/>
+        <v>399</v>
+      </c>
+      <c r="B40" s="51"/>
       <c r="C40" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>403</v>
-      </c>
-      <c r="B41" s="56"/>
+        <v>401</v>
+      </c>
+      <c r="B41" s="51"/>
       <c r="C41" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="B42" s="51"/>
+      <c r="C42" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+      <c r="A43" s="15" t="s">
         <v>405</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="6" t="s">
+      <c r="B43" s="51"/>
+      <c r="C43" s="6" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="B43" s="56"/>
-      <c r="C43" s="6" t="s">
-        <v>408</v>
-      </c>
       <c r="D43" s="6" t="s">
-        <v>409</v>
+        <v>583</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>410</v>
-      </c>
-      <c r="B44" s="56"/>
+        <v>407</v>
+      </c>
+      <c r="B44" s="51"/>
       <c r="C44" s="6" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>412</v>
-      </c>
-      <c r="B45" s="56"/>
+        <v>409</v>
+      </c>
+      <c r="B45" s="51"/>
       <c r="C45" s="6" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>414</v>
-      </c>
-      <c r="B46" s="56"/>
+        <v>411</v>
+      </c>
+      <c r="B46" s="51"/>
       <c r="C46" s="6" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="B47" s="56"/>
+        <v>413</v>
+      </c>
+      <c r="B47" s="51"/>
       <c r="C47" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>418</v>
-      </c>
-      <c r="B48" s="56"/>
+        <v>415</v>
+      </c>
+      <c r="B48" s="51"/>
       <c r="C48" s="6" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>420</v>
-      </c>
-      <c r="B49" s="56"/>
+        <v>417</v>
+      </c>
+      <c r="B49" s="51"/>
       <c r="C49" s="6" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>422</v>
-      </c>
-      <c r="B50" s="56"/>
+        <v>419</v>
+      </c>
+      <c r="B50" s="51"/>
       <c r="C50" s="6" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="B51" s="56"/>
+        <v>421</v>
+      </c>
+      <c r="B51" s="51"/>
       <c r="C51" s="6" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>426</v>
-      </c>
-      <c r="B52" s="56"/>
+        <v>423</v>
+      </c>
+      <c r="B52" s="51"/>
       <c r="C52" s="6" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>428</v>
-      </c>
-      <c r="B53" s="56"/>
+        <v>425</v>
+      </c>
+      <c r="B53" s="51"/>
       <c r="C53" s="6" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>430</v>
-      </c>
-      <c r="B54" s="56"/>
+        <v>427</v>
+      </c>
+      <c r="B54" s="51"/>
       <c r="C54" s="6" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>432</v>
-      </c>
-      <c r="B55" s="56"/>
+        <v>429</v>
+      </c>
+      <c r="B55" s="51"/>
       <c r="C55" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>434</v>
-      </c>
-      <c r="B56" s="56"/>
+        <v>431</v>
+      </c>
+      <c r="B56" s="51"/>
       <c r="C56" s="6" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>436</v>
-      </c>
-      <c r="B57" s="56"/>
+        <v>433</v>
+      </c>
+      <c r="B57" s="51"/>
       <c r="C57" s="6" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>438</v>
-      </c>
-      <c r="B58" s="56"/>
+        <v>435</v>
+      </c>
+      <c r="B58" s="51"/>
       <c r="C58" s="6" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>440</v>
-      </c>
-      <c r="B59" s="56"/>
+        <v>437</v>
+      </c>
+      <c r="B59" s="51"/>
       <c r="C59" s="6" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>442</v>
-      </c>
-      <c r="B60" s="56"/>
+        <v>439</v>
+      </c>
+      <c r="B60" s="51"/>
       <c r="C60" s="6" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
-        <v>444</v>
-      </c>
-      <c r="B61" s="56"/>
+        <v>441</v>
+      </c>
+      <c r="B61" s="51"/>
       <c r="C61" s="6" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>446</v>
-      </c>
-      <c r="B62" s="56"/>
+        <v>443</v>
+      </c>
+      <c r="B62" s="51"/>
       <c r="C62" s="6" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>448</v>
-      </c>
-      <c r="B63" s="56"/>
+        <v>445</v>
+      </c>
+      <c r="B63" s="51"/>
       <c r="C63" s="6" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>450</v>
-      </c>
-      <c r="B64" s="56"/>
+        <v>447</v>
+      </c>
+      <c r="B64" s="51"/>
       <c r="C64" s="6" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>452</v>
-      </c>
-      <c r="B65" s="56"/>
+        <v>449</v>
+      </c>
+      <c r="B65" s="51"/>
       <c r="C65" s="6" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>454</v>
-      </c>
-      <c r="B66" s="56"/>
+        <v>451</v>
+      </c>
+      <c r="B66" s="51"/>
       <c r="C66" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
-        <v>456</v>
-      </c>
-      <c r="B67" s="56"/>
+        <v>453</v>
+      </c>
+      <c r="B67" s="51"/>
       <c r="C67" s="6" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
-        <v>458</v>
-      </c>
-      <c r="B68" s="56"/>
+        <v>455</v>
+      </c>
+      <c r="B68" s="51"/>
       <c r="C68" s="6" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
-        <v>460</v>
-      </c>
-      <c r="B69" s="56"/>
+        <v>457</v>
+      </c>
+      <c r="B69" s="51"/>
       <c r="C69" s="6" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
-        <v>462</v>
-      </c>
-      <c r="B70" s="56"/>
+        <v>459</v>
+      </c>
+      <c r="B70" s="51"/>
       <c r="C70" s="6" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>464</v>
-      </c>
-      <c r="B71" s="56"/>
+        <v>461</v>
+      </c>
+      <c r="B71" s="51"/>
       <c r="C71" s="6" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>466</v>
-      </c>
-      <c r="B72" s="56"/>
+        <v>463</v>
+      </c>
+      <c r="B72" s="51"/>
       <c r="C72" s="6" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>468</v>
-      </c>
-      <c r="B73" s="56"/>
+        <v>465</v>
+      </c>
+      <c r="B73" s="51"/>
       <c r="C73" s="6" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
-        <v>470</v>
-      </c>
-      <c r="B74" s="56"/>
+        <v>467</v>
+      </c>
+      <c r="B74" s="51"/>
       <c r="C74" s="6" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="15" t="s">
-        <v>472</v>
-      </c>
-      <c r="B75" s="56"/>
+        <v>469</v>
+      </c>
+      <c r="B75" s="51"/>
       <c r="C75" s="6" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
-        <v>474</v>
-      </c>
-      <c r="B76" s="56"/>
+        <v>471</v>
+      </c>
+      <c r="B76" s="51"/>
       <c r="C76" s="6" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="15" t="s">
-        <v>476</v>
-      </c>
-      <c r="B77" s="56"/>
+        <v>473</v>
+      </c>
+      <c r="B77" s="51"/>
       <c r="C77" s="6" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>478</v>
-      </c>
-      <c r="B78" s="56"/>
+        <v>475</v>
+      </c>
+      <c r="B78" s="51"/>
       <c r="C78" s="6" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
-        <v>480</v>
-      </c>
-      <c r="B79" s="56"/>
+        <v>477</v>
+      </c>
+      <c r="B79" s="51"/>
       <c r="C79" s="6" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
-        <v>482</v>
-      </c>
-      <c r="B80" s="56"/>
+        <v>479</v>
+      </c>
+      <c r="B80" s="51"/>
       <c r="C80" s="6" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="15" t="s">
-        <v>484</v>
-      </c>
-      <c r="B81" s="56"/>
+        <v>481</v>
+      </c>
+      <c r="B81" s="51"/>
       <c r="C81" s="6" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
-        <v>486</v>
-      </c>
-      <c r="B82" s="56"/>
+        <v>483</v>
+      </c>
+      <c r="B82" s="51"/>
       <c r="C82" s="6" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="s">
-        <v>488</v>
-      </c>
-      <c r="B83" s="56"/>
+        <v>485</v>
+      </c>
+      <c r="B83" s="51"/>
       <c r="C83" s="6" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
-        <v>490</v>
-      </c>
-      <c r="B84" s="56"/>
+        <v>487</v>
+      </c>
+      <c r="B84" s="51"/>
       <c r="C84" s="6" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="B85" s="56"/>
+        <v>489</v>
+      </c>
+      <c r="B85" s="51"/>
       <c r="C85" s="6" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
-        <v>494</v>
-      </c>
-      <c r="B86" s="56"/>
+        <v>491</v>
+      </c>
+      <c r="B86" s="51"/>
       <c r="C86" s="6" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="s">
-        <v>496</v>
-      </c>
-      <c r="B87" s="56"/>
+        <v>493</v>
+      </c>
+      <c r="B87" s="51"/>
       <c r="C87" s="6" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
-        <v>498</v>
-      </c>
-      <c r="B88" s="56"/>
+        <v>495</v>
+      </c>
+      <c r="B88" s="51"/>
       <c r="C88" s="6" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="15" t="s">
-        <v>500</v>
-      </c>
-      <c r="B89" s="56"/>
+        <v>497</v>
+      </c>
+      <c r="B89" s="51"/>
       <c r="C89" s="6" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
-        <v>440</v>
-      </c>
-      <c r="B90" s="56"/>
+        <v>437</v>
+      </c>
+      <c r="B90" s="51"/>
       <c r="C90" s="6" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="s">
-        <v>503</v>
-      </c>
-      <c r="B91" s="56"/>
+        <v>500</v>
+      </c>
+      <c r="B91" s="51"/>
       <c r="C91" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
-        <v>505</v>
-      </c>
-      <c r="B92" s="56"/>
+        <v>502</v>
+      </c>
+      <c r="B92" s="51"/>
       <c r="C92" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="s">
-        <v>507</v>
-      </c>
-      <c r="B93" s="56"/>
+        <v>504</v>
+      </c>
+      <c r="B93" s="51"/>
       <c r="C93" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
-        <v>509</v>
-      </c>
-      <c r="B94" s="56"/>
+        <v>506</v>
+      </c>
+      <c r="B94" s="51"/>
       <c r="C94" s="6" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="s">
-        <v>511</v>
-      </c>
-      <c r="B95" s="56"/>
+        <v>508</v>
+      </c>
+      <c r="B95" s="51"/>
       <c r="C95" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="s">
-        <v>513</v>
-      </c>
-      <c r="B96" s="56"/>
+        <v>510</v>
+      </c>
+      <c r="B96" s="51"/>
       <c r="C96" s="6" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="s">
-        <v>515</v>
-      </c>
-      <c r="B97" s="56"/>
+        <v>512</v>
+      </c>
+      <c r="B97" s="51"/>
       <c r="C97" s="6" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
-        <v>517</v>
-      </c>
-      <c r="B98" s="56"/>
+        <v>514</v>
+      </c>
+      <c r="B98" s="51"/>
       <c r="C98" s="6" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="15" t="s">
-        <v>519</v>
-      </c>
-      <c r="B99" s="56"/>
+        <v>516</v>
+      </c>
+      <c r="B99" s="51"/>
       <c r="C99" s="6" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="15" t="s">
-        <v>521</v>
-      </c>
-      <c r="B100" s="56"/>
+        <v>518</v>
+      </c>
+      <c r="B100" s="51"/>
       <c r="C100" s="6" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="s">
-        <v>523</v>
-      </c>
-      <c r="B101" s="56"/>
+        <v>520</v>
+      </c>
+      <c r="B101" s="51"/>
       <c r="C101" s="6" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="15" t="s">
-        <v>525</v>
-      </c>
-      <c r="B102" s="56"/>
+        <v>522</v>
+      </c>
+      <c r="B102" s="51"/>
       <c r="C102" s="6" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="s">
-        <v>527</v>
-      </c>
-      <c r="B103" s="56"/>
+        <v>524</v>
+      </c>
+      <c r="B103" s="51"/>
       <c r="C103" s="6" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="s">
-        <v>529</v>
-      </c>
-      <c r="B104" s="56"/>
+        <v>526</v>
+      </c>
+      <c r="B104" s="51"/>
       <c r="C104" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="s">
-        <v>531</v>
-      </c>
-      <c r="B105" s="56"/>
+        <v>528</v>
+      </c>
+      <c r="B105" s="51"/>
       <c r="C105" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="s">
-        <v>533</v>
-      </c>
-      <c r="B106" s="56"/>
+        <v>530</v>
+      </c>
+      <c r="B106" s="51"/>
       <c r="C106" s="6" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="s">
-        <v>535</v>
-      </c>
-      <c r="B107" s="56"/>
+        <v>532</v>
+      </c>
+      <c r="B107" s="51"/>
       <c r="C107" s="6" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="s">
-        <v>537</v>
-      </c>
-      <c r="B108" s="56"/>
+        <v>534</v>
+      </c>
+      <c r="B108" s="51"/>
       <c r="C108" s="6" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="s">
-        <v>539</v>
-      </c>
-      <c r="B109" s="56"/>
+        <v>536</v>
+      </c>
+      <c r="B109" s="51"/>
       <c r="C109" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="s">
-        <v>541</v>
-      </c>
-      <c r="B110" s="56"/>
+        <v>538</v>
+      </c>
+      <c r="B110" s="51"/>
       <c r="C110" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="15" t="s">
-        <v>543</v>
-      </c>
-      <c r="B111" s="56"/>
+        <v>540</v>
+      </c>
+      <c r="B111" s="51"/>
       <c r="C111" s="6" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="15" t="s">
-        <v>545</v>
-      </c>
-      <c r="B112" s="56"/>
+        <v>542</v>
+      </c>
+      <c r="B112" s="51"/>
       <c r="C112" s="6" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="15" t="s">
-        <v>547</v>
-      </c>
-      <c r="B113" s="56"/>
+        <v>544</v>
+      </c>
+      <c r="B113" s="51"/>
       <c r="C113" s="6" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="15" t="s">
-        <v>549</v>
-      </c>
-      <c r="B114" s="56"/>
+        <v>546</v>
+      </c>
+      <c r="B114" s="51"/>
       <c r="C114" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="15" t="s">
-        <v>551</v>
-      </c>
-      <c r="B115" s="56"/>
+        <v>548</v>
+      </c>
+      <c r="B115" s="51"/>
       <c r="C115" s="6" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="15" t="s">
-        <v>553</v>
-      </c>
-      <c r="B116" s="56"/>
+        <v>550</v>
+      </c>
+      <c r="B116" s="51"/>
       <c r="C116" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="15" t="s">
-        <v>555</v>
-      </c>
-      <c r="B117" s="56"/>
+        <v>552</v>
+      </c>
+      <c r="B117" s="51"/>
       <c r="C117" s="6" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="15" t="s">
-        <v>557</v>
-      </c>
-      <c r="B118" s="56"/>
+        <v>554</v>
+      </c>
+      <c r="B118" s="51"/>
       <c r="C118" s="6" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="15" t="s">
-        <v>559</v>
-      </c>
-      <c r="B119" s="56"/>
+        <v>556</v>
+      </c>
+      <c r="B119" s="51"/>
       <c r="C119" s="6" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
-        <v>561</v>
-      </c>
-      <c r="B120" s="56"/>
+        <v>558</v>
+      </c>
+      <c r="B120" s="51"/>
       <c r="C120" s="6" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="15" t="s">
-        <v>563</v>
-      </c>
-      <c r="B121" s="56"/>
+        <v>560</v>
+      </c>
+      <c r="B121" s="51"/>
       <c r="C121" s="6" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" s="15" t="s">
-        <v>565</v>
-      </c>
-      <c r="B122" s="56"/>
+        <v>562</v>
+      </c>
+      <c r="B122" s="51"/>
       <c r="C122" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="B123" s="56"/>
+        <v>564</v>
+      </c>
+      <c r="B123" s="51"/>
       <c r="C123" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="15" t="s">
-        <v>569</v>
-      </c>
-      <c r="B124" s="56"/>
+        <v>566</v>
+      </c>
+      <c r="B124" s="51"/>
       <c r="C124" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="15" t="s">
-        <v>571</v>
-      </c>
-      <c r="B125" s="56"/>
+        <v>568</v>
+      </c>
+      <c r="B125" s="51"/>
       <c r="C125" s="6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="15" t="s">
-        <v>573</v>
-      </c>
-      <c r="B126" s="56"/>
+        <v>570</v>
+      </c>
+      <c r="B126" s="51"/>
       <c r="C126" s="6" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="15" t="s">
-        <v>575</v>
-      </c>
-      <c r="B127" s="56"/>
+        <v>572</v>
+      </c>
+      <c r="B127" s="51"/>
       <c r="C127" s="6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="15" t="s">
-        <v>577</v>
-      </c>
-      <c r="B128" s="56"/>
+        <v>574</v>
+      </c>
+      <c r="B128" s="51"/>
       <c r="C128" s="6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="15" t="s">
-        <v>579</v>
-      </c>
-      <c r="B129" s="56"/>
+        <v>576</v>
+      </c>
+      <c r="B129" s="51"/>
       <c r="C129" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="15" t="s">
-        <v>581</v>
-      </c>
-      <c r="B130" s="56"/>
+        <v>578</v>
+      </c>
+      <c r="B130" s="51"/>
       <c r="C130" s="6" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="15" t="s">
-        <v>583</v>
-      </c>
-      <c r="B131" s="56"/>
+        <v>580</v>
+      </c>
+      <c r="B131" s="51"/>
       <c r="C131" s="6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="15" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="15" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="15" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="15" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="15" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="15" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -4962,25 +5024,25 @@
       <c r="A1" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="52" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -5010,65 +5072,65 @@
       <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
     </row>
     <row r="7" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="55" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
@@ -5159,16 +5221,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5393,28 +5455,28 @@
       <c r="C1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56" t="s">
         <v>201</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
       <c r="T1" s="1" t="s">
         <v>272</v>
       </c>

</xml_diff>

<commit_message>
Add simple html strip utility
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D350BA10-0E7D-B748-9CC9-F933C1B004A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1052284F-856C-034C-A3C9-54E0BFAB4B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44780" yWindow="500" windowWidth="44440" windowHeight="25820" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -820,10 +820,6 @@
     <t>50 years</t>
   </si>
   <si>
-    <t>Video-referenced Clinician’s Interview-based Impression of Change (CIBIC+) at
-Week 24</t>
-  </si>
-  <si>
     <t>Vital signs (weight, standing and supine blood pressure, heart rate)</t>
   </si>
   <si>
@@ -882,18 +878,6 @@
     <t>Treatment 3</t>
   </si>
   <si>
-    <t>Alzheimer\'s Disease Assessment Scale - Cognitive Subscale, total of 11 items
-[ADAS-Cog (11)] at Week 24</t>
-  </si>
-  <si>
-    <t>Safety and Efficacy of the Xanomeline Transdermal Therapeutic System (TTS) in Patients with Mild to Moderate Alzheimer\’s Disease</t>
-  </si>
-  <si>
-    <t>Safety and Efficacy of the Xanomeline
-Transdermal Therapeutic System (TTS) in Patients
-with Mild to Moderate Alzheimer\’s Disease</t>
-  </si>
-  <si>
     <t>SPONSOR: MILD_MOD_ALZ=Mild to Moderate Alzheimer\'s Disease, SNOMED: 26929004=Alzheimer\'s disease</t>
   </si>
   <si>
@@ -905,14 +889,6 @@
 Moderate Alzheimer\'s Disease</t>
   </si>
   <si>
-    <t>Alzheimer\'s Disease Assessment Scale - Cognitive Subscale, total of 11 items
-[ADAS-Cog (11)] at Weeks 8 and 16</t>
-  </si>
-  <si>
-    <t>Video-referenced Clinician\’s Interview-based Impression of Change (CIBIC+) at
-Weeks 8 and 16</t>
-  </si>
-  <si>
     <t>H2Q-MC-LZZT</t>
   </si>
   <si>
@@ -929,11 +905,6 @@
   </si>
   <si>
     <t>Laboratory evaluations (Change from Baseline)</t>
-  </si>
-  <si>
-    <t>The change from baseline laboratory value will be 
-calculated as the difference between the baseline lab value and the endpoint value (i.e.,
-the value at the specified visit) or the end of treatment observation</t>
   </si>
   <si>
     <t>Xanomeline High Dose</t>
@@ -1902,12 +1873,35 @@
   &lt;/tr&gt;
 &lt;table&gt;</t>
   </si>
+  <si>
+    <t>Safety and Efficacy of the Xanomeline Transdermal Therapeutic System (TTS) in Patients with Mild to Moderate Alzheimer’s Disease</t>
+  </si>
+  <si>
+    <t>Safety and Efficacy of the Xanomeline
+Transdermal Therapeutic System (TTS) in Patients
+with Mild to Moderate Alzheimer’s Disease</t>
+  </si>
+  <si>
+    <t>Alzheimer's Disease Assessment Scale - Cognitive Subscale, total of 11 items [ADAS-Cog (11)] at Week 24</t>
+  </si>
+  <si>
+    <t>Video-referenced Clinician’s Interview-based Impression of Change (CIBIC+) at Week 24</t>
+  </si>
+  <si>
+    <t>Alzheimer's Disease Assessment Scale - Cognitive Subscale, total of 11 items [ADAS-Cog (11)] at Weeks 8 and 16</t>
+  </si>
+  <si>
+    <t>Video-referenced Clinician’s Interview-based Impression of Change (CIBIC+) at Weeks 8 and 16</t>
+  </si>
+  <si>
+    <t>The change from baseline laboratory value will be  calculated as the difference between the baseline lab value and the endpoint value (i.e., the value at the specified visit) or the end of treatment observation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1951,12 +1945,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2009,7 +1997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2061,15 +2049,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -2092,11 +2071,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2120,10 +2099,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -2154,17 +2133,30 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2481,14 +2473,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="98.1640625" customWidth="1"/>
+    <col min="2" max="2" width="71" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
@@ -2500,8 +2492,8 @@
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="30" t="s">
-        <v>274</v>
+      <c r="B1" s="27" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2533,10 +2525,10 @@
         <v>78</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="106" customHeight="1" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>79</v>
       </c>
@@ -2578,27 +2570,27 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:8" s="58" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>275</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>278</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="B10" s="55" t="s">
+        <v>579</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>274</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>311</v>
+      </c>
+      <c r="E10" s="56">
         <v>1</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="21">
+      <c r="F10" s="56"/>
+      <c r="G10" s="57">
         <v>38718</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="56" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2612,39 +2604,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="59.5" customWidth="1"/>
-    <col min="6" max="7" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="15" customWidth="1"/>
+    <col min="2" max="2" width="44" style="15" customWidth="1"/>
+    <col min="3" max="4" width="18.83203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="59.5" style="15" customWidth="1"/>
+    <col min="6" max="7" width="31.5" style="15" customWidth="1"/>
+    <col min="8" max="11" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="18" t="s">
         <v>57</v>
       </c>
       <c r="I1" s="6"/>
@@ -2652,36 +2645,36 @@
       <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>259</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="41" t="s">
-        <v>273</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E2" s="19" t="s">
+        <v>580</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>58</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
+    <row r="3" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="D3" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="41" t="s">
-        <v>254</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E3" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>58</v>
       </c>
       <c r="I3" s="6"/>
@@ -2689,22 +2682,22 @@
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="15" t="s">
         <v>58</v>
       </c>
       <c r="I4" s="6"/>
@@ -2712,30 +2705,30 @@
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
+      <c r="D5" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E5" t="s">
-        <v>255</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="E5" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>58</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="119" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
+    <row r="6" spans="1:11" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E6" t="s">
-        <v>286</v>
-      </c>
-      <c r="F6" s="41" t="s">
-        <v>287</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="E6" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>584</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>58</v>
       </c>
       <c r="I6" s="6"/>
@@ -2743,36 +2736,36 @@
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="B7" s="41" t="s">
-        <v>260</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D7" t="s">
-        <v>256</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>279</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="D7" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="G7" s="15" t="s">
         <v>61</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
-        <v>257</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>280</v>
-      </c>
-      <c r="G8" t="s">
+    <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="D8" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>583</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="I8" s="6"/>
@@ -2780,13 +2773,13 @@
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
-        <v>258</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="15" t="s">
         <v>61</v>
       </c>
       <c r="I9" s="6"/>
@@ -3000,8 +2993,8 @@
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" style="41" customWidth="1"/>
-    <col min="6" max="6" width="24" style="27" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="24" style="24" customWidth="1"/>
     <col min="7" max="7" width="29.6640625" customWidth="1"/>
     <col min="8" max="8" width="14.83203125" customWidth="1"/>
   </cols>
@@ -3010,22 +3003,22 @@
       <c r="A1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>311</v>
-      </c>
-      <c r="D1" s="25" t="s">
+      <c r="B1" s="22" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="22" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3034,16 +3027,16 @@
         <v>107</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="15"/>
@@ -3077,28 +3070,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="32" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3241,7 +3234,7 @@
       <c r="A8" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="29" t="s">
         <v>229</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -3282,7 +3275,7 @@
         <v>132</v>
       </c>
       <c r="B10" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C10" t="s">
         <v>179</v>
@@ -3396,7 +3389,7 @@
       <c r="F15" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="H15" s="36"/>
+      <c r="H15" s="33"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -3534,19 +3527,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3571,13 +3564,13 @@
       <c r="A3" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>168</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="29" t="s">
         <v>240</v>
       </c>
     </row>
@@ -3591,7 +3584,7 @@
       <c r="C4" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="29" t="s">
         <v>240</v>
       </c>
     </row>
@@ -3613,13 +3606,13 @@
       <c r="A6" t="s">
         <v>151</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="29" t="s">
         <v>245</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="29" t="s">
         <v>246</v>
       </c>
     </row>
@@ -3627,13 +3620,13 @@
       <c r="A7" t="s">
         <v>237</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="29" t="s">
         <v>248</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="29" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3647,10 +3640,10 @@
       <c r="C8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="40" t="s">
         <v>251</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="40" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3672,7 +3665,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>91</v>
       </c>
       <c r="B1" t="s">
@@ -3680,7 +3673,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
         <v>91</v>
       </c>
       <c r="B2" t="s">
@@ -3688,19 +3681,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -3713,8 +3706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3726,1214 +3719,1214 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
-        <v>319</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>320</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>321</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>322</v>
+      <c r="A1" s="47" t="s">
+        <v>312</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>323</v>
-      </c>
-      <c r="B2" s="51"/>
+        <v>316</v>
+      </c>
+      <c r="B2" s="48"/>
       <c r="C2" s="6" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="B12" s="51"/>
+        <v>336</v>
+      </c>
+      <c r="B12" s="48"/>
       <c r="C12" s="6" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="B13" s="51"/>
+        <v>338</v>
+      </c>
+      <c r="B13" s="48"/>
       <c r="C13" s="6" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>347</v>
-      </c>
-      <c r="B14" s="51"/>
+        <v>340</v>
+      </c>
+      <c r="B14" s="48"/>
       <c r="C14" s="6" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="B15" s="51"/>
+        <v>342</v>
+      </c>
+      <c r="B15" s="48"/>
       <c r="C15" s="6" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="B16" s="51"/>
+        <v>344</v>
+      </c>
+      <c r="B16" s="48"/>
       <c r="C16" s="6" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="B17" s="51"/>
+        <v>346</v>
+      </c>
+      <c r="B17" s="48"/>
       <c r="C17" s="6" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="B18" s="51"/>
+        <v>348</v>
+      </c>
+      <c r="B18" s="48"/>
       <c r="C18" s="6" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>357</v>
-      </c>
-      <c r="B19" s="51"/>
+        <v>350</v>
+      </c>
+      <c r="B19" s="48"/>
       <c r="C19" s="6" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>359</v>
-      </c>
-      <c r="B20" s="51"/>
+        <v>352</v>
+      </c>
+      <c r="B20" s="48"/>
       <c r="C20" s="6" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>361</v>
-      </c>
-      <c r="B21" s="51"/>
+        <v>354</v>
+      </c>
+      <c r="B21" s="48"/>
       <c r="C21" s="6" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>363</v>
-      </c>
-      <c r="B22" s="51"/>
+        <v>356</v>
+      </c>
+      <c r="B22" s="48"/>
       <c r="C22" s="6" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>365</v>
-      </c>
-      <c r="B23" s="51"/>
+        <v>358</v>
+      </c>
+      <c r="B23" s="48"/>
       <c r="C23" s="6" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>367</v>
-      </c>
-      <c r="B24" s="51"/>
+        <v>360</v>
+      </c>
+      <c r="B24" s="48"/>
       <c r="C24" s="6" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>369</v>
-      </c>
-      <c r="B25" s="51"/>
+        <v>362</v>
+      </c>
+      <c r="B25" s="48"/>
       <c r="C25" s="6" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>371</v>
-      </c>
-      <c r="B26" s="51"/>
+        <v>364</v>
+      </c>
+      <c r="B26" s="48"/>
       <c r="C26" s="6" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>373</v>
-      </c>
-      <c r="B27" s="51"/>
+        <v>366</v>
+      </c>
+      <c r="B27" s="48"/>
       <c r="C27" s="6" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>375</v>
-      </c>
-      <c r="B28" s="51"/>
+        <v>368</v>
+      </c>
+      <c r="B28" s="48"/>
       <c r="C28" s="6" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="B29" s="51"/>
+        <v>370</v>
+      </c>
+      <c r="B29" s="48"/>
       <c r="C29" s="6" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>379</v>
-      </c>
-      <c r="B30" s="51"/>
+        <v>372</v>
+      </c>
+      <c r="B30" s="48"/>
       <c r="C30" s="6" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="B31" s="51"/>
+        <v>374</v>
+      </c>
+      <c r="B31" s="48"/>
       <c r="C31" s="6" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="B32" s="51"/>
+        <v>376</v>
+      </c>
+      <c r="B32" s="48"/>
       <c r="C32" s="6" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>385</v>
-      </c>
-      <c r="B33" s="51"/>
+        <v>378</v>
+      </c>
+      <c r="B33" s="48"/>
       <c r="C33" s="6" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>387</v>
-      </c>
-      <c r="B34" s="51"/>
+        <v>380</v>
+      </c>
+      <c r="B34" s="48"/>
       <c r="C34" s="6" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>389</v>
-      </c>
-      <c r="B35" s="51"/>
+        <v>382</v>
+      </c>
+      <c r="B35" s="48"/>
       <c r="C35" s="6" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>391</v>
-      </c>
-      <c r="B36" s="51"/>
+        <v>384</v>
+      </c>
+      <c r="B36" s="48"/>
       <c r="C36" s="6" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>393</v>
-      </c>
-      <c r="B37" s="51"/>
+        <v>386</v>
+      </c>
+      <c r="B37" s="48"/>
       <c r="C37" s="6" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="B38" s="51"/>
+        <v>388</v>
+      </c>
+      <c r="B38" s="48"/>
       <c r="C38" s="6" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>397</v>
-      </c>
-      <c r="B39" s="51"/>
+        <v>390</v>
+      </c>
+      <c r="B39" s="48"/>
       <c r="C39" s="6" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>399</v>
-      </c>
-      <c r="B40" s="51"/>
+        <v>392</v>
+      </c>
+      <c r="B40" s="48"/>
       <c r="C40" s="6" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>401</v>
-      </c>
-      <c r="B41" s="51"/>
+        <v>394</v>
+      </c>
+      <c r="B41" s="48"/>
       <c r="C41" s="6" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>403</v>
-      </c>
-      <c r="B42" s="51"/>
+        <v>396</v>
+      </c>
+      <c r="B42" s="48"/>
       <c r="C42" s="6" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>405</v>
-      </c>
-      <c r="B43" s="51"/>
+        <v>398</v>
+      </c>
+      <c r="B43" s="48"/>
       <c r="C43" s="6" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="B44" s="51"/>
+        <v>400</v>
+      </c>
+      <c r="B44" s="48"/>
       <c r="C44" s="6" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>409</v>
-      </c>
-      <c r="B45" s="51"/>
+        <v>402</v>
+      </c>
+      <c r="B45" s="48"/>
       <c r="C45" s="6" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>411</v>
-      </c>
-      <c r="B46" s="51"/>
+        <v>404</v>
+      </c>
+      <c r="B46" s="48"/>
       <c r="C46" s="6" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>413</v>
-      </c>
-      <c r="B47" s="51"/>
+        <v>406</v>
+      </c>
+      <c r="B47" s="48"/>
       <c r="C47" s="6" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>415</v>
-      </c>
-      <c r="B48" s="51"/>
+        <v>408</v>
+      </c>
+      <c r="B48" s="48"/>
       <c r="C48" s="6" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>417</v>
-      </c>
-      <c r="B49" s="51"/>
+        <v>410</v>
+      </c>
+      <c r="B49" s="48"/>
       <c r="C49" s="6" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="B50" s="51"/>
+        <v>412</v>
+      </c>
+      <c r="B50" s="48"/>
       <c r="C50" s="6" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>421</v>
-      </c>
-      <c r="B51" s="51"/>
+        <v>414</v>
+      </c>
+      <c r="B51" s="48"/>
       <c r="C51" s="6" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>423</v>
-      </c>
-      <c r="B52" s="51"/>
+        <v>416</v>
+      </c>
+      <c r="B52" s="48"/>
       <c r="C52" s="6" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>425</v>
-      </c>
-      <c r="B53" s="51"/>
+        <v>418</v>
+      </c>
+      <c r="B53" s="48"/>
       <c r="C53" s="6" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>427</v>
-      </c>
-      <c r="B54" s="51"/>
+        <v>420</v>
+      </c>
+      <c r="B54" s="48"/>
       <c r="C54" s="6" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>429</v>
-      </c>
-      <c r="B55" s="51"/>
+        <v>422</v>
+      </c>
+      <c r="B55" s="48"/>
       <c r="C55" s="6" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>431</v>
-      </c>
-      <c r="B56" s="51"/>
+        <v>424</v>
+      </c>
+      <c r="B56" s="48"/>
       <c r="C56" s="6" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>433</v>
-      </c>
-      <c r="B57" s="51"/>
+        <v>426</v>
+      </c>
+      <c r="B57" s="48"/>
       <c r="C57" s="6" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="B58" s="51"/>
+        <v>428</v>
+      </c>
+      <c r="B58" s="48"/>
       <c r="C58" s="6" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>437</v>
-      </c>
-      <c r="B59" s="51"/>
+        <v>430</v>
+      </c>
+      <c r="B59" s="48"/>
       <c r="C59" s="6" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>439</v>
-      </c>
-      <c r="B60" s="51"/>
+        <v>432</v>
+      </c>
+      <c r="B60" s="48"/>
       <c r="C60" s="6" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
-        <v>441</v>
-      </c>
-      <c r="B61" s="51"/>
+        <v>434</v>
+      </c>
+      <c r="B61" s="48"/>
       <c r="C61" s="6" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>443</v>
-      </c>
-      <c r="B62" s="51"/>
+        <v>436</v>
+      </c>
+      <c r="B62" s="48"/>
       <c r="C62" s="6" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>445</v>
-      </c>
-      <c r="B63" s="51"/>
+        <v>438</v>
+      </c>
+      <c r="B63" s="48"/>
       <c r="C63" s="6" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>447</v>
-      </c>
-      <c r="B64" s="51"/>
+        <v>440</v>
+      </c>
+      <c r="B64" s="48"/>
       <c r="C64" s="6" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>449</v>
-      </c>
-      <c r="B65" s="51"/>
+        <v>442</v>
+      </c>
+      <c r="B65" s="48"/>
       <c r="C65" s="6" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>451</v>
-      </c>
-      <c r="B66" s="51"/>
+        <v>444</v>
+      </c>
+      <c r="B66" s="48"/>
       <c r="C66" s="6" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
-        <v>453</v>
-      </c>
-      <c r="B67" s="51"/>
+        <v>446</v>
+      </c>
+      <c r="B67" s="48"/>
       <c r="C67" s="6" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
-        <v>455</v>
-      </c>
-      <c r="B68" s="51"/>
+        <v>448</v>
+      </c>
+      <c r="B68" s="48"/>
       <c r="C68" s="6" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
-        <v>457</v>
-      </c>
-      <c r="B69" s="51"/>
+        <v>450</v>
+      </c>
+      <c r="B69" s="48"/>
       <c r="C69" s="6" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
-        <v>459</v>
-      </c>
-      <c r="B70" s="51"/>
+        <v>452</v>
+      </c>
+      <c r="B70" s="48"/>
       <c r="C70" s="6" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>461</v>
-      </c>
-      <c r="B71" s="51"/>
+        <v>454</v>
+      </c>
+      <c r="B71" s="48"/>
       <c r="C71" s="6" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>463</v>
-      </c>
-      <c r="B72" s="51"/>
+        <v>456</v>
+      </c>
+      <c r="B72" s="48"/>
       <c r="C72" s="6" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>465</v>
-      </c>
-      <c r="B73" s="51"/>
+        <v>458</v>
+      </c>
+      <c r="B73" s="48"/>
       <c r="C73" s="6" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
-        <v>467</v>
-      </c>
-      <c r="B74" s="51"/>
+        <v>460</v>
+      </c>
+      <c r="B74" s="48"/>
       <c r="C74" s="6" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="B75" s="51"/>
+        <v>462</v>
+      </c>
+      <c r="B75" s="48"/>
       <c r="C75" s="6" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
-        <v>471</v>
-      </c>
-      <c r="B76" s="51"/>
+        <v>464</v>
+      </c>
+      <c r="B76" s="48"/>
       <c r="C76" s="6" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="15" t="s">
-        <v>473</v>
-      </c>
-      <c r="B77" s="51"/>
+        <v>466</v>
+      </c>
+      <c r="B77" s="48"/>
       <c r="C77" s="6" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>475</v>
-      </c>
-      <c r="B78" s="51"/>
+        <v>468</v>
+      </c>
+      <c r="B78" s="48"/>
       <c r="C78" s="6" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
-        <v>477</v>
-      </c>
-      <c r="B79" s="51"/>
+        <v>470</v>
+      </c>
+      <c r="B79" s="48"/>
       <c r="C79" s="6" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
-        <v>479</v>
-      </c>
-      <c r="B80" s="51"/>
+        <v>472</v>
+      </c>
+      <c r="B80" s="48"/>
       <c r="C80" s="6" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A81" s="15" t="s">
-        <v>481</v>
-      </c>
-      <c r="B81" s="51"/>
+        <v>474</v>
+      </c>
+      <c r="B81" s="48"/>
       <c r="C81" s="6" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
-        <v>483</v>
-      </c>
-      <c r="B82" s="51"/>
+        <v>476</v>
+      </c>
+      <c r="B82" s="48"/>
       <c r="C82" s="6" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="s">
-        <v>485</v>
-      </c>
-      <c r="B83" s="51"/>
+        <v>478</v>
+      </c>
+      <c r="B83" s="48"/>
       <c r="C83" s="6" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
-        <v>487</v>
-      </c>
-      <c r="B84" s="51"/>
+        <v>480</v>
+      </c>
+      <c r="B84" s="48"/>
       <c r="C84" s="6" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="s">
-        <v>489</v>
-      </c>
-      <c r="B85" s="51"/>
+        <v>482</v>
+      </c>
+      <c r="B85" s="48"/>
       <c r="C85" s="6" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
-        <v>491</v>
-      </c>
-      <c r="B86" s="51"/>
+        <v>484</v>
+      </c>
+      <c r="B86" s="48"/>
       <c r="C86" s="6" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="s">
-        <v>493</v>
-      </c>
-      <c r="B87" s="51"/>
+        <v>486</v>
+      </c>
+      <c r="B87" s="48"/>
       <c r="C87" s="6" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
-        <v>495</v>
-      </c>
-      <c r="B88" s="51"/>
+        <v>488</v>
+      </c>
+      <c r="B88" s="48"/>
       <c r="C88" s="6" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="15" t="s">
-        <v>497</v>
-      </c>
-      <c r="B89" s="51"/>
+        <v>490</v>
+      </c>
+      <c r="B89" s="48"/>
       <c r="C89" s="6" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
-        <v>437</v>
-      </c>
-      <c r="B90" s="51"/>
+        <v>430</v>
+      </c>
+      <c r="B90" s="48"/>
       <c r="C90" s="6" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="s">
-        <v>500</v>
-      </c>
-      <c r="B91" s="51"/>
+        <v>493</v>
+      </c>
+      <c r="B91" s="48"/>
       <c r="C91" s="6" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
-        <v>502</v>
-      </c>
-      <c r="B92" s="51"/>
+        <v>495</v>
+      </c>
+      <c r="B92" s="48"/>
       <c r="C92" s="6" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="s">
-        <v>504</v>
-      </c>
-      <c r="B93" s="51"/>
+        <v>497</v>
+      </c>
+      <c r="B93" s="48"/>
       <c r="C93" s="6" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
-        <v>506</v>
-      </c>
-      <c r="B94" s="51"/>
+        <v>499</v>
+      </c>
+      <c r="B94" s="48"/>
       <c r="C94" s="6" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="s">
-        <v>508</v>
-      </c>
-      <c r="B95" s="51"/>
+        <v>501</v>
+      </c>
+      <c r="B95" s="48"/>
       <c r="C95" s="6" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="s">
-        <v>510</v>
-      </c>
-      <c r="B96" s="51"/>
+        <v>503</v>
+      </c>
+      <c r="B96" s="48"/>
       <c r="C96" s="6" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="s">
-        <v>512</v>
-      </c>
-      <c r="B97" s="51"/>
+        <v>505</v>
+      </c>
+      <c r="B97" s="48"/>
       <c r="C97" s="6" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
-        <v>514</v>
-      </c>
-      <c r="B98" s="51"/>
+        <v>507</v>
+      </c>
+      <c r="B98" s="48"/>
       <c r="C98" s="6" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="15" t="s">
-        <v>516</v>
-      </c>
-      <c r="B99" s="51"/>
+        <v>509</v>
+      </c>
+      <c r="B99" s="48"/>
       <c r="C99" s="6" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="15" t="s">
-        <v>518</v>
-      </c>
-      <c r="B100" s="51"/>
+        <v>511</v>
+      </c>
+      <c r="B100" s="48"/>
       <c r="C100" s="6" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="s">
-        <v>520</v>
-      </c>
-      <c r="B101" s="51"/>
+        <v>513</v>
+      </c>
+      <c r="B101" s="48"/>
       <c r="C101" s="6" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="15" t="s">
-        <v>522</v>
-      </c>
-      <c r="B102" s="51"/>
+        <v>515</v>
+      </c>
+      <c r="B102" s="48"/>
       <c r="C102" s="6" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="s">
-        <v>524</v>
-      </c>
-      <c r="B103" s="51"/>
+        <v>517</v>
+      </c>
+      <c r="B103" s="48"/>
       <c r="C103" s="6" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="s">
-        <v>526</v>
-      </c>
-      <c r="B104" s="51"/>
+        <v>519</v>
+      </c>
+      <c r="B104" s="48"/>
       <c r="C104" s="6" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="s">
-        <v>528</v>
-      </c>
-      <c r="B105" s="51"/>
+        <v>521</v>
+      </c>
+      <c r="B105" s="48"/>
       <c r="C105" s="6" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="s">
-        <v>530</v>
-      </c>
-      <c r="B106" s="51"/>
+        <v>523</v>
+      </c>
+      <c r="B106" s="48"/>
       <c r="C106" s="6" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="s">
-        <v>532</v>
-      </c>
-      <c r="B107" s="51"/>
+        <v>525</v>
+      </c>
+      <c r="B107" s="48"/>
       <c r="C107" s="6" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="s">
-        <v>534</v>
-      </c>
-      <c r="B108" s="51"/>
+        <v>527</v>
+      </c>
+      <c r="B108" s="48"/>
       <c r="C108" s="6" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="s">
-        <v>536</v>
-      </c>
-      <c r="B109" s="51"/>
+        <v>529</v>
+      </c>
+      <c r="B109" s="48"/>
       <c r="C109" s="6" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="s">
-        <v>538</v>
-      </c>
-      <c r="B110" s="51"/>
+        <v>531</v>
+      </c>
+      <c r="B110" s="48"/>
       <c r="C110" s="6" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="15" t="s">
-        <v>540</v>
-      </c>
-      <c r="B111" s="51"/>
+        <v>533</v>
+      </c>
+      <c r="B111" s="48"/>
       <c r="C111" s="6" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="15" t="s">
-        <v>542</v>
-      </c>
-      <c r="B112" s="51"/>
+        <v>535</v>
+      </c>
+      <c r="B112" s="48"/>
       <c r="C112" s="6" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="15" t="s">
-        <v>544</v>
-      </c>
-      <c r="B113" s="51"/>
+        <v>537</v>
+      </c>
+      <c r="B113" s="48"/>
       <c r="C113" s="6" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="15" t="s">
-        <v>546</v>
-      </c>
-      <c r="B114" s="51"/>
+        <v>539</v>
+      </c>
+      <c r="B114" s="48"/>
       <c r="C114" s="6" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="15" t="s">
-        <v>548</v>
-      </c>
-      <c r="B115" s="51"/>
+        <v>541</v>
+      </c>
+      <c r="B115" s="48"/>
       <c r="C115" s="6" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="15" t="s">
-        <v>550</v>
-      </c>
-      <c r="B116" s="51"/>
+        <v>543</v>
+      </c>
+      <c r="B116" s="48"/>
       <c r="C116" s="6" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="15" t="s">
-        <v>552</v>
-      </c>
-      <c r="B117" s="51"/>
+        <v>545</v>
+      </c>
+      <c r="B117" s="48"/>
       <c r="C117" s="6" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="15" t="s">
-        <v>554</v>
-      </c>
-      <c r="B118" s="51"/>
+        <v>547</v>
+      </c>
+      <c r="B118" s="48"/>
       <c r="C118" s="6" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="15" t="s">
-        <v>556</v>
-      </c>
-      <c r="B119" s="51"/>
+        <v>549</v>
+      </c>
+      <c r="B119" s="48"/>
       <c r="C119" s="6" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
-        <v>558</v>
-      </c>
-      <c r="B120" s="51"/>
+        <v>551</v>
+      </c>
+      <c r="B120" s="48"/>
       <c r="C120" s="6" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="15" t="s">
-        <v>560</v>
-      </c>
-      <c r="B121" s="51"/>
+        <v>553</v>
+      </c>
+      <c r="B121" s="48"/>
       <c r="C121" s="6" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" s="15" t="s">
-        <v>562</v>
-      </c>
-      <c r="B122" s="51"/>
+        <v>555</v>
+      </c>
+      <c r="B122" s="48"/>
       <c r="C122" s="6" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="15" t="s">
-        <v>564</v>
-      </c>
-      <c r="B123" s="51"/>
+        <v>557</v>
+      </c>
+      <c r="B123" s="48"/>
       <c r="C123" s="6" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="B124" s="51"/>
+        <v>559</v>
+      </c>
+      <c r="B124" s="48"/>
       <c r="C124" s="6" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="B125" s="51"/>
+        <v>561</v>
+      </c>
+      <c r="B125" s="48"/>
       <c r="C125" s="6" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="B126" s="51"/>
+        <v>563</v>
+      </c>
+      <c r="B126" s="48"/>
       <c r="C126" s="6" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="15" t="s">
-        <v>572</v>
-      </c>
-      <c r="B127" s="51"/>
+        <v>565</v>
+      </c>
+      <c r="B127" s="48"/>
       <c r="C127" s="6" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="B128" s="51"/>
+        <v>567</v>
+      </c>
+      <c r="B128" s="48"/>
       <c r="C128" s="6" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="15" t="s">
-        <v>576</v>
-      </c>
-      <c r="B129" s="51"/>
+        <v>569</v>
+      </c>
+      <c r="B129" s="48"/>
       <c r="C129" s="6" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="15" t="s">
-        <v>578</v>
-      </c>
-      <c r="B130" s="51"/>
+        <v>571</v>
+      </c>
+      <c r="B130" s="48"/>
       <c r="C130" s="6" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="15" t="s">
-        <v>580</v>
-      </c>
-      <c r="B131" s="51"/>
+        <v>573</v>
+      </c>
+      <c r="B131" s="48"/>
       <c r="C131" s="6" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="15" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="15" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="15" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="15" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="15" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="15" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -4989,7 +4982,7 @@
         <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F2" t="s">
         <v>161</v>
@@ -5021,116 +5014,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>276</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
+      <c r="B3" s="50" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="50" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
     </row>
     <row r="7" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
@@ -5150,17 +5143,17 @@
         <v>201</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>272</v>
-      </c>
       <c r="F12" s="10" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="28" t="s">
         <v>166</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -5175,7 +5168,7 @@
       <c r="E13" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="31" t="s">
         <v>250</v>
       </c>
     </row>
@@ -5186,51 +5179,51 @@
       <c r="B14" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="31" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>288</v>
+      <c r="A15" s="30" t="s">
+        <v>281</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="31" t="s">
         <v>250</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5256,71 +5249,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>290</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>291</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>293</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>294</v>
+      <c r="A1" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="44" t="s">
         <v>168</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>168</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="45" t="s">
         <v>167</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>295</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -5344,25 +5337,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>301</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>302</v>
+      <c r="A1" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -5370,7 +5363,7 @@
         <v>201</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>164</v>
@@ -5378,10 +5371,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>164</v>
@@ -5389,24 +5382,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="49" t="s">
-        <v>307</v>
+      <c r="A6" s="46" t="s">
+        <v>300</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -5446,52 +5439,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>97</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56" t="s">
+      <c r="E1" s="53"/>
+      <c r="F1" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56" t="s">
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
       <c r="T1" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>99</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -5550,13 +5543,13 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>101</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -5617,7 +5610,7 @@
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
       <c r="B4" s="15"/>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -5678,7 +5671,7 @@
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -5739,11 +5732,11 @@
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
       <c r="B6" s="15"/>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>202</v>
@@ -5752,55 +5745,55 @@
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="P6" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="21" t="s">
         <v>109</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -5812,7 +5805,7 @@
       <c r="F7" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="36" t="s">
         <v>127</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -5821,7 +5814,7 @@
       <c r="I7" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J7" s="36" t="s">
         <v>130</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -5830,25 +5823,25 @@
       <c r="L7" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="M7" s="39" t="s">
+      <c r="M7" s="36" t="s">
         <v>133</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="O7" s="39" t="s">
+      <c r="O7" s="36" t="s">
         <v>136</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Q7" s="39" t="s">
+      <c r="Q7" s="36" t="s">
         <v>138</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="S7" s="39" t="s">
+      <c r="S7" s="36" t="s">
         <v>140</v>
       </c>
       <c r="T7" s="1" t="s">
@@ -5861,7 +5854,7 @@
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="21" t="s">
         <v>110</v>
       </c>
       <c r="H8" s="2"/>
@@ -5880,13 +5873,13 @@
       <c r="U8" s="2"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="25" t="s">
         <v>111</v>
       </c>
     </row>
@@ -5968,49 +5961,49 @@
       <c r="F11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="O11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="P11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="R11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="S11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="T11" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="U11" s="40" t="s">
+      <c r="G11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="R11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="S11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="T11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="U11" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6073,7 +6066,7 @@
       <c r="T12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U12" s="40" t="s">
+      <c r="U12" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6091,52 +6084,52 @@
       <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="N13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="O13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="P13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="R13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="S13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="T13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="U13" s="40" t="s">
+      <c r="F13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="R13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="S13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="T13" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="U13" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6154,52 +6147,52 @@
       <c r="E14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="L14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="N14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="O14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="P14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="R14" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="S14" s="40" t="s">
+      <c r="F14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="R14" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="S14" s="37" t="s">
         <v>24</v>
       </c>
       <c r="T14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U14" s="40" t="s">
+      <c r="U14" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6217,52 +6210,52 @@
       <c r="E15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="M15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="N15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="O15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="P15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="R15" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="S15" s="40" t="s">
+      <c r="F15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="P15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="R15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="S15" s="37" t="s">
         <v>24</v>
       </c>
       <c r="T15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U15" s="40" t="s">
+      <c r="U15" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6280,46 +6273,46 @@
       <c r="E16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="N16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="O16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="P16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="R16" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="S16" s="40" t="s">
+      <c r="F16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="P16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="R16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="S16" s="37" t="s">
         <v>24</v>
       </c>
       <c r="T16" s="2" t="s">
@@ -6388,7 +6381,7 @@
       <c r="T17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U17" s="40" t="s">
+      <c r="U17" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6645,8 +6638,8 @@
       <c r="B22" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C22" s="41" t="s">
-        <v>283</v>
+      <c r="C22" s="38" t="s">
+        <v>277</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>5</v>
@@ -6757,10 +6750,10 @@
       <c r="S23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T23" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="U23" s="40" t="s">
+      <c r="T23" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="U23" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6818,10 +6811,10 @@
       <c r="S24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T24" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="U24" s="40" t="s">
+      <c r="T24" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="U24" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6953,7 +6946,7 @@
         <v>214</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>5</v>
@@ -7133,12 +7126,12 @@
       </c>
     </row>
     <row r="30" spans="1:21" ht="238" x14ac:dyDescent="0.2">
-      <c r="A30" s="45"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="46" t="s">
-        <v>284</v>
+      <c r="C30" s="43" t="s">
+        <v>278</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>5</v>
@@ -7252,7 +7245,7 @@
       <c r="T31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U31" s="40" t="s">
+      <c r="U31" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7262,16 +7255,16 @@
         <v>216</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="40" t="s">
+      <c r="D32" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="37" t="s">
         <v>24</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="40" t="s">
+      <c r="G32" s="37" t="s">
         <v>24</v>
       </c>
       <c r="H32" s="2" t="s">
@@ -7313,7 +7306,7 @@
       <c r="T32" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U32" s="40" t="s">
+      <c r="U32" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7322,8 +7315,8 @@
       <c r="B33" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C33" s="42" t="s">
-        <v>282</v>
+      <c r="C33" s="39" t="s">
+        <v>276</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>232</v>
@@ -7367,16 +7360,16 @@
       <c r="Q33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="R33" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="S33" s="40" t="s">
+      <c r="R33" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="S33" s="37" t="s">
         <v>24</v>
       </c>
       <c r="T33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U33" s="40" t="s">
+      <c r="U33" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7513,7 +7506,7 @@
       <c r="D36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" s="37" t="s">
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
@@ -7546,22 +7539,22 @@
       <c r="O36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P36" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q36" s="40" t="s">
+      <c r="P36" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="37" t="s">
         <v>24</v>
       </c>
       <c r="R36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S36" s="40" t="s">
+      <c r="S36" s="37" t="s">
         <v>24</v>
       </c>
       <c r="T36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U36" s="40" t="s">
+      <c r="U36" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7574,55 +7567,55 @@
       <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="37" t="s">
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="H37" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="I37" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J37" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K37" s="40" t="s">
+      <c r="G37" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K37" s="37" t="s">
         <v>24</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M37" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="N37" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="O37" s="40" t="s">
+      <c r="M37" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="N37" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="O37" s="37" t="s">
         <v>24</v>
       </c>
       <c r="P37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q37" s="40" t="s">
+      <c r="Q37" s="37" t="s">
         <v>24</v>
       </c>
       <c r="R37" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S37" s="40" t="s">
+      <c r="S37" s="37" t="s">
         <v>24</v>
       </c>
       <c r="T37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U37" s="40" t="s">
+      <c r="U37" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7671,19 +7664,19 @@
       <c r="P38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q38" s="40" t="s">
+      <c r="Q38" s="37" t="s">
         <v>24</v>
       </c>
       <c r="R38" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="S38" s="40" t="s">
+      <c r="S38" s="37" t="s">
         <v>24</v>
       </c>
       <c r="T38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U38" s="40" t="s">
+      <c r="U38" s="37" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7744,7 +7737,7 @@
       <c r="T39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U39" s="40" t="s">
+      <c r="U39" s="37" t="s">
         <v>5</v>
       </c>
     </row>
@@ -7754,7 +7747,7 @@
         <v>14</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>5</v>
@@ -7783,7 +7776,7 @@
       <c r="L40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M40" s="40" t="s">
+      <c r="M40" s="37" t="s">
         <v>24</v>
       </c>
       <c r="N40" s="2" t="s">
@@ -7828,7 +7821,7 @@
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
-      <c r="U41" s="40"/>
+      <c r="U41" s="37"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
@@ -7847,7 +7840,7 @@
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
-      <c r="U42" s="40"/>
+      <c r="U42" s="37"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
@@ -7866,7 +7859,7 @@
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
-      <c r="U43" s="40"/>
+      <c r="U43" s="37"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
@@ -7885,7 +7878,7 @@
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
-      <c r="U44" s="40"/>
+      <c r="U44" s="37"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
@@ -8337,24 +8330,24 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -8398,8 +8391,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
-        <v>277</v>
+      <c r="A2" s="38" t="s">
+        <v>273</v>
       </c>
       <c r="B2">
         <v>300</v>
@@ -8407,8 +8400,8 @@
       <c r="C2" t="s">
         <v>253</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>264</v>
+      <c r="D2" s="29" t="s">
+        <v>263</v>
       </c>
       <c r="E2" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Add primary objective / endpoints to CDISC Pilot
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1052284F-856C-034C-A3C9-54E0BFAB4B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F863F78E-2AD5-BA44-A956-E7D770783C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="588">
   <si>
     <t>Epoch</t>
   </si>
@@ -1895,6 +1895,35 @@
   </si>
   <si>
     <t>The change from baseline laboratory value will be  calculated as the difference between the baseline lab value and the endpoint value (i.e., the value at the specified visit) or the end of treatment observation</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>Primary Objectives</t>
+  </si>
+  <si>
+    <t>&lt;table&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top"&gt;&lt;p&gt;Primary Objective&lt;/p&gt;&lt;/th&gt;
+    &lt;th style="vertical-align: top"&gt;&lt;p&gt;Primary Endpoint&lt;/p&gt;&lt;/th&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;td style="vertical-align: top"&gt;&lt;p&gt;&lt;usdm:ref klass="Objective" namexref="OBJ1" attribute="description"/&gt;&lt;/p&gt;&lt;/td&gt;
+    &lt;td style="vertical-align: top"&gt;
+      &lt;p&gt;&lt;usdm:ref klass="Endpoint" namexref="END1" attribute="description"/&gt;&lt;/p&gt;
+      &lt;p&gt;&lt;usdm:ref klass="Endpoint" namexref="END2" attribute="description"/&gt;&lt;/p&gt;
+    &lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;td style="vertical-align: top"&gt;&lt;p&gt;&lt;usdm:ref klass="Objective" namexref="OBJ2" attribute="description"/&gt;&lt;/p&gt;&lt;/td&gt;
+    &lt;td style="vertical-align: top"&gt;
+      &lt;p&gt;&lt;usdm:ref klass="Endpoint" namexref="END3" attribute="description"/&gt;&lt;/p&gt;
+      &lt;p&gt;&lt;usdm:ref klass="Endpoint" namexref="END4" attribute="description"/&gt;&lt;/p&gt;
+      &lt;p&gt;&lt;usdm:ref klass="Endpoint" namexref="END5" attribute="description"/&gt;&lt;/p&gt;
+    &lt;/td&gt;
+  &lt;/tr&gt;
+&lt;/table&gt;</t>
   </si>
 </sst>
 </file>
@@ -1997,7 +2026,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2129,11 +2158,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2142,21 +2171,14 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2570,27 +2592,27 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="58" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="54" t="s">
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="19" t="s">
         <v>579</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57">
+      <c r="F10" s="1"/>
+      <c r="G10" s="49">
         <v>38718</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2604,7 +2626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -3704,10 +3726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3797,1111 +3819,1117 @@
         <v>331</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>332</v>
+    <row r="10" spans="1:4" ht="388" x14ac:dyDescent="0.2">
+      <c r="A10" s="55" t="s">
+        <v>585</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>333</v>
+        <v>586</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="B12" s="48"/>
+        <v>334</v>
+      </c>
       <c r="C12" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B17" s="48"/>
       <c r="C17" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B18" s="48"/>
       <c r="C18" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B19" s="48"/>
       <c r="C19" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B20" s="48"/>
       <c r="C20" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="6" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B22" s="48"/>
       <c r="C22" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B24" s="48"/>
       <c r="C24" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B25" s="48"/>
       <c r="C25" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B26" s="48"/>
       <c r="C26" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B27" s="48"/>
       <c r="C27" s="6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B28" s="48"/>
       <c r="C28" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B29" s="48"/>
       <c r="C29" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B31" s="48"/>
       <c r="C31" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B32" s="48"/>
       <c r="C32" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B33" s="48"/>
       <c r="C33" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B34" s="48"/>
       <c r="C34" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B40" s="48"/>
       <c r="C40" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B41" s="48"/>
       <c r="C41" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B42" s="48"/>
       <c r="C42" s="6" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B43" s="48"/>
       <c r="C43" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B44" s="48"/>
       <c r="C44" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B45" s="48"/>
       <c r="C45" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B46" s="48"/>
       <c r="C46" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B47" s="48"/>
       <c r="C47" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B48" s="48"/>
       <c r="C48" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B49" s="48"/>
       <c r="C49" s="6" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B50" s="48"/>
       <c r="C50" s="6" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B51" s="48"/>
       <c r="C51" s="6" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B52" s="48"/>
       <c r="C52" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B53" s="48"/>
       <c r="C53" s="6" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B54" s="48"/>
       <c r="C54" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B55" s="48"/>
       <c r="C55" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B56" s="48"/>
       <c r="C56" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B57" s="48"/>
       <c r="C57" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B58" s="48"/>
       <c r="C58" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B59" s="48"/>
       <c r="C59" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B60" s="48"/>
       <c r="C60" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B61" s="48"/>
       <c r="C61" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B62" s="48"/>
       <c r="C62" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B63" s="48"/>
       <c r="C63" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B64" s="48"/>
       <c r="C64" s="6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B65" s="48"/>
       <c r="C65" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B66" s="48"/>
       <c r="C66" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B67" s="48"/>
       <c r="C67" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B68" s="48"/>
       <c r="C68" s="6" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B69" s="48"/>
       <c r="C69" s="6" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B70" s="48"/>
       <c r="C70" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B71" s="48"/>
       <c r="C71" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B72" s="48"/>
       <c r="C72" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B73" s="48"/>
       <c r="C73" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B74" s="48"/>
       <c r="C74" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="15" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B75" s="48"/>
       <c r="C75" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B76" s="48"/>
       <c r="C76" s="6" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="15" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B77" s="48"/>
       <c r="C77" s="6" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B78" s="48"/>
       <c r="C78" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B79" s="48"/>
       <c r="C79" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B80" s="48"/>
       <c r="C80" s="6" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="15" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B81" s="48"/>
       <c r="C81" s="6" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B82" s="48"/>
       <c r="C82" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B83" s="48"/>
       <c r="C83" s="6" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B84" s="48"/>
       <c r="C84" s="6" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B85" s="48"/>
       <c r="C85" s="6" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B86" s="48"/>
       <c r="C86" s="6" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B87" s="48"/>
       <c r="C87" s="6" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B88" s="48"/>
       <c r="C88" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="15" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B89" s="48"/>
       <c r="C89" s="6" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
-        <v>430</v>
+        <v>490</v>
       </c>
       <c r="B90" s="48"/>
       <c r="C90" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="s">
-        <v>493</v>
+        <v>430</v>
       </c>
       <c r="B91" s="48"/>
       <c r="C91" s="6" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B92" s="48"/>
       <c r="C92" s="6" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B93" s="48"/>
       <c r="C93" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B94" s="48"/>
       <c r="C94" s="6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B95" s="48"/>
       <c r="C95" s="6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B96" s="48"/>
       <c r="C96" s="6" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B97" s="48"/>
       <c r="C97" s="6" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B98" s="48"/>
       <c r="C98" s="6" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="15" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B99" s="48"/>
       <c r="C99" s="6" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="15" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B100" s="48"/>
       <c r="C100" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B101" s="48"/>
       <c r="C101" s="6" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="15" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B102" s="48"/>
       <c r="C102" s="6" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B103" s="48"/>
       <c r="C103" s="6" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B104" s="48"/>
       <c r="C104" s="6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B105" s="48"/>
       <c r="C105" s="6" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B106" s="48"/>
       <c r="C106" s="6" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B107" s="48"/>
       <c r="C107" s="6" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B108" s="48"/>
       <c r="C108" s="6" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B109" s="48"/>
       <c r="C109" s="6" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B110" s="48"/>
       <c r="C110" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="15" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B111" s="48"/>
       <c r="C111" s="6" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="15" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B112" s="48"/>
       <c r="C112" s="6" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="15" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B113" s="48"/>
       <c r="C113" s="6" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="15" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B114" s="48"/>
       <c r="C114" s="6" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B115" s="48"/>
       <c r="C115" s="6" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B116" s="48"/>
       <c r="C116" s="6" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="15" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B117" s="48"/>
       <c r="C117" s="6" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="15" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B118" s="48"/>
       <c r="C118" s="6" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="15" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B119" s="48"/>
       <c r="C119" s="6" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B120" s="48"/>
       <c r="C120" s="6" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="15" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B121" s="48"/>
       <c r="C121" s="6" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="15" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B122" s="48"/>
       <c r="C122" s="6" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="15" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B123" s="48"/>
       <c r="C123" s="6" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="15" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B124" s="48"/>
       <c r="C124" s="6" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="15" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B125" s="48"/>
       <c r="C125" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="15" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B126" s="48"/>
       <c r="C126" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="15" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B127" s="48"/>
       <c r="C127" s="6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="15" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B128" s="48"/>
       <c r="C128" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="15" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B129" s="48"/>
       <c r="C129" s="6" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="15" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B130" s="48"/>
       <c r="C130" s="6" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="15" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B131" s="48"/>
       <c r="C131" s="6" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="15" t="s">
+        <v>573</v>
+      </c>
+      <c r="B132" s="48"/>
+      <c r="C132" s="6" t="s">
         <v>574</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="15" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -4926,6 +4954,11 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="15" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="15" t="s">
         <v>575</v>
       </c>
     </row>
@@ -5017,49 +5050,49 @@
       <c r="A1" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="53" t="s">
         <v>272</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -5076,12 +5109,12 @@
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
     </row>
     <row r="7" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -5090,40 +5123,40 @@
       <c r="B7" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
@@ -5214,16 +5247,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5448,28 +5481,28 @@
       <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53" t="s">
+      <c r="E1" s="54"/>
+      <c r="F1" s="54" t="s">
         <v>201</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53" t="s">
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54" t="s">
         <v>200</v>
       </c>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
       <c r="T1" s="1" t="s">
         <v>271</v>
       </c>

</xml_diff>

<commit_message>
Tweak to titles in CDISC Pilot study
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F863F78E-2AD5-BA44-A956-E7D770783C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDC3A6E-8306-2341-AAEA-ED57214B0EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="586">
   <si>
     <t>Epoch</t>
   </si>
@@ -882,11 +882,6 @@
   </si>
   <si>
     <t>Patients with Probable Mild to Moderate Alzheimer\'s Disease</t>
-  </si>
-  <si>
-    <t>Safety and Efficacy of the Xanomeline Transdermal
-Therapeutic System (TTS) in Patients with Mild to
-Moderate Alzheimer\'s Disease</t>
   </si>
   <si>
     <t>H2Q-MC-LZZT</t>
@@ -1874,14 +1869,6 @@
 &lt;table&gt;</t>
   </si>
   <si>
-    <t>Safety and Efficacy of the Xanomeline Transdermal Therapeutic System (TTS) in Patients with Mild to Moderate Alzheimer’s Disease</t>
-  </si>
-  <si>
-    <t>Safety and Efficacy of the Xanomeline
-Transdermal Therapeutic System (TTS) in Patients
-with Mild to Moderate Alzheimer’s Disease</t>
-  </si>
-  <si>
     <t>Alzheimer's Disease Assessment Scale - Cognitive Subscale, total of 11 items [ADAS-Cog (11)] at Week 24</t>
   </si>
   <si>
@@ -1924,6 +1911,9 @@
     &lt;/td&gt;
   &lt;/tr&gt;
 &lt;/table&gt;</t>
+  </si>
+  <si>
+    <t>Safety and Efficacy of the Xanomeline Transdermal Therapeutic System (TTS) in Patients with Mild to Moderate Alzheimer's Disease</t>
   </si>
 </sst>
 </file>
@@ -2161,8 +2151,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2171,13 +2167,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2495,8 +2485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2515,7 +2505,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>578</v>
+        <v>585</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2547,7 +2537,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -2597,13 +2587,13 @@
         <v>159</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>579</v>
+        <v>585</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>274</v>
+        <v>585</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -2680,7 +2670,7 @@
         <v>62</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>58</v>
@@ -2694,7 +2684,7 @@
         <v>74</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>58</v>
@@ -2745,10 +2735,10 @@
         <v>77</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>58</v>
@@ -2771,7 +2761,7 @@
         <v>255</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>61</v>
@@ -2785,7 +2775,7 @@
         <v>256</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>61</v>
@@ -3026,10 +3016,10 @@
         <v>69</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>303</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>304</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>103</v>
@@ -3297,7 +3287,7 @@
         <v>132</v>
       </c>
       <c r="B10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C10" t="s">
         <v>179</v>
@@ -3707,7 +3697,7 @@
         <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3715,7 +3705,7 @@
         <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -3728,7 +3718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3742,1224 +3732,1224 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>312</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="C1" s="32" t="s">
         <v>313</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>314</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>318</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>322</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>324</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>328</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>331</v>
-      </c>
     </row>
     <row r="10" spans="1:4" ht="388" x14ac:dyDescent="0.2">
-      <c r="A10" s="55" t="s">
-        <v>585</v>
+      <c r="A10" s="50" t="s">
+        <v>582</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>332</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>334</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B17" s="48"/>
       <c r="C17" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B18" s="48"/>
       <c r="C18" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B19" s="48"/>
       <c r="C19" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B20" s="48"/>
       <c r="C20" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B22" s="48"/>
       <c r="C22" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B24" s="48"/>
       <c r="C24" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B25" s="48"/>
       <c r="C25" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B26" s="48"/>
       <c r="C26" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B27" s="48"/>
       <c r="C27" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B28" s="48"/>
       <c r="C28" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B29" s="48"/>
       <c r="C29" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B31" s="48"/>
       <c r="C31" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B32" s="48"/>
       <c r="C32" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B33" s="48"/>
       <c r="C33" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B34" s="48"/>
       <c r="C34" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B40" s="48"/>
       <c r="C40" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B41" s="48"/>
       <c r="C41" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B42" s="48"/>
       <c r="C42" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B43" s="48"/>
       <c r="C43" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B44" s="48"/>
       <c r="C44" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B45" s="48"/>
       <c r="C45" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B46" s="48"/>
       <c r="C46" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B47" s="48"/>
       <c r="C47" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B48" s="48"/>
       <c r="C48" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B49" s="48"/>
       <c r="C49" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B50" s="48"/>
       <c r="C50" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B51" s="48"/>
       <c r="C51" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B52" s="48"/>
       <c r="C52" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B53" s="48"/>
       <c r="C53" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B54" s="48"/>
       <c r="C54" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B55" s="48"/>
       <c r="C55" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B56" s="48"/>
       <c r="C56" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B57" s="48"/>
       <c r="C57" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B58" s="48"/>
       <c r="C58" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B59" s="48"/>
       <c r="C59" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B60" s="48"/>
       <c r="C60" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B61" s="48"/>
       <c r="C61" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B62" s="48"/>
       <c r="C62" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B63" s="48"/>
       <c r="C63" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B64" s="48"/>
       <c r="C64" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B65" s="48"/>
       <c r="C65" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B66" s="48"/>
       <c r="C66" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B67" s="48"/>
       <c r="C67" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B68" s="48"/>
       <c r="C68" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B69" s="48"/>
       <c r="C69" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B70" s="48"/>
       <c r="C70" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B71" s="48"/>
       <c r="C71" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B72" s="48"/>
       <c r="C72" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B73" s="48"/>
       <c r="C73" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B74" s="48"/>
       <c r="C74" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B75" s="48"/>
       <c r="C75" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B76" s="48"/>
       <c r="C76" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B77" s="48"/>
       <c r="C77" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B78" s="48"/>
       <c r="C78" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B79" s="48"/>
       <c r="C79" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B80" s="48"/>
       <c r="C80" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B81" s="48"/>
       <c r="C81" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B82" s="48"/>
       <c r="C82" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B83" s="48"/>
       <c r="C83" s="6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B84" s="48"/>
       <c r="C84" s="6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B85" s="48"/>
       <c r="C85" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B86" s="48"/>
       <c r="C86" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B87" s="48"/>
       <c r="C87" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B88" s="48"/>
       <c r="C88" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B89" s="48"/>
       <c r="C89" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B90" s="48"/>
       <c r="C90" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B91" s="48"/>
       <c r="C91" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B92" s="48"/>
       <c r="C92" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B93" s="48"/>
       <c r="C93" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B94" s="48"/>
       <c r="C94" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B95" s="48"/>
       <c r="C95" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B96" s="48"/>
       <c r="C96" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B97" s="48"/>
       <c r="C97" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B98" s="48"/>
       <c r="C98" s="6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="15" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B99" s="48"/>
       <c r="C99" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B100" s="48"/>
       <c r="C100" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B101" s="48"/>
       <c r="C101" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B102" s="48"/>
       <c r="C102" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B103" s="48"/>
       <c r="C103" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B104" s="48"/>
       <c r="C104" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B105" s="48"/>
       <c r="C105" s="6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B106" s="48"/>
       <c r="C106" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B107" s="48"/>
       <c r="C107" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B108" s="48"/>
       <c r="C108" s="6" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B109" s="48"/>
       <c r="C109" s="6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B110" s="48"/>
       <c r="C110" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="15" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B111" s="48"/>
       <c r="C111" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="15" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B112" s="48"/>
       <c r="C112" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="15" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B113" s="48"/>
       <c r="C113" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B114" s="48"/>
       <c r="C114" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B115" s="48"/>
       <c r="C115" s="6" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B116" s="48"/>
       <c r="C116" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B117" s="48"/>
       <c r="C117" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="15" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B118" s="48"/>
       <c r="C118" s="6" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="15" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B119" s="48"/>
       <c r="C119" s="6" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B120" s="48"/>
       <c r="C120" s="6" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="15" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B121" s="48"/>
       <c r="C121" s="6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="15" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B122" s="48"/>
       <c r="C122" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="15" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B123" s="48"/>
       <c r="C123" s="6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="15" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B124" s="48"/>
       <c r="C124" s="6" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="15" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B125" s="48"/>
       <c r="C125" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="15" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B126" s="48"/>
       <c r="C126" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B127" s="48"/>
       <c r="C127" s="6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B128" s="48"/>
       <c r="C128" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="15" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B129" s="48"/>
       <c r="C129" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="15" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B130" s="48"/>
       <c r="C130" s="6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B131" s="48"/>
       <c r="C131" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="15" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B132" s="48"/>
       <c r="C132" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -5015,7 +5005,7 @@
         <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F2" t="s">
         <v>161</v>
@@ -5050,113 +5040,113 @@
       <c r="A1" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>272</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
     </row>
     <row r="7" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
@@ -5182,7 +5172,7 @@
         <v>271</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -5227,7 +5217,7 @@
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>145</v>
@@ -5247,16 +5237,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5283,19 +5273,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="25" t="s">
         <v>286</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -5306,13 +5296,13 @@
         <v>168</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -5320,33 +5310,33 @@
         <v>167</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -5371,24 +5361,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>294</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>297</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -5396,7 +5386,7 @@
         <v>201</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>164</v>
@@ -5407,7 +5397,7 @@
         <v>270</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>164</v>
@@ -5418,7 +5408,7 @@
         <v>271</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>164</v>
@@ -5426,13 +5416,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="46" t="s">
+        <v>299</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -5481,33 +5471,33 @@
       <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54" t="s">
+      <c r="E1" s="55"/>
+      <c r="F1" s="55" t="s">
         <v>201</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54" t="s">
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55" t="s">
         <v>200</v>
       </c>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
       <c r="T1" s="1" t="s">
         <v>271</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -6672,7 +6662,7 @@
         <v>210</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>5</v>
@@ -7164,7 +7154,7 @@
         <v>17</v>
       </c>
       <c r="C30" s="43" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>5</v>
@@ -7349,7 +7339,7 @@
         <v>217</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>232</v>
@@ -7780,7 +7770,7 @@
         <v>14</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>5</v>
@@ -8363,24 +8353,24 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding more protocol content
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDC3A6E-8306-2341-AAEA-ED57214B0EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0166703C-73A8-EA4C-B3D3-D41E03454D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="589">
   <si>
     <t>Epoch</t>
   </si>
@@ -1914,6 +1914,61 @@
   </si>
   <si>
     <t>Safety and Efficacy of the Xanomeline Transdermal Therapeutic System (TTS) in Patients with Mild to Moderate Alzheimer's Disease</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>TITLE PAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;table&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Protocol Full Title:&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="StudyProtocolVersion" id="StudyProtocolVersion_1" attribute="officialTitle"/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Protocol Number:&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="StudyIdentifier" id="StudyIdentifier_1" attribute="studyIdentifier"/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Version:&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Amendment Number:&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Amendment Scope:&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Compound Number(s):&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt; 
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Compound Name(s):&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;  
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Trial Phase:&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="Code" id="Code_2" attribute="decode"/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Acronym:&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="Study" namexref="STUDY" attribute="studyAcronym"/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Short Title:&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="StudyProtocolVersion" id="StudyProtocolVersion_1" attribute="briefTitle"/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Sponsor Name and Address:&lt;/p&gt;&lt;/th&gt;
+    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+&lt;/table&gt;
+</t>
   </si>
 </sst>
 </file>
@@ -2158,13 +2213,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2485,7 +2540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -3716,10 +3771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
-  <dimension ref="A1:D138"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3727,7 +3782,7 @@
     <col min="1" max="1" width="14.1640625" style="15" customWidth="1"/>
     <col min="2" max="2" width="16" style="3" customWidth="1"/>
     <col min="3" max="3" width="49.83203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="81.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="129.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3744,1187 +3799,1194 @@
         <v>314</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>315</v>
+    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A2" s="50" t="s">
+        <v>586</v>
       </c>
       <c r="B2" s="48"/>
       <c r="C2" s="6" t="s">
-        <v>316</v>
+        <v>587</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>317</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="B3" s="48"/>
       <c r="C3" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="388" x14ac:dyDescent="0.2">
-      <c r="A10" s="50" t="s">
+    <row r="11" spans="1:4" ht="388" x14ac:dyDescent="0.2">
+      <c r="A11" s="50" t="s">
         <v>582</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>584</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="B13" s="48"/>
+        <v>333</v>
+      </c>
       <c r="C13" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B15" s="48"/>
       <c r="C15" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B17" s="48"/>
       <c r="C17" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B18" s="48"/>
       <c r="C18" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B19" s="48"/>
       <c r="C19" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B20" s="48"/>
       <c r="C20" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B21" s="48"/>
       <c r="C21" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B22" s="48"/>
       <c r="C22" s="6" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B23" s="48"/>
       <c r="C23" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B24" s="48"/>
       <c r="C24" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B25" s="48"/>
       <c r="C25" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B26" s="48"/>
       <c r="C26" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B27" s="48"/>
       <c r="C27" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B28" s="48"/>
       <c r="C28" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B29" s="48"/>
       <c r="C29" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B31" s="48"/>
       <c r="C31" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B32" s="48"/>
       <c r="C32" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B33" s="48"/>
       <c r="C33" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B34" s="48"/>
       <c r="C34" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B40" s="48"/>
       <c r="C40" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B41" s="48"/>
       <c r="C41" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B42" s="48"/>
       <c r="C42" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B43" s="48"/>
       <c r="C43" s="6" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B44" s="48"/>
       <c r="C44" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B45" s="48"/>
       <c r="C45" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B46" s="48"/>
       <c r="C46" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B47" s="48"/>
       <c r="C47" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B48" s="48"/>
       <c r="C48" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B49" s="48"/>
       <c r="C49" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B50" s="48"/>
       <c r="C50" s="6" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B51" s="48"/>
       <c r="C51" s="6" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B52" s="48"/>
       <c r="C52" s="6" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B53" s="48"/>
       <c r="C53" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B54" s="48"/>
       <c r="C54" s="6" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B55" s="48"/>
       <c r="C55" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B56" s="48"/>
       <c r="C56" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B57" s="48"/>
       <c r="C57" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B58" s="48"/>
       <c r="C58" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B59" s="48"/>
       <c r="C59" s="6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B60" s="48"/>
       <c r="C60" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B61" s="48"/>
       <c r="C61" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B62" s="48"/>
       <c r="C62" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B63" s="48"/>
       <c r="C63" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B64" s="48"/>
       <c r="C64" s="6" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B65" s="48"/>
       <c r="C65" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B66" s="48"/>
       <c r="C66" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B67" s="48"/>
       <c r="C67" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B68" s="48"/>
       <c r="C68" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B69" s="48"/>
       <c r="C69" s="6" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B70" s="48"/>
       <c r="C70" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B71" s="48"/>
       <c r="C71" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B72" s="48"/>
       <c r="C72" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B73" s="48"/>
       <c r="C73" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B74" s="48"/>
       <c r="C74" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B75" s="48"/>
       <c r="C75" s="6" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B76" s="48"/>
       <c r="C76" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="15" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B77" s="48"/>
       <c r="C77" s="6" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B78" s="48"/>
       <c r="C78" s="6" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B79" s="48"/>
       <c r="C79" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B80" s="48"/>
       <c r="C80" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="15" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B81" s="48"/>
       <c r="C81" s="6" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B82" s="48"/>
       <c r="C82" s="6" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B83" s="48"/>
       <c r="C83" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B84" s="48"/>
       <c r="C84" s="6" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B85" s="48"/>
       <c r="C85" s="6" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B86" s="48"/>
       <c r="C86" s="6" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B87" s="48"/>
       <c r="C87" s="6" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B88" s="48"/>
       <c r="C88" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="15" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B89" s="48"/>
       <c r="C89" s="6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B90" s="48"/>
       <c r="C90" s="6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="s">
-        <v>429</v>
+        <v>489</v>
       </c>
       <c r="B91" s="48"/>
       <c r="C91" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
-        <v>492</v>
+        <v>429</v>
       </c>
       <c r="B92" s="48"/>
       <c r="C92" s="6" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B93" s="48"/>
       <c r="C93" s="6" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B94" s="48"/>
       <c r="C94" s="6" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B95" s="48"/>
       <c r="C95" s="6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B96" s="48"/>
       <c r="C96" s="6" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B97" s="48"/>
       <c r="C97" s="6" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B98" s="48"/>
       <c r="C98" s="6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="15" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B99" s="48"/>
       <c r="C99" s="6" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="15" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B100" s="48"/>
       <c r="C100" s="6" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B101" s="48"/>
       <c r="C101" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="15" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B102" s="48"/>
       <c r="C102" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B103" s="48"/>
       <c r="C103" s="6" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B104" s="48"/>
       <c r="C104" s="6" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B105" s="48"/>
       <c r="C105" s="6" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B106" s="48"/>
       <c r="C106" s="6" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B107" s="48"/>
       <c r="C107" s="6" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B108" s="48"/>
       <c r="C108" s="6" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B109" s="48"/>
       <c r="C109" s="6" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B110" s="48"/>
       <c r="C110" s="6" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="15" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B111" s="48"/>
       <c r="C111" s="6" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B112" s="48"/>
       <c r="C112" s="6" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="15" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B113" s="48"/>
       <c r="C113" s="6" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B114" s="48"/>
       <c r="C114" s="6" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="15" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B115" s="48"/>
       <c r="C115" s="6" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="15" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B116" s="48"/>
       <c r="C116" s="6" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="15" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B117" s="48"/>
       <c r="C117" s="6" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="15" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B118" s="48"/>
       <c r="C118" s="6" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" s="15" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B119" s="48"/>
       <c r="C119" s="6" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B120" s="48"/>
       <c r="C120" s="6" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="15" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B121" s="48"/>
       <c r="C121" s="6" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="15" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B122" s="48"/>
       <c r="C122" s="6" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="15" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B123" s="48"/>
       <c r="C123" s="6" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="15" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B124" s="48"/>
       <c r="C124" s="6" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="15" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B125" s="48"/>
       <c r="C125" s="6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="15" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B126" s="48"/>
       <c r="C126" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="15" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B127" s="48"/>
       <c r="C127" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="15" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B128" s="48"/>
       <c r="C128" s="6" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="15" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B129" s="48"/>
       <c r="C129" s="6" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="15" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B130" s="48"/>
       <c r="C130" s="6" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="15" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B131" s="48"/>
       <c r="C131" s="6" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="15" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B132" s="48"/>
       <c r="C132" s="6" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="B133" s="48"/>
+      <c r="C133" s="6" t="s">
         <v>573</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" s="15" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -4949,6 +5011,11 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="15" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="15" t="s">
         <v>574</v>
       </c>
     </row>
@@ -5064,36 +5131,36 @@
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="54" t="s">
         <v>272</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -5110,7 +5177,7 @@
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="53" t="s">
         <v>165</v>
       </c>
       <c r="C7" s="51"/>
@@ -5237,16 +5304,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update for Objectives and Endpoints
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED223D7-254A-5348-A2C6-656D81B5CC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E9C4D9-BD37-284B-8B6F-B11F83B5030D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="660" windowWidth="50380" windowHeight="27240" firstSheet="6" activeTab="20" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="23700" yWindow="500" windowWidth="50380" windowHeight="27240" firstSheet="6" activeTab="20" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="712">
   <si>
     <t>Screening</t>
   </si>
@@ -1564,83 +1564,6 @@
 &lt;p&gt;The investigator should make every effort to contact the clinical research physician prior to unblinding a patient’s therapy assignment. If a patient’s therapy assignment is unblinded, Lilly must be notified immediately by telephone. After the study, the investigator must return all sealed and any opened codes.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Patients may be included in the study only if they meet &lt;strong&gt;all&lt;/strong&gt; the following criteria:&lt;/p&gt;
-&lt;table&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;[1]&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;
-      Males and postmenopausal females at least 50 years of age.
-    &lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;[2]&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;Diagnosis of probable AD as defined by National Institute of Neurological and Communicative Disorders and Stroke
-      (NINCDS) and the Alzheimer’s Disease and Related Disorders Association (ADRDA) guidelines (Attachment LZZT.7).
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;[3]&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;MMSE score of 10 to 23.&lt;/td&gt; 
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;[4]&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;Hachinski Ischemic Scale score of ≤4 (Attachment LZZT.8).&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;[5]&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;CNS imaging (CT scan or MRI of brain) compatible with AD within past 1 year.
-      The following findings are incompatible with AD:
-      &lt;ol type="a"&gt;
-        &lt;li&gt;Large vessel strokes
-          &lt;ol type="1"&gt;
-            &lt;li&gt;Any definite area of encephalomalacia consistent with ischemic necrosis in any cerebral artery
-              territory.&lt;/li&gt;
-            &lt;li&gt;Large, confluent areas of encephalomalacia in parieto-occipital or frontal regions consistent with
-              watershed infarcts. The above are exclusionary. Exceptions are made for small areas of cortical asymmetry
-              which may represent a small cortical stroke or a focal area of atrophy provided there is no abnormal
-              signal intensity in the immediately underlying parenchyma. Only one such questionable area allowed per
-              scan, and size is restricted to ≤1cm in frontal/parietal/temporal cortices and ≤2 cm in occipital cortex.
-            &lt;/li&gt;
-          &lt;/ol&gt;
-        &lt;/li&gt;
-        &lt;li&gt;Small vessel ischemia
-          &lt;ol type="1"&gt;
-            &lt;li&gt;Lacunar infarct is defined as an area of abnormal intensity seen on CT scan or on both T1 and T2
-              weighted MRI images in the basal ganglia, thalamus or deep white matter which is ≤1 cm in maximal
-              diameter. A maximum of one lacune is allowed per scan.&lt;/li&gt;
-            &lt;li&gt;Leukoariosis or leukoencephalopathy is regarded as an abnormality seen on T2 but not T1 weighted MRIs,
-              or on CT. This is accepted if mild or moderate in extent, meaning involvement of less than 25% of cortical
-              white matter.&lt;/li&gt;
-          &lt;/ol&gt;
-        &lt;/li&gt;
-        &lt;li&gt;Miscellaneous
-          &lt;ol type="1"&gt;
-            &lt;li&gt;Benign small extra-axial tumors (ie, meningiomas) are accepted if they do not contact or indent the
-              brain parenchyma.&lt;/li&gt;
-            &lt;li&gt;extra-axial arachnoid cysts are accepted if they do not indent or deform the brain parenchyma.&lt;/li&gt;
-          &lt;/ol&gt;
-        &lt;/li&gt;
-      &lt;/ol&gt;
-    &lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;[6]&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;Investigator has obtained informed consent signed by the patient (and/or legal representative) and by the
-      caregiver.&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;[7]&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;Geographic proximity to investigator’s site that allows adequate follow-up.&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;[8]&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;A reliable caregiver who is in frequent or daily contact with the patient and who will accompany the patient to
-      the office and/or be available by telephone at designated times, will monitor administration of prescribed
-      medications, and will be responsible for the overall care of the patient at home. The caregiver and the patient
-      must be able to communicate in English and willing to comply with 26 weeks of transdermal therapy.&lt;/td&gt;
-  &lt;/tr&gt;
-&lt;table&gt;</t>
-  </si>
-  <si>
     <t>Alzheimer's Disease Assessment Scale - Cognitive Subscale, total of 11 items [ADAS-Cog (11)] at Week 24</t>
   </si>
   <si>
@@ -1662,29 +1585,6 @@
     <t>Primary Objectives</t>
   </si>
   <si>
-    <t>&lt;table&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top"&gt;&lt;p&gt;Primary Objective&lt;/p&gt;&lt;/th&gt;
-    &lt;th style="vertical-align: top"&gt;&lt;p&gt;Primary Endpoint&lt;/p&gt;&lt;/th&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;&lt;p&gt;&lt;usdm:ref klass="Objective" namexref="OBJ1" attribute="description"/&gt;&lt;/p&gt;&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;
-      &lt;p&gt;&lt;usdm:ref klass="Endpoint" namexref="END1" attribute="description"/&gt;&lt;/p&gt;
-      &lt;p&gt;&lt;usdm:ref klass="Endpoint" namexref="END2" attribute="description"/&gt;&lt;/p&gt;
-    &lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;&lt;p&gt;&lt;usdm:ref klass="Objective" namexref="OBJ2" attribute="description"/&gt;&lt;/p&gt;&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;
-      &lt;p&gt;&lt;usdm:ref klass="Endpoint" namexref="END3" attribute="description"/&gt;&lt;/p&gt;
-      &lt;p&gt;&lt;usdm:ref klass="Endpoint" namexref="END4" attribute="description"/&gt;&lt;/p&gt;
-      &lt;p&gt;&lt;usdm:ref klass="Endpoint" namexref="END5" attribute="description"/&gt;&lt;/p&gt;
-    &lt;/td&gt;
-  &lt;/tr&gt;
-&lt;/table&gt;</t>
-  </si>
-  <si>
     <t>Safety and Efficacy of the Xanomeline Transdermal Therapeutic System (TTS) in Patients with Mild to Moderate Alzheimer's Disease</t>
   </si>
   <si>
@@ -1692,55 +1592,6 @@
   </si>
   <si>
     <t>TITLE PAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;table&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Protocol Full Title:&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="StudyProtocolVersion" id="StudyProtocolVersion_1" attribute="officialTitle"/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Protocol Number:&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="StudyIdentifier" id="StudyIdentifier_1" attribute="studyIdentifier"/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Version:&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Amendment Number:&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Amendment Scope:&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Compound Number(s):&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt; 
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Compound Name(s):&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;  
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Trial Phase:&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="Code" id="Code_2" attribute="decode"/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Acronym:&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="Study" namexref="STUDY" attribute="studyAcronym"/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Short Title:&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="StudyProtocolVersion" id="StudyProtocolVersion_1" attribute="briefTitle"/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top; text-align: left"&gt;&lt;p&gt;Sponsor Name and Address:&lt;/p&gt;&lt;/th&gt;
-    &lt;td style="vertical-align: top; text-align: left"&gt;&lt;p&gt;&lt;usdm:ref klass="" namexref="" attribute=""/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-&lt;/table&gt;
-</t>
   </si>
   <si>
     <t>category</t>
@@ -2333,6 +2184,18 @@
   </si>
   <si>
     <t>Screen One</t>
+  </si>
+  <si>
+    <t>&lt;usdm:section name="M11-title-page"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;usdm:section name="M11-inclusion"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;usdm:section name="M11-exclusion"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;usdm:section name="M11-objective-endpoints"&gt;</t>
   </si>
 </sst>
 </file>
@@ -2569,10 +2432,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2910,7 +2773,7 @@
         <v>237</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
@@ -2920,7 +2783,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E2" s="41"/>
       <c r="F2" s="41"/>
@@ -3000,7 +2863,7 @@
         <v>71</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E10" s="41"/>
       <c r="F10" s="41"/>
@@ -3010,7 +2873,7 @@
         <v>72</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E11" s="41"/>
       <c r="F11" s="41"/>
@@ -3049,7 +2912,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="42" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B16" s="42" t="s">
         <v>237</v>
@@ -3058,62 +2921,62 @@
         <v>37</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>36</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="G16" s="42" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="C17" t="s">
+        <v>517</v>
+      </c>
+      <c r="D17" t="s">
         <v>518</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="E17" t="s">
         <v>519</v>
-      </c>
-      <c r="C17" t="s">
-        <v>520</v>
-      </c>
-      <c r="D17" t="s">
-        <v>521</v>
-      </c>
-      <c r="E17" t="s">
-        <v>522</v>
       </c>
       <c r="F17" s="43">
         <v>38899</v>
       </c>
       <c r="G17" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="C18" t="s">
+        <v>521</v>
+      </c>
+      <c r="D18" t="s">
+        <v>522</v>
+      </c>
+      <c r="E18" t="s">
         <v>523</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>519</v>
-      </c>
-      <c r="C18" t="s">
-        <v>524</v>
-      </c>
-      <c r="D18" t="s">
-        <v>525</v>
-      </c>
-      <c r="E18" t="s">
-        <v>526</v>
       </c>
       <c r="F18" s="43">
         <v>38899</v>
       </c>
       <c r="G18" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -3144,13 +3007,13 @@
         <v>85</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>237</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3158,7 +3021,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>37</v>
@@ -3172,13 +3035,13 @@
         <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3188,38 +3051,38 @@
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="17" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="17" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="17" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="17" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3246,7 +3109,7 @@
     <row r="11" spans="1:4" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="3" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>213</v>
@@ -3291,7 +3154,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -3310,7 +3173,7 @@
     <row r="17" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
@@ -3320,7 +3183,7 @@
     <row r="18" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="1" t="s">
@@ -3382,10 +3245,10 @@
     <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>705</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>708</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>1</v>
@@ -3576,519 +3439,519 @@
         <v>37</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D1" s="44" t="s">
         <v>36</v>
       </c>
       <c r="E1" s="44" t="s">
+        <v>543</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>544</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>545</v>
+      </c>
+      <c r="H1" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="I1" s="44" t="s">
         <v>547</v>
-      </c>
-      <c r="G1" s="44" t="s">
-        <v>548</v>
-      </c>
-      <c r="H1" s="44" t="s">
-        <v>549</v>
-      </c>
-      <c r="I1" s="44" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>557</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>562</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>565</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>153</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>217</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>154</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>155</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>156</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>157</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>158</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>670</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="41" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="41" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -4122,13 +3985,13 @@
         <v>37</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4196,10 +4059,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C14" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -4249,7 +4112,7 @@
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -4259,10 +4122,10 @@
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -4297,7 +4160,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
   </sheetData>
@@ -4340,7 +4203,7 @@
         <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C2" t="s">
         <v>230</v>
@@ -4354,7 +4217,7 @@
         <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C3" t="s">
         <v>230</v>
@@ -4408,7 +4271,7 @@
     </row>
     <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>210</v>
@@ -4457,34 +4320,34 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>45</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>46</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>47</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="K1" s="21" t="s">
         <v>48</v>
@@ -4497,11 +4360,11 @@
         <v>62</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>50</v>
@@ -4511,7 +4374,7 @@
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="16" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="14" t="s">
@@ -4528,7 +4391,7 @@
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="J3" s="16"/>
       <c r="K3" s="14" t="s">
@@ -4543,10 +4406,10 @@
         <v>63</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>50</v>
@@ -4587,7 +4450,7 @@
         <v>67</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I6" s="16" t="s">
         <v>215</v>
@@ -4605,11 +4468,11 @@
         <v>182</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>51</v>
@@ -4619,7 +4482,7 @@
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J7" s="16"/>
       <c r="K7" s="14" t="s">
@@ -4635,7 +4498,7 @@
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="14" t="s">
@@ -4922,7 +4785,7 @@
         <v>37</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>91</v>
@@ -4993,16 +4856,16 @@
         <v>37</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>98</v>
@@ -5034,7 +4897,7 @@
         <v>104</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -5163,7 +5026,7 @@
         <v>141</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -5183,7 +5046,7 @@
         <v>141</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -5203,7 +5066,7 @@
         <v>141</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -5223,7 +5086,7 @@
         <v>141</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -5301,7 +5164,7 @@
         <v>37</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>98</v>
@@ -5363,7 +5226,7 @@
         <v>190</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>186</v>
@@ -5377,7 +5240,7 @@
         <v>193</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D6" s="46" t="s">
         <v>192</v>
@@ -5391,7 +5254,7 @@
         <v>190</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D7" s="46" t="s">
         <v>194</v>
@@ -5405,7 +5268,7 @@
         <v>123</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="D8" s="47" t="s">
         <v>196</v>
@@ -5438,22 +5301,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
+        <v>527</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>529</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>530</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="E1" s="42" t="s">
         <v>531</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="F1" s="45" t="s">
         <v>532</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>533</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>534</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5461,19 +5324,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>533</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>534</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>536</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>537</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>538</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>540</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -5505,39 +5368,39 @@
         <v>37</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>60</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B2" t="s">
+        <v>609</v>
+      </c>
+      <c r="C2" t="s">
+        <v>610</v>
+      </c>
+      <c r="D2" t="s">
+        <v>611</v>
+      </c>
+      <c r="E2" t="s">
         <v>612</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>613</v>
-      </c>
-      <c r="D2" t="s">
-        <v>614</v>
-      </c>
-      <c r="E2" t="s">
-        <v>615</v>
-      </c>
-      <c r="F2" t="s">
-        <v>616</v>
       </c>
       <c r="G2" t="s">
         <v>41</v>
@@ -5545,13 +5408,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E3" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F3" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="G3" t="s">
         <v>42</v>
@@ -5567,7 +5430,7 @@
   <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5592,16 +5455,16 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>513</v>
+        <v>708</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5669,15 +5532,15 @@
         <v>255</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="388" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="40" t="s">
+        <v>506</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>508</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>509</v>
+        <v>711</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5786,7 +5649,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>280</v>
       </c>
@@ -5795,7 +5658,7 @@
         <v>281</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>501</v>
+        <v>709</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5806,6 +5669,9 @@
       <c r="C25" s="6" t="s">
         <v>283</v>
       </c>
+      <c r="D25" s="6" t="s">
+        <v>710</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
@@ -6814,6 +6680,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6917,24 +6784,24 @@
         <v>211</v>
       </c>
       <c r="F2" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>538</v>
+      </c>
+      <c r="B3" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3" t="s">
+        <v>540</v>
+      </c>
+      <c r="D3" t="s">
         <v>541</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>542</v>
-      </c>
-      <c r="C3" t="s">
-        <v>543</v>
-      </c>
-      <c r="D3" t="s">
-        <v>544</v>
-      </c>
-      <c r="E3" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -6990,24 +6857,24 @@
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="50" t="s">
         <v>209</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -7038,8 +6905,8 @@
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>704</v>
+      <c r="B7" s="51" t="s">
+        <v>701</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
@@ -7075,7 +6942,7 @@
         <v>84</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="C10" s="49"/>
       <c r="D10" s="49"/>
@@ -7111,7 +6978,7 @@
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>118</v>
@@ -7171,16 +7038,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7208,10 +7075,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>237</v>
@@ -7220,33 +7087,33 @@
         <v>37</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>239</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>600</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="C2" t="s">
+        <v>602</v>
+      </c>
+      <c r="D2" t="s">
         <v>603</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="F2" t="s">
         <v>604</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>605</v>
-      </c>
-      <c r="D2" t="s">
-        <v>606</v>
-      </c>
-      <c r="F2" t="s">
-        <v>607</v>
-      </c>
-      <c r="G2" t="s">
-        <v>608</v>
       </c>
     </row>
   </sheetData>
@@ -7279,16 +7146,16 @@
         <v>37</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7380,7 +7247,7 @@
         <v>37</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>36</v>
@@ -7408,7 +7275,7 @@
         <v>226</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>136</v>
@@ -7422,7 +7289,7 @@
         <v>226</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>136</v>
@@ -7436,7 +7303,7 @@
         <v>226</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>136</v>
@@ -7450,7 +7317,7 @@
         <v>228</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>229</v>
@@ -7500,52 +7367,52 @@
         <v>237</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>584</v>
-      </c>
       <c r="S1" s="10" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -7615,16 +7482,16 @@
         <v>90</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>144</v>
@@ -7639,25 +7506,25 @@
         <v>217</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>154</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>155</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>156</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>157</v>
@@ -7673,121 +7540,121 @@
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="17" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="J5" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="N5" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="P5" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="10" t="s">
+        <v>645</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>648</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="17" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="17" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -7842,7 +7709,7 @@
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="17" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>100</v>
@@ -8569,7 +8436,7 @@
     <row r="22" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="3" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>213</v>
@@ -9016,7 +8883,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>1</v>
@@ -9125,7 +8992,7 @@
     <row r="32" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="6" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="30" t="s">
@@ -9237,7 +9104,7 @@
     <row r="34" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="6" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="1" t="s">
@@ -10031,13 +9898,13 @@
         <v>85</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>237</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="17" x14ac:dyDescent="0.2">
@@ -10045,7 +9912,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>37</v>
@@ -10059,13 +9926,13 @@
         <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -10075,38 +9942,38 @@
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="17" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="17" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="17" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="17" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add in Berber examples for workshop
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E9C4D9-BD37-284B-8B6F-B11F83B5030D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE547185-6B5D-5740-9B47-065C4F665496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23700" yWindow="500" windowWidth="50380" windowHeight="27240" firstSheet="6" activeTab="20" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="16720" yWindow="500" windowWidth="50380" windowHeight="27240" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="727">
   <si>
     <t>Screening</t>
   </si>
@@ -2196,6 +2196,51 @@
   </si>
   <si>
     <t>&lt;usdm:section name="M11-objective-endpoints"&gt;</t>
+  </si>
+  <si>
+    <t>StudyPopulation</t>
+  </si>
+  <si>
+    <t>AS_Dict</t>
+  </si>
+  <si>
+    <t>Dictionary for Study Assessments</t>
+  </si>
+  <si>
+    <t>Assessment Dictionary</t>
+  </si>
+  <si>
+    <t>Activity1</t>
+  </si>
+  <si>
+    <t>MMSE</t>
+  </si>
+  <si>
+    <t>Hachinski</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>Pop Criteria</t>
+  </si>
+  <si>
+    <t>The study population criterion</t>
+  </si>
+  <si>
+    <t>[StudyPopulation] as defined by the NINCDS and the ADRDA guidelines (Attachment LZZT.7)</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Diag Criteria</t>
+  </si>
+  <si>
+    <t>The study diagnosis criterion</t>
+  </si>
+  <si>
+    <t>[Activity1] score of 10 to 23</t>
   </si>
 </sst>
 </file>
@@ -2432,10 +2477,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2990,7 +3035,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3418,7 +3463,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3965,7 +4010,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4019,12 +4064,12 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>162</v>
+        <v>718</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>163</v>
+        <v>717</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -5346,15 +5391,17 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989384DC-1C54-514A-8A1E-ADD84D891BA4}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="16" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" customWidth="1"/>
     <col min="7" max="7" width="31.1640625" customWidth="1"/>
@@ -5418,6 +5465,43 @@
       </c>
       <c r="G3" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>712</v>
+      </c>
+      <c r="E4" t="s">
+        <v>612</v>
+      </c>
+      <c r="F4" t="s">
+        <v>613</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>713</v>
+      </c>
+      <c r="B5" t="s">
+        <v>714</v>
+      </c>
+      <c r="C5" t="s">
+        <v>715</v>
+      </c>
+      <c r="D5" t="s">
+        <v>716</v>
+      </c>
+      <c r="E5" t="s">
+        <v>583</v>
+      </c>
+      <c r="F5" t="s">
+        <v>717</v>
+      </c>
+      <c r="G5" t="s">
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -5429,16 +5513,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="3" width="49.83203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="129.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="14" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24" style="6" customWidth="1"/>
+    <col min="4" max="4" width="44.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5844,7 +5928,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="181" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>322</v>
       </c>
@@ -6857,24 +6941,24 @@
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -6905,7 +6989,7 @@
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="50" t="s">
         <v>701</v>
       </c>
       <c r="C7" s="49"/>
@@ -7038,16 +7122,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7057,10 +7141,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1EE44-0F6C-474B-8770-DA2A14736511}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7068,9 +7152,9 @@
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" customWidth="1"/>
-    <col min="6" max="6" width="64.83203125" customWidth="1"/>
+    <col min="6" max="6" width="79" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -7114,6 +7198,46 @@
       </c>
       <c r="G2" t="s">
         <v>605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>600</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="C3" t="s">
+        <v>720</v>
+      </c>
+      <c r="D3" t="s">
+        <v>721</v>
+      </c>
+      <c r="F3" t="s">
+        <v>722</v>
+      </c>
+      <c r="G3" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>600</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>723</v>
+      </c>
+      <c r="C4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D4" t="s">
+        <v>725</v>
+      </c>
+      <c r="F4" t="s">
+        <v>726</v>
+      </c>
+      <c r="G4" t="s">
+        <v>713</v>
       </c>
     </row>
   </sheetData>
@@ -7333,7 +7457,7 @@
   <dimension ref="A1:V68"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add eligibility criteria (exclusion)
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718AF4CC-6791-9840-8888-411F7AEC427E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB716AE-4D6C-2342-B993-40DB65B61883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26820" yWindow="500" windowWidth="50380" windowHeight="27240" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="26820" yWindow="500" windowWidth="61200" windowHeight="27240" activeTab="19" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1654" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="736">
   <si>
     <t>Screening</t>
   </si>
@@ -4057,7 +4057,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4116,6 +4116,9 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="C7" t="s">
         <v>717</v>
       </c>
     </row>
@@ -5440,8 +5443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989384DC-1C54-514A-8A1E-ADD84D891BA4}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7202,8 +7205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1EE44-0F6C-474B-8770-DA2A14736511}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updates for new version of USDM package
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5934A97A-B1B8-E449-8EC6-8B43D6B67F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5ACB54C-97B7-1A4E-9DC6-A93F42D9F4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31360" yWindow="500" windowWidth="47700" windowHeight="27240" firstSheet="12" activeTab="23" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="31360" yWindow="500" windowWidth="47700" windowHeight="27240" firstSheet="12" activeTab="13" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="818">
   <si>
     <t>Screening</t>
   </si>
@@ -2526,9 +2526,6 @@
   </si>
   <si>
     <t>If this is true</t>
-  </si>
-  <si>
-    <t>Procedures</t>
   </si>
   <si>
     <t>@plannedAge/Range/@minValue</t>
@@ -2749,15 +2746,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2766,6 +2754,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2785,9 +2782,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2825,7 +2822,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2931,7 +2928,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3073,7 +3070,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4547,22 +4544,22 @@
       <c r="C3" s="14" t="s">
         <v>499</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="43" t="s">
         <v>718</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="44" t="s">
         <v>763</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="44" t="s">
         <v>764</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="44" t="s">
         <v>765</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="44" t="s">
         <v>766</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="44" t="s">
         <v>767</v>
       </c>
     </row>
@@ -5541,8 +5538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8C14B1-8C62-2C45-8CB1-1E9EDDA367B1}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5588,7 +5585,7 @@
         <v>813</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>814</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>90</v>
@@ -6040,7 +6037,7 @@
       <c r="H1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="45" t="s">
         <v>779</v>
       </c>
     </row>
@@ -6052,7 +6049,7 @@
         <v>598</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E2" s="3">
         <v>300</v>
@@ -7174,7 +7171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989384DC-1C54-514A-8A1E-ADD84D891BA4}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -7231,7 +7228,7 @@
         <v>598</v>
       </c>
       <c r="G2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -7245,7 +7242,7 @@
         <v>598</v>
       </c>
       <c r="G3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -8710,144 +8707,144 @@
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="44" t="s">
-        <v>817</v>
-      </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
+      <c r="B3" s="48" t="s">
+        <v>816</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
     </row>
     <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="46" t="s">
         <v>682</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>805</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="47" t="s">
         <v>806</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>807</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="47" t="s">
         <v>808</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="46" t="s">
         <v>717</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -8939,6 +8936,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:F4"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -8946,11 +8948,6 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11919,26 +11916,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -12139,32 +12116,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12181,4 +12153,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update CDISC Pilot Study
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C1A7D0-CE88-1043-9209-96450C8735B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF1932B-CA56-EE46-ABC9-EA26FB11E249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31360" yWindow="500" windowWidth="47700" windowHeight="27240" firstSheet="12" activeTab="24" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="1580" yWindow="500" windowWidth="47700" windowHeight="27240" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="908">
   <si>
     <t>Screening</t>
   </si>
@@ -1826,15 +1826,6 @@
     <t>01</t>
   </si>
   <si>
-    <t>Age Criteria</t>
-  </si>
-  <si>
-    <t>The study age criterion</t>
-  </si>
-  <si>
-    <t>Subjects shall be between [min_age] and [max_age]</t>
-  </si>
-  <si>
     <t>IE_Dict</t>
   </si>
   <si>
@@ -2157,25 +2148,7 @@
     <t>02</t>
   </si>
   <si>
-    <t>Pop Criteria</t>
-  </si>
-  <si>
-    <t>The study population criterion</t>
-  </si>
-  <si>
-    <t>[StudyPopulation] as defined by the NINCDS and the ADRDA guidelines (Attachment LZZT.7)</t>
-  </si>
-  <si>
     <t>03</t>
-  </si>
-  <si>
-    <t>Diag Criteria</t>
-  </si>
-  <si>
-    <t>The study diagnosis criterion</t>
-  </si>
-  <si>
-    <t>[Activity1] score of 10 to 23</t>
   </si>
   <si>
     <t>&lt;p&gt;Previous studies of the oral formulation have shown that xanomeline tartrate may improve behavior and cognition. Effects on behavior are manifest within 2 to 4 weeks of initiation of treatment. The same studies have shown that 8 to 12 weeks are required to demonstrate effects on cognition and clinical global assessment. This study is intended to determine the acute and chronic effects of the TTS formulation in AD; for that reason, the study is of 26 weeks duration. Dosage specification has been made on the basis of tolerance to the xanomeline TTS in a clinical pharmacology study (H2Q-EW-LKAA), and target plasma levels as determined in studies of the oral formulation of xanomeline (H2Q-MC-LZZA).&lt;/p&gt;</t>
@@ -2216,15 +2189,6 @@
     <t>09</t>
   </si>
   <si>
-    <t>Persons who have previously completed or withdrawn from this study or any other study investigating xanomeline TTS or the oral formulation of xanomeline.</t>
-  </si>
-  <si>
-    <t>Previous Criteria</t>
-  </si>
-  <si>
-    <t>The previous xanomeline TTS criterion</t>
-  </si>
-  <si>
     <t>adverseEventTimeline, earlyTerminationTimeline, vsBloodPressure</t>
   </si>
   <si>
@@ -2538,6 +2502,415 @@
   </si>
   <si>
     <t>&lt;usdm:macro id="section" name="exclusion" template="M11"/&gt;</t>
+  </si>
+  <si>
+    <t>To assess the dose-dependent improvements in activities of daily living. Improved scores on the Disability Assessment for Dementia (DAD) will indicate improvement in these areas (see Attachment LZZT.5).</t>
+  </si>
+  <si>
+    <t>To assess the dose-dependent improvements in an extended assessment of cognition that integrates attention/concentration tasks. The Alzheimer's Disease Assessment Scale-14 item Cognitive Subscale, hereafter referred to as ADAS-Cog (14), will be used for this assessment (see Attachment LZZT.2).</t>
+  </si>
+  <si>
+    <t>To assess the treatment response as a function of Apo E genotype.</t>
+  </si>
+  <si>
+    <t>OBJ4</t>
+  </si>
+  <si>
+    <t>OBJ5</t>
+  </si>
+  <si>
+    <t>OBJ6</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Males and postmenopausal females at least 50 years of age.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Diagnosis of probable AD as defined by National Institute of Neurological and Communicative Disorders and Stroke (NINCDS) and the Alzheimer's Disease and Related Disorders Association (ADRDA) guidelines (Attachment LZZT.7).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;MMSE score of 10 to 23.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Hachinski Ischemic Scale score of ≤4 (Attachment LZZT.8).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Investigator has obtained informed consent signed by the patient (and/or legal representative) and by the caregiver.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Geographic proximity to investigator's site that allows adequate follow-up.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A reliable caregiver who is in frequent or daily contact with the patient and who will accompany the patient to the office and/or be available by telephone at designated times, will monitor administration of prescribed medications, and will be responsible for the overall care of the patient at home. The caregiver and the patient must be able to communicate in English and willing to comply with 26 weeks of transdermal therapy.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;CNS imaging (CT scan or MRI of brain) compatible with AD within past 1 year.&lt;/p&gt;
+&lt;p&gt;The following findings are incompatible with AD:&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;
+&lt;p&gt;Large vessel strokes&lt;/p&gt;
+&lt;ol&gt;
+&lt;li&gt;&lt;p&gt;Any definite area of encephalomalacia consistent with ischemic necrosis in any cerebral artery territory.&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Large, confluent areas of encephalomalacia in parieto-occipital or frontal regions consistent with watershed infarcts.&lt;/p&gt;&lt;/li&gt;
+&lt;p&gt;The above are exclusionary. Exceptions are made for small areas of cortical asymmetry which may represent a small cortical stroke or a focal area of atrophy provided there is no abnormal signal intensity in the immediately underlying parenchyma. Only one such questionable area allowed per scan, and size is restricted to ≤1cm in frontal/parietal/temporal cortices and ≤2 cm in occipital cortex.&lt;/p&gt;
+&lt;/li&gt;
+&lt;/ol&gt;
+&lt;li&gt;
+&lt;p&gt;Small vessel ischemia&lt;/p&gt;
+&lt;ol&gt;
+&lt;li&gt;&lt;p&gt;Lacunar infarct is defined as an area of abnormal intensity seen on CT scan or on both T1 and T2 weighted MRI images in the basal ganglia, thalamus or deep white matter which is ≤1 cm in maximal diameter. A maximum of one lacune is allowed per scan.&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Leukoariosis or leukoencephalopathy is regarded as an abnormality seen on T2 but not T1 weighted MRIs, or on CT. This is accepted if mild or moderate in extent, meaning involvement of less than 25% of cortical white matter. &lt;/li&gt;
+&lt;/ol&gt;
+&lt;li&gt;&lt;p&gt;Miscellaneous&lt;/p&gt;
+&lt;ol&gt;
+&lt;li&gt;&lt;p&gt;Benign small extra-axial tumors (ie, meningiomas) are accepted if they do not contact or indent the brain parenchyma.&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Small extra-axial arachnoid cysts are accepted if they do not indent or deform the brain parenchyma.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>DIAGNOSIS</t>
+  </si>
+  <si>
+    <t>CNS IMAGING</t>
+  </si>
+  <si>
+    <t>HACHINSKI</t>
+  </si>
+  <si>
+    <t>INFORMED CONSENT</t>
+  </si>
+  <si>
+    <t>GEOGRAPHIC</t>
+  </si>
+  <si>
+    <t>CAREGIVER</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Persons who have previously completed or withdrawn from this study or any other study investigating xanomeline TTS or the oral formulation of xanomeline.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Use of any investigational agent or approved Alzheimer's therapeutic medication within 30 days prior to enrollment into the study.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Serious illness which required hospitalization within 3 months of screening.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Diagnosis of serious neurological conditions, including 
+&lt;ol type="a"&gt;
+&lt;li&gt;a) Stroke or vascular dementia documented by clinical history and/or radiographic findings interpretable by the investigator as indicative of these disorders&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Seizure disorder other than simple childhood febrile seizures&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Severe head trauma resulting in protracted loss of consciousness within the last 5 years, or multiple episodes of head trauma&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Parkinson's disease&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Multiple sclerosis&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Amyotrophic lateral sclerosis&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Myasthenia gravis.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Episode of depression meeting DSM-IV criteria within 3 months of screening.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A history within the last 5 years of the following:&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;a)  Schizophrenia&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;b)  Bipolar Disease&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;c)  Ethanol or psychoactive drug abuse or dependence. &lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A history of syncope within the last 5 years.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Evidence from ECG recording at screening of any of the following conditions :&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;a)  Left bundle branch block&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;b)  Bradycardia ≤50 beats per minute&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;c)  Sinus pauses &amp;gt;2 seconds&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;d)  Second or third degree heart block unless treated with a pacemaker&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;e)  Wolff-Parkinson-White syndrome&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;f) Sustained supraventricular tachyarrhythmia including SVT≥10 sec, atrial fibrillation, atrial flutter.&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;g) Ventricular tachycardia at a rate of ≥120 beats per minute lasting&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;≥10 seconds.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>16b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;p&gt;A history within the last 5 years of a serious cardiovascular disorder, including&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;a)  Clinically significant arrhythmia&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;b)  Symptomatic sick sinus syndrome not treated with a pacemaker&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;c)  Congestive heart failure refractory to treatment&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;d)  Angina except angina controlled with PRN nitroglycerin&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;e)  Resting heart rate &amp;lt;50 or &amp;gt;100 beats per minute, on physical exam&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;f)  Uncontrolled hypertension.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A history within the last 5 years of a serious gastrointestinal disorder, including 
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;Chronic peptic/duodenal/gastric/esophageal ulcer that are untreated or refractory to treatment&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Symptomatic diverticular disease&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Inflammatory bowel disease&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Pancreatitis&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Hepatitis&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Cirrhosis of the liver.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A history within the last 5 years of a serious endocrine disorder, including&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;Uncontrolled Insulin Dependent Diabetes Mellitus (IDDM)&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Diabetic ketoacidosis&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Untreated hyperthyroidism&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Untreated hypothyroidism&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Other untreated endocrinological disorder&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; A history within the last 5 years of a serious respiratory disorder, including&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;Asthma with bronchospasm refractory to treatment&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Decompensated chronic obstructive pulmonary disease.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A history within the last 5 years of a serious genitourinary disorder, including&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;Renal failure&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Uncontrolled urinary retention.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A history within the last 5 years of a serious rheumatologic disorder, including&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;Lupus&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Temporal arteritis&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Severe rheumatoid arthritis.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A history within the last 5 years of a serious infectious disease including&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;a)  Neurosyphilis&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;b)  Meningitis&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;c)  Encephalitis.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A known history of human immunodeficiency virus (HIV) within the last 5 years.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;A history within the last 5 years of a primary or recurrent malignant disease with the exception of resected cutaneous squamous cell carcinoma in situ, basal cell carcinoma, cervical carcinoma in situ, or in situ prostate cancer with a normal PSA postresection.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Visual, hearing, or communication disabilities impairing the ability to participate in the study; (for example, inability to speak or understand English, illiteracy).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>27b</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;[Laboratory test values exceeding the Lilly Reference Range III for the patient's age in any of the following analytes: ↑ creatinine, ↑ total bilirubin, ↑ SGOT, ↑ SGPT, ↑ alkaline phosphatase, ↑ GGT, ↑↓ hemoglobin, ↑↓ white blood cell count, ↑↓ platelet count, ↑↓ serum sodium, potassium, or calcium.&lt;/p&gt;
+&lt;p&gt;If values exceed these laboratory reference ranges, clinical significance will be judged by the monitoring physicians. If the monitoring physician determines that the deviation from the reference range is not clinically significant, the patient may be included in the study. This decision will be documented.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Central laboratory test values below reference range for folate, and Vitamin B 12 , and outside reference range for thyroid function tests.&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;Folate reference range 2.0 to 25.0 ng/mL. Patients will be allowed to enroll if their folate levels are above the upper end of the range if patients are taking vitamin supplements.&lt;/p&gt;
+&lt;li&gt;&lt;p&gt;Vitamin B 12 reference range 130 to 900 pg/mL. Patients will be 
+allowed to enroll if their B 12 levels are above the upper reference 
+range if patients are taking oral vitamin supplements.&lt;/p&gt;
+&lt;li&gt;&lt;p&gt;Thyroid functions&lt;/p&gt;
+&lt;ol type="i"&gt;
+&lt;li&gt;&lt;p&gt;Thyroid Uptake reference range 25 to 38%. Patients will be allowed to enroll with results of 23 to 51% provided the remainder of the thyroid profile is normal and there are no clinical signs or symptoms of thyroid abnormality.&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;TSH reference range 0.32 to 5.0. Patients will be allowed to enroll with results of 0.03 to 6.2 if patients are taking stable doses of exogenous thyroid supplements, with normal free thyroid index, and show no clinical signs or symptoms of thyroid abnormality.&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Total T4 reference range 4.5 to 12.5. Patients will be allowed to enroll with results of 4.1 to 13.4 if patients are taking stable doses of exogenous thyroid hormone, with normal free thyroid index, and show no clinical signs or symptoms of thyroid 
+abnormality.&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Free Thyroid Index reference range 1.1 to 4.6.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>28b</t>
+  </si>
+  <si>
+    <t>29b</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Positive syphilis screening.&lt;/p&gt;
+&lt;p&gt;Positive syphilis screening. As determined by positive RPR followed up by confirmatory FTA-Abs. Confirmed patients are excluded unless there is a documented medical history of an alternative disease (for example, yaws) which caused the lab abnormality.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Glycosylated hemoglobin (A1C). Required only on patients with known diabetes mellitus or random blood sugar &amp;gt;200 on screening labs. Patients will be excluded if levels are &amp;gt;9.5%&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>30b</t>
+  </si>
+  <si>
+    <t>31b</t>
   </si>
 </sst>
 </file>
@@ -2756,13 +3129,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3081,7 +3454,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3150,7 +3523,7 @@
         <v>65</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>734</v>
+        <v>722</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="35"/>
@@ -3265,7 +3638,7 @@
         <v>502</v>
       </c>
       <c r="B17" t="s">
-        <v>731</v>
+        <v>719</v>
       </c>
       <c r="C17" t="s">
         <v>503</v>
@@ -3288,7 +3661,7 @@
         <v>506</v>
       </c>
       <c r="B18" t="s">
-        <v>732</v>
+        <v>720</v>
       </c>
       <c r="C18" t="s">
         <v>507</v>
@@ -3334,13 +3707,13 @@
         <v>82</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>224</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="17" x14ac:dyDescent="0.2">
@@ -3348,7 +3721,7 @@
         <v>84</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>37</v>
@@ -3362,13 +3735,13 @@
         <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>499</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -3388,7 +3761,7 @@
         <v>553</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -4071,13 +4444,13 @@
         <v>82</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>224</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4085,7 +4458,7 @@
         <v>84</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>37</v>
@@ -4099,13 +4472,13 @@
         <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>499</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4125,7 +4498,7 @@
         <v>553</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4173,7 +4546,7 @@
     <row r="11" spans="1:4" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="3" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>200</v>
@@ -4218,7 +4591,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -4237,7 +4610,7 @@
     <row r="17" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
@@ -4247,7 +4620,7 @@
     <row r="18" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
@@ -4309,10 +4682,10 @@
     <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>683</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>686</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>1</v>
@@ -4498,28 +4871,28 @@
         <v>82</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>728</v>
+        <v>716</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>224</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>753</v>
+        <v>741</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>754</v>
+        <v>742</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>755</v>
+        <v>743</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>756</v>
+        <v>744</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>757</v>
+        <v>745</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>758</v>
+        <v>746</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4527,7 +4900,7 @@
         <v>84</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>729</v>
+        <v>717</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>37</v>
@@ -4539,28 +4912,28 @@
         <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>730</v>
+        <v>718</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>499</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>714</v>
+        <v>702</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>759</v>
+        <v>747</v>
       </c>
       <c r="F3" s="44" t="s">
-        <v>760</v>
+        <v>748</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>761</v>
+        <v>749</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>762</v>
+        <v>750</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>763</v>
+        <v>751</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4595,22 +4968,22 @@
         <v>553</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>754</v>
+        <v>742</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>755</v>
+        <v>743</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>756</v>
+        <v>744</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>757</v>
+        <v>745</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>758</v>
+        <v>746</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4648,10 +5021,10 @@
     <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="3" t="s">
-        <v>764</v>
+        <v>752</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>724</v>
+        <v>712</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -4660,10 +5033,10 @@
     <row r="11" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="3" t="s">
-        <v>765</v>
+        <v>753</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>766</v>
+        <v>754</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
@@ -4672,10 +5045,10 @@
     <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>767</v>
+        <v>755</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>725</v>
+        <v>713</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>1</v>
@@ -4687,10 +5060,10 @@
     <row r="13" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
-        <v>768</v>
+        <v>756</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>766</v>
+        <v>754</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>1</v>
@@ -4894,7 +5267,7 @@
         <v>541</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>537</v>
@@ -4960,7 +5333,7 @@
         <v>548</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>139</v>
@@ -4975,7 +5348,7 @@
         <v>541</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>537</v>
@@ -4989,7 +5362,7 @@
         <v>550</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>140</v>
@@ -5004,7 +5377,7 @@
         <v>541</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>537</v>
@@ -5018,7 +5391,7 @@
         <v>570</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>148</v>
@@ -5033,7 +5406,7 @@
         <v>541</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>537</v>
@@ -5047,7 +5420,7 @@
         <v>571</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>204</v>
@@ -5062,7 +5435,7 @@
         <v>541</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>537</v>
@@ -5076,22 +5449,22 @@
         <v>572</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>549</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>562</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>537</v>
@@ -5102,7 +5475,7 @@
         <v>573</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>149</v>
@@ -5117,13 +5490,13 @@
         <v>541</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>537</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5131,22 +5504,22 @@
         <v>574</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>549</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>563</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>537</v>
@@ -5157,7 +5530,7 @@
         <v>575</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>150</v>
@@ -5172,13 +5545,13 @@
         <v>541</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>537</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -5186,22 +5559,22 @@
         <v>576</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>549</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>564</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>537</v>
@@ -5212,7 +5585,7 @@
         <v>577</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>151</v>
@@ -5227,13 +5600,13 @@
         <v>541</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>537</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -5241,22 +5614,22 @@
         <v>578</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>549</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>565</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>537</v>
@@ -5268,7 +5641,7 @@
         <v>579</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>152</v>
@@ -5283,13 +5656,13 @@
         <v>541</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>537</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -5297,7 +5670,7 @@
         <v>580</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>153</v>
@@ -5306,13 +5679,13 @@
         <v>549</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>541</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>537</v>
@@ -5326,19 +5699,19 @@
         <v>581</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>546</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>547</v>
@@ -5350,19 +5723,19 @@
         <v>582</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>546</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>547</v>
@@ -5370,50 +5743,50 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>717</v>
+        <v>705</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>777</v>
+        <v>765</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>777</v>
+        <v>765</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>546</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>753</v>
+        <v>741</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>753</v>
+        <v>741</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>716</v>
+        <v>704</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>718</v>
+        <v>706</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>778</v>
+        <v>766</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>778</v>
+        <v>766</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>549</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>754</v>
+        <v>742</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>753</v>
+        <v>741</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>715</v>
+        <v>703</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>537</v>
@@ -5422,52 +5795,52 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>719</v>
+        <v>707</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>779</v>
+        <v>767</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>779</v>
+        <v>767</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>549</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>755</v>
+        <v>743</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>754</v>
+        <v>742</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>780</v>
+        <v>768</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>721</v>
+        <v>709</v>
       </c>
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>720</v>
+        <v>708</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>781</v>
+        <v>769</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>781</v>
+        <v>769</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>549</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>756</v>
+        <v>744</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>755</v>
+        <v>743</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>782</v>
+        <v>770</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>537</v>
@@ -5476,52 +5849,52 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>783</v>
+        <v>771</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>779</v>
+        <v>767</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>779</v>
+        <v>767</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>549</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>757</v>
+        <v>745</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>756</v>
+        <v>744</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>780</v>
+        <v>768</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>721</v>
+        <v>709</v>
       </c>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>784</v>
+        <v>772</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>781</v>
+        <v>769</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>781</v>
+        <v>769</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>549</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>758</v>
+        <v>746</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>757</v>
+        <v>745</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>785</v>
+        <v>773</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>537</v>
@@ -5565,24 +5938,24 @@
         <v>226</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>805</v>
+        <v>793</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>806</v>
+        <v>794</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>807</v>
+        <v>795</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>808</v>
+        <v>796</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>809</v>
+        <v>797</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -5647,18 +6020,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="C7" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -5693,10 +6066,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C14" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -5746,7 +6119,7 @@
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5756,10 +6129,10 @@
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -5794,39 +6167,39 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>777</v>
+        <v>765</v>
       </c>
       <c r="C34" t="s">
-        <v>786</v>
+        <v>774</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>765</v>
+        <v>753</v>
       </c>
       <c r="C35" t="s">
-        <v>787</v>
+        <v>775</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>788</v>
+        <v>776</v>
       </c>
       <c r="C36" t="s">
-        <v>770</v>
+        <v>758</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>768</v>
+        <v>756</v>
       </c>
       <c r="C37" t="s">
-        <v>789</v>
+        <v>777</v>
       </c>
     </row>
   </sheetData>
@@ -5879,49 +6252,49 @@
         <v>38</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>739</v>
+        <v>727</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>36</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>728</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>729</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>730</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>731</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>732</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>735</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>737</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>738</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>739</v>
+      </c>
+      <c r="S1" s="16" t="s">
         <v>740</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>741</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>742</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>743</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>744</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>745</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>746</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>747</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>748</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>749</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>750</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>751</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>752</v>
       </c>
     </row>
   </sheetData>
@@ -6014,7 +6387,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>735</v>
+        <v>723</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>224</v>
@@ -6026,30 +6399,30 @@
         <v>499</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>736</v>
+        <v>724</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>737</v>
+        <v>725</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>773</v>
+        <v>761</v>
       </c>
       <c r="H1" s="17" t="s">
         <v>40</v>
       </c>
       <c r="I1" s="45" t="s">
-        <v>775</v>
+        <v>763</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>738</v>
+        <v>726</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>813</v>
+        <v>801</v>
       </c>
       <c r="E2" s="3">
         <v>300</v>
@@ -6058,13 +6431,13 @@
         <v>300</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>776</v>
+        <v>764</v>
       </c>
     </row>
   </sheetData>
@@ -6077,8 +6450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6098,34 +6471,34 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>43</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>44</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>45</v>
@@ -6138,11 +6511,11 @@
         <v>59</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>47</v>
@@ -6184,10 +6557,10 @@
         <v>60</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>47</v>
@@ -6246,11 +6619,11 @@
         <v>174</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>48</v>
@@ -6301,15 +6674,26 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>809</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>806</v>
+      </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>810</v>
+      </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="13" t="s">
+        <v>807</v>
+      </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -6320,10 +6704,15 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>811</v>
+      </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="13" t="s">
+        <v>808</v>
+      </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -6540,7 +6929,7 @@
         <v>522</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>733</v>
+        <v>721</v>
       </c>
     </row>
   </sheetData>
@@ -6652,25 +7041,25 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>722</v>
+        <v>710</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>769</v>
+        <v>757</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>771</v>
+        <v>759</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>723</v>
+        <v>711</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>770</v>
+        <v>758</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="26" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
     </row>
   </sheetData>
@@ -6713,10 +7102,10 @@
         <v>36</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>93</v>
@@ -6751,7 +7140,7 @@
         <v>99</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -6892,7 +7281,7 @@
         <v>136</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>571</v>
@@ -6915,7 +7304,7 @@
         <v>136</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>573</v>
@@ -6938,7 +7327,7 @@
         <v>136</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>575</v>
@@ -6961,7 +7350,7 @@
         <v>136</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>577</v>
@@ -7110,7 +7499,7 @@
         <v>182</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>178</v>
@@ -7124,7 +7513,7 @@
         <v>185</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>184</v>
@@ -7138,7 +7527,7 @@
         <v>182</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>186</v>
@@ -7152,7 +7541,7 @@
         <v>118</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="D8" s="41" t="s">
         <v>188</v>
@@ -7196,64 +7585,64 @@
         <v>499</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>57</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C2" t="s">
+        <v>592</v>
+      </c>
+      <c r="D2" t="s">
+        <v>593</v>
+      </c>
+      <c r="E2" t="s">
         <v>594</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>595</v>
       </c>
-      <c r="D2" t="s">
-        <v>596</v>
-      </c>
-      <c r="E2" t="s">
-        <v>597</v>
-      </c>
-      <c r="F2" t="s">
-        <v>598</v>
-      </c>
       <c r="G2" t="s">
-        <v>811</v>
+        <v>799</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="E3" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F3" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="G3" t="s">
-        <v>810</v>
+        <v>798</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="E4" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F4" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="G4" t="s">
         <v>37</v>
@@ -7261,22 +7650,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>687</v>
+      </c>
+      <c r="B5" t="s">
+        <v>688</v>
+      </c>
+      <c r="C5" t="s">
+        <v>689</v>
+      </c>
+      <c r="D5" t="s">
         <v>690</v>
-      </c>
-      <c r="B5" t="s">
-        <v>691</v>
-      </c>
-      <c r="C5" t="s">
-        <v>692</v>
-      </c>
-      <c r="D5" t="s">
-        <v>693</v>
       </c>
       <c r="E5" t="s">
         <v>568</v>
       </c>
       <c r="F5" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="G5" t="s">
         <v>499</v>
@@ -7291,7 +7680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -7326,7 +7715,7 @@
         <v>497</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>814</v>
+        <v>802</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7402,7 +7791,7 @@
         <v>494</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>815</v>
+        <v>803</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7439,7 +7828,7 @@
         <v>250</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>704</v>
+        <v>695</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -7451,7 +7840,7 @@
         <v>252</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>705</v>
+        <v>696</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -7508,7 +7897,7 @@
         <v>264</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>706</v>
+        <v>697</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -7529,7 +7918,7 @@
         <v>268</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>816</v>
+        <v>804</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7541,7 +7930,7 @@
         <v>270</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>817</v>
+        <v>805</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7571,7 +7960,7 @@
         <v>276</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>707</v>
+        <v>698</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -8658,7 +9047,7 @@
         <v>198</v>
       </c>
       <c r="F2" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -8707,144 +9096,144 @@
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="47" t="s">
-        <v>812</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
+      <c r="B3" s="48" t="s">
+        <v>800</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
     </row>
     <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="48" t="s">
-        <v>682</v>
-      </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+      <c r="B7" s="46" t="s">
+        <v>679</v>
+      </c>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>801</v>
-      </c>
-      <c r="B9" s="46" t="s">
-        <v>802</v>
-      </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+        <v>789</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>790</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>803</v>
-      </c>
-      <c r="B10" s="46" t="s">
-        <v>804</v>
-      </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
+        <v>791</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>792</v>
+      </c>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="48" t="s">
-        <v>713</v>
-      </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
+      <c r="B12" s="46" t="s">
+        <v>701</v>
+      </c>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -8876,7 +9265,7 @@
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>113</v>
@@ -8936,6 +9325,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:F4"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -8943,11 +9337,6 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8986,30 +9375,30 @@
         <v>36</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>790</v>
+        <v>778</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>583</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>791</v>
+        <v>779</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>792</v>
+        <v>780</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>793</v>
+        <v>781</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>794</v>
+        <v>782</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>795</v>
+        <v>783</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>796</v>
+        <v>784</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>79</v>
@@ -9021,16 +9410,16 @@
         <v>123456789</v>
       </c>
       <c r="F2" t="s">
-        <v>797</v>
+        <v>785</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>798</v>
+        <v>786</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>799</v>
+        <v>787</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>800</v>
+        <v>788</v>
       </c>
     </row>
   </sheetData>
@@ -9040,10 +9429,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1EE44-0F6C-474B-8770-DA2A14736511}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9053,7 +9442,7 @@
     <col min="3" max="3" width="16" style="11" customWidth="1"/>
     <col min="4" max="4" width="33.83203125" style="11" customWidth="1"/>
     <col min="5" max="5" width="6.5" style="11" customWidth="1"/>
-    <col min="6" max="6" width="79" style="13" customWidth="1"/>
+    <col min="6" max="6" width="104.5" style="13" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
@@ -9088,36 +9477,24 @@
         <v>586</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>587</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>588</v>
+        <v>825</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>589</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>585</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>697</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>698</v>
+        <v>826</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>699</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>590</v>
+        <v>813</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -9125,39 +9502,644 @@
         <v>585</v>
       </c>
       <c r="B4" s="34" t="s">
+        <v>694</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>820</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>828</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>821</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>827</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>822</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>829</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>823</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>830</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>824</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>831</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>700</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>701</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>702</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>703</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>708</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>709</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>711</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>712</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>710</v>
+      <c r="F10" s="13" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>436</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>448</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>456</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>466</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>482</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>484</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="187" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>846</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="170" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>836</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>837</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>838</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>839</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>840</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>841</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>855</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>856</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>857</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>858</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>899</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="372" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>902</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>903</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>906</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>907</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B53" s="34" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B54" s="34" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B57" s="34" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B60" s="34" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B67" s="34" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B69" s="34" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="B70" s="34" t="s">
+        <v>896</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9193,10 +10175,10 @@
         <v>36</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -9316,7 +10298,7 @@
         <v>213</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>131</v>
@@ -9330,7 +10312,7 @@
         <v>213</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>131</v>
@@ -9344,7 +10326,7 @@
         <v>213</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>131</v>
@@ -9429,31 +10411,31 @@
         <v>562</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>563</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>564</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>565</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>566</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -9526,10 +10508,10 @@
         <v>499</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>567</v>
@@ -9547,25 +10529,25 @@
         <v>204</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>149</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>150</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>151</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>152</v>
@@ -9654,31 +10636,31 @@
         <v>562</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>563</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>564</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>565</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>566</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>569</v>
@@ -10035,7 +11017,7 @@
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1" t="s">
@@ -10090,7 +11072,7 @@
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="3" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1" t="s">
@@ -10475,10 +11457,10 @@
     <row r="22" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="3" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>727</v>
+        <v>715</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>1</v>
@@ -10755,7 +11737,7 @@
         <v>164</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>726</v>
+        <v>714</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>1</v>
@@ -10922,7 +11904,7 @@
         <v>13</v>
       </c>
       <c r="C30" s="42" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>1</v>
@@ -11031,7 +12013,7 @@
     <row r="32" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="5" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="25" t="s">
@@ -11143,7 +12125,7 @@
     <row r="34" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="5" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="1" t="s">
@@ -11916,26 +12898,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -12136,32 +13098,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12178,4 +13135,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
More fixes and improvements
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4479BB1C-6651-EC4D-9D54-0177EF3DD935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF7D300-7B95-0C4E-9B08-51D6FED5D89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="500" windowWidth="40620" windowHeight="25860" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="18600" yWindow="500" windowWidth="40620" windowHeight="25860" firstSheet="14" activeTab="24" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1916" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="866">
   <si>
     <t>Screening</t>
   </si>
@@ -4760,6 +4760,9 @@
   &lt;/li&gt;
 &lt;/ol&gt;</t>
   </si>
+  <si>
+    <t>&lt;usdm:macro id="note" text="The following SoA timelines are auto generated using the detailed study design held within the USDM."/&gt; &lt;usdm:macro id="section" name="soa"/&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -4998,8 +5001,8 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -5007,8 +5010,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7847,7 +7850,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7872,16 +7875,25 @@
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>156</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -7911,31 +7923,49 @@
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>157</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>158</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>159</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>160</v>
       </c>
+      <c r="C13" s="3" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -7949,56 +7979,89 @@
       <c r="A15" s="3" t="s">
         <v>161</v>
       </c>
+      <c r="C15" s="3" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>162</v>
       </c>
+      <c r="C16" s="3" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>163</v>
       </c>
+      <c r="C18" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>164</v>
       </c>
+      <c r="C19" s="3" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="C20" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="C21" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C22" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>165</v>
       </c>
+      <c r="C23" s="3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>378</v>
       </c>
+      <c r="C24" s="5" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>166</v>
       </c>
+      <c r="C25" s="5" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
@@ -8012,34 +8075,55 @@
       <c r="A27" s="3" t="s">
         <v>167</v>
       </c>
+      <c r="C27" s="3" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>168</v>
       </c>
+      <c r="C28" s="3" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>169</v>
       </c>
+      <c r="C29" s="3" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>170</v>
       </c>
+      <c r="C30" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>171</v>
       </c>
+      <c r="C31" s="3" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="C32" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>422</v>
+      </c>
+      <c r="C33" t="s">
         <v>422</v>
       </c>
     </row>
@@ -9582,8 +9666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9608,7 +9692,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="388" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="372" x14ac:dyDescent="0.2">
       <c r="A2" s="47">
         <v>0</v>
       </c>
@@ -9620,7 +9704,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="47">
         <v>1</v>
       </c>
@@ -9676,7 +9760,7 @@
       </c>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A8" s="48" t="s">
         <v>611</v>
       </c>
@@ -9852,7 +9936,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A23" s="48" t="s">
         <v>652</v>
       </c>
@@ -9876,7 +9960,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="306" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A25" s="48" t="s">
         <v>658</v>
       </c>
@@ -9934,7 +10018,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="255" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A30" s="48" t="s">
         <v>672</v>
       </c>
@@ -9982,7 +10066,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A34" s="48" t="s">
         <v>683</v>
       </c>
@@ -10006,7 +10090,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A36" s="48" t="s">
         <v>689</v>
       </c>
@@ -10014,11 +10098,11 @@
       <c r="C36" s="45" t="s">
         <v>690</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D36" s="49" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A37" s="48" t="s">
         <v>691</v>
       </c>
@@ -10088,7 +10172,7 @@
       </c>
       <c r="D42" s="13"/>
     </row>
-    <row r="43" spans="1:4" ht="306" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A43" s="48" t="s">
         <v>707</v>
       </c>
@@ -10100,7 +10184,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="48" t="s">
         <v>710</v>
       </c>
@@ -10112,7 +10196,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="48" t="s">
         <v>713</v>
       </c>
@@ -10124,7 +10208,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="48" t="s">
         <v>716</v>
       </c>
@@ -10136,7 +10220,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="306" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="289" x14ac:dyDescent="0.2">
       <c r="A47" s="48" t="s">
         <v>719</v>
       </c>
@@ -10148,7 +10232,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="372" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="306" x14ac:dyDescent="0.2">
       <c r="A48" s="48" t="s">
         <v>722</v>
       </c>
@@ -10170,7 +10254,7 @@
       </c>
       <c r="D49" s="13"/>
     </row>
-    <row r="50" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A50" s="48" t="s">
         <v>726</v>
       </c>
@@ -10182,7 +10266,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A51" s="48" t="s">
         <v>729</v>
       </c>
@@ -10204,7 +10288,7 @@
       </c>
       <c r="D52" s="13"/>
     </row>
-    <row r="53" spans="1:4" ht="372" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="323" x14ac:dyDescent="0.2">
       <c r="A53" s="48" t="s">
         <v>734</v>
       </c>
@@ -10216,7 +10300,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="289" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A54" s="48" t="s">
         <v>737</v>
       </c>
@@ -10240,7 +10324,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="323" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="272" x14ac:dyDescent="0.2">
       <c r="A56" s="48" t="s">
         <v>743</v>
       </c>
@@ -10252,7 +10336,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="404" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="306" x14ac:dyDescent="0.2">
       <c r="A57" s="48" t="s">
         <v>746</v>
       </c>
@@ -10264,7 +10348,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="289" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="204" x14ac:dyDescent="0.2">
       <c r="A58" s="48" t="s">
         <v>749</v>
       </c>
@@ -10276,7 +10360,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A59" s="48" t="s">
         <v>752</v>
       </c>
@@ -10288,7 +10372,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A60" s="48" t="s">
         <v>755</v>
       </c>
@@ -10300,7 +10384,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A61" s="48" t="s">
         <v>758</v>
       </c>
@@ -10312,7 +10396,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A62" s="48" t="s">
         <v>761</v>
       </c>
@@ -10346,7 +10430,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="153" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A65" s="48" t="s">
         <v>768</v>
       </c>
@@ -10358,7 +10442,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="48" t="s">
         <v>771</v>
       </c>
@@ -10382,7 +10466,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="48" t="s">
         <v>775</v>
       </c>
@@ -10391,10 +10475,10 @@
         <v>776</v>
       </c>
       <c r="D68" s="46" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="48" t="s">
         <v>778</v>
       </c>
@@ -10406,7 +10490,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="48" t="s">
         <v>780</v>
       </c>
@@ -10418,7 +10502,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="48" t="s">
         <v>782</v>
       </c>
@@ -10430,7 +10514,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="48" t="s">
         <v>784</v>
       </c>
@@ -10442,7 +10526,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="48" t="s">
         <v>786</v>
       </c>
@@ -10454,7 +10538,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="48" t="s">
         <v>788</v>
       </c>
@@ -10466,7 +10550,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="48" t="s">
         <v>790</v>
       </c>
@@ -10478,7 +10562,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="48" t="s">
         <v>792</v>
       </c>
@@ -10490,7 +10574,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="48" t="s">
         <v>794</v>
       </c>
@@ -10697,13 +10781,13 @@
       <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
@@ -10733,7 +10817,7 @@
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="52" t="s">
         <v>421</v>
       </c>
       <c r="C7" s="50"/>
@@ -10793,12 +10877,12 @@
       <c r="A12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="52" t="s">
         <v>439</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -10890,11 +10974,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:F4"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -10902,6 +10981,11 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10996,7 +11080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1EE44-0F6C-474B-8770-DA2A14736511}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D30" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="D30" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -11544,7 +11628,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>437</v>
       </c>
@@ -14321,6 +14405,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -14521,27 +14625,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14558,29 +14667,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix for error messages and non-water marked PDF
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF7D300-7B95-0C4E-9B08-51D6FED5D89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA5CBC1-6898-5B4E-8366-CD8F27DCF144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="500" windowWidth="40620" windowHeight="25860" firstSheet="14" activeTab="24" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="18600" yWindow="500" windowWidth="40620" windowHeight="25860" firstSheet="14" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="867">
   <si>
     <t>Screening</t>
   </si>
@@ -4763,6 +4763,9 @@
   <si>
     <t>&lt;usdm:macro id="note" text="The following SoA timelines are auto generated using the detailed study design held within the USDM."/&gt; &lt;usdm:macro id="section" name="soa"/&gt;</t>
   </si>
+  <si>
+    <t>Inclusion and exclusion criteria</t>
+  </si>
 </sst>
 </file>
 
@@ -5005,13 +5008,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7849,8 +7852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4305555-B5C2-8349-A6D3-AA57DAC0BCD5}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7884,7 +7887,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>866</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -9666,7 +9669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
@@ -10454,7 +10457,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A67" s="47">
         <v>6</v>
       </c>
@@ -10745,144 +10748,144 @@
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>538</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="50" t="s">
         <v>421</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="51" t="s">
         <v>528</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>529</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="51" t="s">
         <v>530</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="50" t="s">
         <v>439</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -10974,6 +10977,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:F4"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -10981,11 +10989,6 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14405,26 +14408,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -14625,32 +14608,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14667,4 +14645,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add in IE dict references and fix bugs
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA5CBC1-6898-5B4E-8366-CD8F27DCF144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3F1A09-4119-7242-B8B3-2439F53A63CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="500" windowWidth="40620" windowHeight="25860" firstSheet="14" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="18600" yWindow="500" windowWidth="73180" windowHeight="25860" firstSheet="1" activeTab="23" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="867">
   <si>
     <t>Screening</t>
   </si>
@@ -1700,15 +1700,6 @@
   </si>
   <si>
     <t>OBJ6</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Males and postmenopausal females at least 50 years of age.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Diagnosis of probable AD as defined by National Institute of Neurological and Communicative Disorders and Stroke (NINCDS) and the Alzheimer's Disease and Related Disorders Association (ADRDA) guidelines (Attachment LZZT.7).&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;MMSE score of 10 to 23.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Hachinski Ischemic Scale score of ≤4 (Attachment LZZT.8).&lt;/p&gt;</t>
@@ -4766,6 +4757,15 @@
   <si>
     <t>Inclusion and exclusion criteria</t>
   </si>
+  <si>
+    <t>&lt;p&gt;Males and postmenopausal females at least &lt;usdm:tag name="min_age"/&gt; years of age.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;usdm:tag name="Activity1"/&gt; score of 10 to 23.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;usdm:tag name="StudyPopulation"/&gt; as defined by National Institute of Neurological and Communicative Disorders and Stroke (NINCDS) and the Alzheimer's Disease and Related Disorders Association (ADRDA) guidelines (Attachment LZZT.7).&lt;/p&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -7852,7 +7852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4305555-B5C2-8349-A6D3-AA57DAC0BCD5}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -7887,7 +7887,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -8645,10 +8645,10 @@
         <v>48</v>
       </c>
       <c r="F10" s="11" t="s">
+        <v>844</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>847</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>850</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>49</v>
@@ -8670,12 +8670,12 @@
         <v>48</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="11" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>49</v>
@@ -8697,12 +8697,12 @@
         <v>48</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="11" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>49</v>
@@ -9549,8 +9549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989384DC-1C54-514A-8A1E-ADD84D891BA4}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9605,8 +9605,8 @@
       <c r="F2" t="s">
         <v>337</v>
       </c>
-      <c r="G2" t="s">
-        <v>537</v>
+      <c r="G2" s="8" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -9619,8 +9619,8 @@
       <c r="F3" t="s">
         <v>337</v>
       </c>
-      <c r="G3" t="s">
-        <v>536</v>
+      <c r="G3" s="8" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -9701,10 +9701,10 @@
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="45" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
@@ -9713,10 +9713,10 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="45" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="D3" s="46" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -9725,20 +9725,20 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="45" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="48" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="45" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="119" x14ac:dyDescent="0.2">
@@ -9747,10 +9747,10 @@
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="45" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -9759,492 +9759,492 @@
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="45" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A8" s="48" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="45" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="204" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="45" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="45" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="48" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="45" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="48" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="45" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="48" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="45" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="48" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="45" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="48" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="45" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="48" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="45" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="48" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="45" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="D17" s="46" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A18" s="48" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="45" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D18" s="46" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="48" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="45" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="48" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="45" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D20" s="46" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="48" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="45" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:4" ht="255" x14ac:dyDescent="0.2">
       <c r="A22" s="48" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="45" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A23" s="48" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="45" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A24" s="48" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="45" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A25" s="48" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="45" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D25" s="46" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="48" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="45" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="48" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="45" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D27" s="46" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A28" s="48" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="45" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D28" s="46" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" s="48" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="45" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A30" s="48" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="45" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D30" s="46" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="48" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="45" t="s">
         <v>345</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="48" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="45" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="D32" s="46" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A33" s="48" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="45" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="D33" s="46" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A34" s="48" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="45" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="D34" s="46" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="255" x14ac:dyDescent="0.2">
       <c r="A35" s="48" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="45" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D35" s="46" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A36" s="48" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="45" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A37" s="48" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="45" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="D37" s="46" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A38" s="48" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="45" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="D38" s="46" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A39" s="48" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="45" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="D39" s="46" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A40" s="48" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="45" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D40" s="46" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="48" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="45" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D41" s="46" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="48" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="45" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A43" s="48" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="45" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="D43" s="46" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="48" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="45" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D44" s="46" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="48" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="45" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="D45" s="46" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="48" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="45" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="D46" s="46" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="289" x14ac:dyDescent="0.2">
       <c r="A47" s="48" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="45" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="D47" s="46" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="306" x14ac:dyDescent="0.2">
       <c r="A48" s="48" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="45" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D48" s="46" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -10253,162 +10253,162 @@
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="45" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="D49" s="13"/>
     </row>
     <row r="50" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A50" s="48" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="B50" s="11"/>
       <c r="C50" s="45" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="D50" s="46" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A51" s="48" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="46" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="D51" s="46" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="48" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="45" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="D52" s="13"/>
     </row>
     <row r="53" spans="1:4" ht="323" x14ac:dyDescent="0.2">
       <c r="A53" s="48" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="45" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="D53" s="46" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A54" s="48" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="45" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="D54" s="46" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A55" s="48" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="45" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="D55" s="46" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="272" x14ac:dyDescent="0.2">
       <c r="A56" s="48" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="45" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="D56" s="46" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="306" x14ac:dyDescent="0.2">
       <c r="A57" s="48" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="45" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="D57" s="46" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="204" x14ac:dyDescent="0.2">
       <c r="A58" s="48" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="45" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="D58" s="46" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A59" s="48" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="45" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="D59" s="46" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A60" s="48" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="45" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="D60" s="46" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A61" s="48" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="B61" s="11"/>
       <c r="C61" s="45" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="D61" s="46" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A62" s="48" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="B62" s="11"/>
       <c r="C62" s="45" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="D62" s="46" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -10417,44 +10417,44 @@
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="46" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A64" s="48" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="B64" s="11"/>
       <c r="C64" s="45" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="D64" s="46" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A65" s="48" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="B65" s="11"/>
       <c r="C65" s="45" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D65" s="46" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="48" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="B66" s="11"/>
       <c r="C66" s="45" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D66" s="46" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
@@ -10463,130 +10463,130 @@
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="45" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D67" s="46" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="48" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="B68" s="11"/>
       <c r="C68" s="45" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="D68" s="46" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="48" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="B69" s="11"/>
       <c r="C69" s="45" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="D69" s="46" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="B70" s="11"/>
       <c r="C70" s="45" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="D70" s="46" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="48" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="B71" s="11"/>
       <c r="C71" s="45" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D71" s="46" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="48" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="B72" s="11"/>
       <c r="C72" s="45" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="D72" s="46" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="48" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="45" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="D73" s="46" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="48" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="B74" s="11"/>
       <c r="C74" s="45" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="D74" s="46" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="48" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="B75" s="11"/>
       <c r="C75" s="45" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="D75" s="46" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="48" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="45" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D76" s="46" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="48" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="B77" s="11"/>
       <c r="C77" s="45" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="D77" s="46" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
   </sheetData>
@@ -11083,8 +11083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1EE44-0F6C-474B-8770-DA2A14736511}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="D30" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="D1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11129,16 +11129,19 @@
         <v>328</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>864</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>327</v>
       </c>
@@ -11146,13 +11149,16 @@
         <v>435</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>547</v>
+        <v>866</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -11163,13 +11169,16 @@
         <v>436</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>548</v>
+        <v>865</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -11177,16 +11186,16 @@
         <v>327</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
@@ -11194,16 +11203,16 @@
         <v>327</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -11211,16 +11220,16 @@
         <v>327</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -11228,16 +11237,16 @@
         <v>327</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -11245,16 +11254,16 @@
         <v>327</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -11265,13 +11274,13 @@
         <v>438</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -11282,13 +11291,13 @@
         <v>228</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -11299,13 +11308,13 @@
         <v>229</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="204" x14ac:dyDescent="0.2">
@@ -11316,13 +11325,13 @@
         <v>230</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -11333,13 +11342,13 @@
         <v>231</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -11350,13 +11359,13 @@
         <v>232</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -11367,13 +11376,13 @@
         <v>233</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="170" x14ac:dyDescent="0.2">
@@ -11381,16 +11390,16 @@
         <v>437</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="153" x14ac:dyDescent="0.2">
@@ -11398,16 +11407,16 @@
         <v>437</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="153" x14ac:dyDescent="0.2">
@@ -11415,16 +11424,16 @@
         <v>437</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -11432,16 +11441,16 @@
         <v>437</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -11449,16 +11458,16 @@
         <v>437</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -11466,16 +11475,16 @@
         <v>437</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -11483,16 +11492,16 @@
         <v>437</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11500,16 +11509,16 @@
         <v>437</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -11517,16 +11526,16 @@
         <v>437</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -11534,16 +11543,16 @@
         <v>437</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -11551,16 +11560,16 @@
         <v>437</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -11568,16 +11577,16 @@
         <v>437</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="372" x14ac:dyDescent="0.2">
@@ -11585,16 +11594,16 @@
         <v>437</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -11602,16 +11611,16 @@
         <v>437</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -11619,16 +11628,16 @@
         <v>437</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
@@ -11636,16 +11645,16 @@
         <v>437</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve test program, kill off yaml error file
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A76BC58-D4D4-1240-9CCA-B572274A0758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2D39A0-E989-C146-9E6E-B695DAE3E49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="500" windowWidth="73180" windowHeight="25860" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="18600" yWindow="500" windowWidth="73180" windowHeight="25860" activeTab="13" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="869">
   <si>
     <t>Screening</t>
   </si>
@@ -1664,12 +1664,6 @@
   </si>
   <si>
     <t>COND1</t>
-  </si>
-  <si>
-    <t>Condition for X</t>
-  </si>
-  <si>
-    <t>If this is true</t>
   </si>
   <si>
     <t>@plannedAge/Range/@minValue</t>
@@ -4769,6 +4763,15 @@
   <si>
     <t>National Library of Medicine, 8600 Rockville Pike,Bethesda, MD, 20894, USA</t>
   </si>
+  <si>
+    <t>Performed if patient is an insulin-dependent diabetic</t>
+  </si>
+  <si>
+    <t>Hemoglobin A&lt;sup&gt;1C&lt;/sup&gt; and insulin-dependent subjects</t>
+  </si>
+  <si>
+    <t>HA1C</t>
+  </si>
 </sst>
 </file>
 
@@ -7793,16 +7796,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8C14B1-8C62-2C45-8CB1-1E9EDDA367B1}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="51" customWidth="1"/>
     <col min="5" max="6" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7826,24 +7829,24 @@
         <v>532</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>533</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>90</v>
+      <c r="B2" s="13" t="s">
+        <v>867</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>868</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>866</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -7890,7 +7893,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -8385,7 +8388,7 @@
         <v>337</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E2" s="3">
         <v>300</v>
@@ -8639,19 +8642,19 @@
     </row>
     <row r="10" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>49</v>
@@ -8662,23 +8665,23 @@
     </row>
     <row r="11" spans="1:15" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="13" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="11" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>49</v>
@@ -8689,23 +8692,23 @@
     </row>
     <row r="12" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>48</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="11" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>49</v>
@@ -9609,7 +9612,7 @@
         <v>337</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -9623,7 +9626,7 @@
         <v>337</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -9704,10 +9707,10 @@
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="45" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
@@ -9716,10 +9719,10 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="45" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D3" s="46" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -9728,20 +9731,20 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="45" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="48" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="45" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="119" x14ac:dyDescent="0.2">
@@ -9750,10 +9753,10 @@
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="45" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -9762,492 +9765,492 @@
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="45" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A8" s="48" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="45" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="204" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="45" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="45" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D10" s="46" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="48" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="45" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D11" s="46" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="48" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="45" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="48" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="45" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="48" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="45" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="48" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="45" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D15" s="46" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="48" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="45" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="48" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="45" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D17" s="46" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A18" s="48" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="45" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D18" s="46" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="48" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="45" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="48" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="45" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D20" s="46" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="48" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="45" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:4" ht="255" x14ac:dyDescent="0.2">
       <c r="A22" s="48" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="45" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A23" s="48" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="45" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A24" s="48" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="45" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A25" s="48" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="45" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D25" s="46" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="48" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="45" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="48" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="45" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D27" s="46" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A28" s="48" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="45" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D28" s="46" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" s="48" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="45" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A30" s="48" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="45" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D30" s="46" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="48" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="45" t="s">
         <v>345</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="48" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="45" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D32" s="46" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A33" s="48" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="45" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D33" s="46" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A34" s="48" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="45" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D34" s="46" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="255" x14ac:dyDescent="0.2">
       <c r="A35" s="48" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="45" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D35" s="46" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A36" s="48" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="45" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A37" s="48" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="45" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D37" s="46" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A38" s="48" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="45" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D38" s="46" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A39" s="48" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="45" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="D39" s="46" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A40" s="48" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="45" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D40" s="46" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="48" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="45" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D41" s="46" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="48" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="45" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A43" s="48" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="45" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D43" s="46" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="48" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="45" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D44" s="46" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="48" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="45" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D45" s="46" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="48" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="45" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D46" s="46" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="289" x14ac:dyDescent="0.2">
       <c r="A47" s="48" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="45" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D47" s="46" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="306" x14ac:dyDescent="0.2">
       <c r="A48" s="48" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="45" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="D48" s="46" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -10256,162 +10259,162 @@
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="45" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D49" s="13"/>
     </row>
     <row r="50" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A50" s="48" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B50" s="11"/>
       <c r="C50" s="45" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D50" s="46" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A51" s="48" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="46" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D51" s="46" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="48" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="45" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D52" s="13"/>
     </row>
     <row r="53" spans="1:4" ht="323" x14ac:dyDescent="0.2">
       <c r="A53" s="48" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="45" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D53" s="46" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A54" s="48" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="45" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D54" s="46" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A55" s="48" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="45" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D55" s="46" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="272" x14ac:dyDescent="0.2">
       <c r="A56" s="48" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="45" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D56" s="46" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="306" x14ac:dyDescent="0.2">
       <c r="A57" s="48" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="45" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D57" s="46" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="204" x14ac:dyDescent="0.2">
       <c r="A58" s="48" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="45" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D58" s="46" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A59" s="48" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="45" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D59" s="46" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A60" s="48" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="45" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D60" s="46" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A61" s="48" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B61" s="11"/>
       <c r="C61" s="45" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D61" s="46" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A62" s="48" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B62" s="11"/>
       <c r="C62" s="45" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D62" s="46" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -10420,44 +10423,44 @@
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="46" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A64" s="48" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B64" s="11"/>
       <c r="C64" s="45" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D64" s="46" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A65" s="48" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B65" s="11"/>
       <c r="C65" s="45" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D65" s="46" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="48" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B66" s="11"/>
       <c r="C66" s="45" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D66" s="46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
@@ -10466,130 +10469,130 @@
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="45" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D67" s="46" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="48" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B68" s="11"/>
       <c r="C68" s="45" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D68" s="46" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="48" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B69" s="11"/>
       <c r="C69" s="45" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D69" s="46" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="48" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B70" s="11"/>
       <c r="C70" s="45" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D70" s="46" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="48" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="B71" s="11"/>
       <c r="C71" s="45" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D71" s="46" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="48" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B72" s="11"/>
       <c r="C72" s="45" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D72" s="46" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="48" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="45" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="D73" s="46" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="48" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B74" s="11"/>
       <c r="C74" s="45" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D74" s="46" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="48" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B75" s="11"/>
       <c r="C75" s="45" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D75" s="46" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="48" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="45" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D76" s="46" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="48" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B77" s="11"/>
       <c r="C77" s="45" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D77" s="46" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
   </sheetData>
@@ -10655,7 +10658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A054F5-5F55-D04A-9603-B97FC15141C8}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -10722,7 +10725,7 @@
         <v>269</v>
       </c>
       <c r="F3" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -10779,7 +10782,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C3" s="52"/>
       <c r="D3" s="52"/>
@@ -11135,13 +11138,13 @@
         <v>328</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>329</v>
@@ -11155,13 +11158,13 @@
         <v>435</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>329</v>
@@ -11175,13 +11178,13 @@
         <v>436</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>429</v>
@@ -11192,16 +11195,16 @@
         <v>327</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
@@ -11209,16 +11212,16 @@
         <v>327</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -11226,16 +11229,16 @@
         <v>327</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -11243,16 +11246,16 @@
         <v>327</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -11260,16 +11263,16 @@
         <v>327</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -11280,13 +11283,13 @@
         <v>438</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -11297,13 +11300,13 @@
         <v>228</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -11314,13 +11317,13 @@
         <v>229</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="204" x14ac:dyDescent="0.2">
@@ -11331,13 +11334,13 @@
         <v>230</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -11348,13 +11351,13 @@
         <v>231</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -11365,13 +11368,13 @@
         <v>232</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -11382,13 +11385,13 @@
         <v>233</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="170" x14ac:dyDescent="0.2">
@@ -11396,16 +11399,16 @@
         <v>437</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="153" x14ac:dyDescent="0.2">
@@ -11413,16 +11416,16 @@
         <v>437</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="153" x14ac:dyDescent="0.2">
@@ -11430,16 +11433,16 @@
         <v>437</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -11447,16 +11450,16 @@
         <v>437</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -11464,16 +11467,16 @@
         <v>437</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -11481,16 +11484,16 @@
         <v>437</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -11498,16 +11501,16 @@
         <v>437</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11515,16 +11518,16 @@
         <v>437</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -11532,16 +11535,16 @@
         <v>437</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -11549,16 +11552,16 @@
         <v>437</v>
       </c>
       <c r="B26" s="32" t="s">
+        <v>574</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>592</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>829</v>
+      </c>
+      <c r="F26" s="13" t="s">
         <v>576</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>594</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>831</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -11566,16 +11569,16 @@
         <v>437</v>
       </c>
       <c r="B27" s="32" t="s">
+        <v>575</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>593</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>830</v>
+      </c>
+      <c r="F27" s="13" t="s">
         <v>577</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>595</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>832</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -11583,16 +11586,16 @@
         <v>437</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="372" x14ac:dyDescent="0.2">
@@ -11600,16 +11603,16 @@
         <v>437</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -11617,16 +11620,16 @@
         <v>437</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -11634,16 +11637,16 @@
         <v>437</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
@@ -11651,16 +11654,16 @@
         <v>437</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -11881,7 +11884,7 @@
   <dimension ref="A1:V68"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:C25"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updates to to USDM changes
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2D4BAE-3EC1-B24F-B696-AB6D5FD53ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BD3412-97EA-1045-93F4-CD596DF41C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="500" windowWidth="73180" windowHeight="25860" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" firstSheet="16" activeTab="24" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -2154,19 +2154,6 @@
   </si>
   <si>
     <t>Efficacy Measures</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;The following measures will be performed in the course of the study. At Visits 3, 8, 10, and 12, ADAS-Cog, CIBIC+, and DAD will be administered. NPI-X will be administered at 2-week intervals either at clinic visits or via a telephone interview. Efficacy measures will also be collected at early termination visits, and at the retrieval visit. The neuropsychological assessment should be performed first; other protocol requirements, such as labs and the physical, should follow.&lt;/p&gt;
-&lt;ol type="a"&gt;
-&lt;li&gt;&lt;p&gt;&lt;b&gt;Alzheimer's Disease Assessment Scale - Cognitive Subscale (ADAS-Cog):&lt;/b&gt; ADAS-Cog is an established measure of cognitive function in Alzheimer's Disease. This scale has been incorporated into this study by permission of Dr. Richard C. Mohs and the American Journal of Psychiatry and was adapted from an article entitled, “The Alzheimer's Disease Assessment Scale (ADAS),” which was published in the American Journal of Psychiatry, Volume No.141, pages 1356-1364, November, 1984, Copyright 1984.&lt;/p&gt;
-&lt;p&gt;&lt;b&gt;The ADAS-Cog (11) and the ADAS-Cog (14):&lt;/b&gt; The ADAS-Cog (11) is a standard 11-item instrument used to assess word recall, naming objects, commands, constructional praxis, ideational praxis, orientation, word recognition tasks, spoken language ability, comprehension, word finding difficulty, and recall of test instructions. For the purposes of this study, three items (delayed word recall, attention/visual search task, and maze solution) have been added to the ADAS-Cog (11) to assess the patient's attention and concentration. The 14 item instrument will be referred to as the ADAS-Cog (14). At each efficacy visit, all 14 items will be assessed, and in subsequent data analyses, performance on the ADAS-Cog (14) and performance on the subset ADAS-Cog (11) will be considered.&lt;/p&gt;&lt;/li&gt;
-&lt;li&gt;&lt;p&gt;&lt;b&gt;Video-referenced Clinician's Interview-Based Impression of Change (CIBIC+):&lt;/b&gt; The CIBIC+ is an assessment of the global clinical status relative to baseline. The CIBIC+ used in this study is derived from the Clinical Global Impression of Change, an instrument in the public domain, developed by the National Institute on Aging Alzheimer's Disease Study Units Program (1 U01 AG10483; Leon Thal, Principal Investigator). The instrument employs semi-structured interviews with the patient and caregiver, to assess mental/cognitive state, behavior, and function. These domains are not individually scored, but rather are aggregated in the assignment of a global numeric score on a 1 to 7 scale (1 = marked improvement; 4 = no change; and 7 = marked worsening).&lt;/p&gt;
-&lt;p&gt;The clinician assessing CIBIC+ will have at least one year of experience with the instrument and will remain blinded to all other efficacy and safety measures.&lt;/p&gt;&lt;/li&gt;
-&lt;li&gt;&lt;p&gt;&lt;b&gt;Revised Neuropsychiatric Inventory (NPI-X):&lt;/b&gt; The NPI-X is an assessment of change in psychopathology in patients with dementia. The NPI-X is administered to the designated caregiver. This instrument has been revised from its original version (Cummings et al. 1994) and incorporated into this study with the permission of Dr. Jeffrey L. Cummings.&lt;/p&gt;&lt;/li&gt;
-&lt;li&gt;&lt;p&gt;d) &lt;b&gt;Disability Assessment for Dementia (DAD):&lt;/b&gt; The DAD is used to assess functional abilities of activities of daily living (ADL) in individuals with cognitive impairment. This scale has been revised and incorporated into this study by permission of Louise Gauthier, M.Sc., and Dr. Isabelle Gelinas. The DAD is administered to the designated caregiver.&lt;/p&gt;&lt;/li&gt;
-&lt;/ol&gt;
-&lt;p&gt;For each instrument, each assessment is to be performed by the same trained health care professional. If circumstances preclude meeting this requirement, the situation is to be documented on the Clinical Report Form (CRF), and the CRO research physician is to be notified.&lt;/p&gt;
-&lt;p&gt;In addition to the efficacy measures noted above, a survey form will be used to collect information from the caregiver on TTS acceptability (Attachment LZZT.9).&lt;/p&gt;</t>
   </si>
   <si>
     <t>3.9.1.2.</t>
@@ -4787,6 +4774,19 @@
   <si>
     <t>ADAS-Cog, CIBIC+, DAD, NPI-X</t>
   </si>
+  <si>
+    <t>&lt;p&gt;The following measures will be performed in the course of the study. At Visits 3, 8, 10, and 12, ADAS-Cog, CIBIC+, and DAD will be administered. NPI-X will be administered at 2-week intervals either at clinic visits or via a telephone interview. Efficacy measures will also be collected at early termination visits, and at the retrieval visit. The neuropsychological assessment should be performed first; other protocol requirements, such as labs and the physical, should follow.&lt;/p&gt;
+&lt;ol type="a"&gt;
+&lt;li&gt;&lt;p&gt;&lt;b&gt;Alzheimer's Disease Assessment Scale - Cognitive Subscale (ADAS-Cog):&lt;/b&gt; ADAS-Cog is an established measure of cognitive function in Alzheimer's Disease. This scale has been incorporated into this study by permission of Dr. Richard C. Mohs and the American Journal of Psychiatry and was adapted from an article entitled, “The Alzheimer's Disease Assessment Scale (ADAS),” which was published in the American Journal of Psychiatry, Volume No.141, pages 1356-1364, November, 1984, Copyright 1984.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;The ADAS-Cog (11) and the ADAS-Cog (14):&lt;/b&gt; The ADAS-Cog (11) is a standard 11-item instrument used to assess word recall, naming objects, commands, constructional praxis, ideational praxis, orientation, word recognition tasks, spoken language ability, comprehension, word finding difficulty, and recall of test instructions. For the purposes of this study, three items (delayed word recall, attention/visual search task, and maze solution) have been added to the ADAS-Cog (11) to assess the patient's attention and concentration. The 14 item instrument will be referred to as the ADAS-Cog (14). At each efficacy visit, all 14 items will be assessed, and in subsequent data analyses, performance on the ADAS-Cog (14) and performance on the subset ADAS-Cog (11) will be considered.&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;&lt;b&gt;Video-referenced Clinician's Interview-Based Impression of Change (CIBIC+):&lt;/b&gt; The CIBIC+ is an assessment of the global clinical status relative to baseline. The CIBIC+ used in this study is derived from the Clinical Global Impression of Change, an instrument in the public domain, developed by the National Institute on Aging Alzheimer's Disease Study Units Program (1 U01 AG10483; Leon Thal, Principal Investigator). The instrument employs semi-structured interviews with the patient and caregiver, to assess mental/cognitive state, behavior, and function. These domains are not individually scored, but rather are aggregated in the assignment of a global numeric score on a 1 to 7 scale (1 = marked improvement; 4 = no change; and 7 = marked worsening).&lt;/p&gt;
+&lt;p&gt;The clinician assessing CIBIC+ will have at least one year of experience with the instrument and will remain blinded to all other efficacy and safety measures.&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;&lt;b&gt;Revised Neuropsychiatric Inventory (NPI-X):&lt;/b&gt; The NPI-X is an assessment of change in psychopathology in patients with dementia. The NPI-X is administered to the designated caregiver. This instrument has been revised from its original version (Cummings et al. 1994) and incorporated into this study with the permission of Dr. Jeffrey L. Cummings.&lt;/p&gt;&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;&lt;b&gt;Disability Assessment for Dementia (DAD):&lt;/b&gt; The DAD is used to assess functional abilities of activities of daily living (ADL) in individuals with cognitive impairment. This scale has been revised and incorporated into this study by permission of Louise Gauthier, M.Sc., and Dr. Isabelle Gelinas. The DAD is administered to the designated caregiver.&lt;/p&gt;&lt;/li&gt;
+&lt;/ol&gt;
+&lt;p&gt;For each instrument, each assessment is to be performed by the same trained health care professional. If circumstances preclude meeting this requirement, the situation is to be documented on the Clinical Report Form (CRF), and the CRO research physician is to be notified.&lt;/p&gt;
+&lt;p&gt;In addition to the efficacy measures noted above, a survey form will be used to collect information from the caregiver on TTS acceptability (Attachment LZZT.9).&lt;/p&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -5029,13 +5029,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5353,7 +5353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -7850,13 +7850,13 @@
         <v>533</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>867</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>868</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>299</v>
@@ -7867,22 +7867,22 @@
     </row>
     <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>868</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>869</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>871</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>870</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>872</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -8097,7 +8097,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -8855,10 +8855,10 @@
         <v>48</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>49</v>
@@ -8880,12 +8880,12 @@
         <v>48</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="11" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>49</v>
@@ -8907,12 +8907,12 @@
         <v>48</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="11" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>49</v>
@@ -9879,8 +9879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9914,7 +9914,7 @@
         <v>599</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
@@ -9926,7 +9926,7 @@
         <v>600</v>
       </c>
       <c r="D3" s="46" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -9948,7 +9948,7 @@
         <v>603</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="119" x14ac:dyDescent="0.2">
@@ -9960,7 +9960,7 @@
         <v>604</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -10052,7 +10052,7 @@
         <v>624</v>
       </c>
       <c r="D14" s="46" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -10076,7 +10076,7 @@
         <v>629</v>
       </c>
       <c r="D16" s="46" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -10216,245 +10216,245 @@
         <v>662</v>
       </c>
       <c r="D28" s="46" t="s">
-        <v>663</v>
+        <v>873</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" s="48" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="45" t="s">
+        <v>664</v>
+      </c>
+      <c r="D29" s="46" t="s">
         <v>665</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A30" s="48" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="45" t="s">
+        <v>667</v>
+      </c>
+      <c r="D30" s="46" t="s">
         <v>668</v>
-      </c>
-      <c r="D30" s="46" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="48" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="45" t="s">
         <v>345</v>
       </c>
       <c r="D31" s="46" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="48" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="45" t="s">
+        <v>672</v>
+      </c>
+      <c r="D32" s="46" t="s">
         <v>673</v>
-      </c>
-      <c r="D32" s="46" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A33" s="48" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="45" t="s">
+        <v>675</v>
+      </c>
+      <c r="D33" s="46" t="s">
         <v>676</v>
-      </c>
-      <c r="D33" s="46" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A34" s="48" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="45" t="s">
+        <v>678</v>
+      </c>
+      <c r="D34" s="46" t="s">
         <v>679</v>
-      </c>
-      <c r="D34" s="46" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="255" x14ac:dyDescent="0.2">
       <c r="A35" s="48" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="45" t="s">
+        <v>681</v>
+      </c>
+      <c r="D35" s="46" t="s">
         <v>682</v>
-      </c>
-      <c r="D35" s="46" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A36" s="48" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="45" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A37" s="48" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="45" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D37" s="46" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A38" s="48" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="45" t="s">
+        <v>688</v>
+      </c>
+      <c r="D38" s="46" t="s">
         <v>689</v>
-      </c>
-      <c r="D38" s="46" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A39" s="48" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="45" t="s">
+        <v>691</v>
+      </c>
+      <c r="D39" s="46" t="s">
         <v>692</v>
-      </c>
-      <c r="D39" s="46" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A40" s="48" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="45" t="s">
+        <v>694</v>
+      </c>
+      <c r="D40" s="46" t="s">
         <v>695</v>
-      </c>
-      <c r="D40" s="46" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="48" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="45" t="s">
+        <v>697</v>
+      </c>
+      <c r="D41" s="46" t="s">
         <v>698</v>
-      </c>
-      <c r="D41" s="46" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="48" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="45" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A43" s="48" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="45" t="s">
+        <v>702</v>
+      </c>
+      <c r="D43" s="46" t="s">
         <v>703</v>
-      </c>
-      <c r="D43" s="46" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="48" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="45" t="s">
+        <v>705</v>
+      </c>
+      <c r="D44" s="46" t="s">
         <v>706</v>
-      </c>
-      <c r="D44" s="46" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="48" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="45" t="s">
+        <v>708</v>
+      </c>
+      <c r="D45" s="46" t="s">
         <v>709</v>
-      </c>
-      <c r="D45" s="46" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="48" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="45" t="s">
+        <v>711</v>
+      </c>
+      <c r="D46" s="46" t="s">
         <v>712</v>
-      </c>
-      <c r="D46" s="46" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="289" x14ac:dyDescent="0.2">
       <c r="A47" s="48" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="45" t="s">
+        <v>714</v>
+      </c>
+      <c r="D47" s="46" t="s">
         <v>715</v>
-      </c>
-      <c r="D47" s="46" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="306" x14ac:dyDescent="0.2">
       <c r="A48" s="48" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="45" t="s">
+        <v>717</v>
+      </c>
+      <c r="D48" s="46" t="s">
         <v>718</v>
-      </c>
-      <c r="D48" s="46" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -10463,162 +10463,162 @@
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="45" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D49" s="13"/>
     </row>
     <row r="50" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A50" s="48" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B50" s="11"/>
       <c r="C50" s="45" t="s">
+        <v>721</v>
+      </c>
+      <c r="D50" s="46" t="s">
         <v>722</v>
-      </c>
-      <c r="D50" s="46" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A51" s="48" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="46" t="s">
+        <v>724</v>
+      </c>
+      <c r="D51" s="46" t="s">
         <v>725</v>
-      </c>
-      <c r="D51" s="46" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="48" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="45" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D52" s="13"/>
     </row>
     <row r="53" spans="1:4" ht="323" x14ac:dyDescent="0.2">
       <c r="A53" s="48" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="45" t="s">
+        <v>729</v>
+      </c>
+      <c r="D53" s="46" t="s">
         <v>730</v>
-      </c>
-      <c r="D53" s="46" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A54" s="48" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="45" t="s">
+        <v>732</v>
+      </c>
+      <c r="D54" s="46" t="s">
         <v>733</v>
-      </c>
-      <c r="D54" s="46" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A55" s="48" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="45" t="s">
+        <v>735</v>
+      </c>
+      <c r="D55" s="46" t="s">
         <v>736</v>
-      </c>
-      <c r="D55" s="46" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="272" x14ac:dyDescent="0.2">
       <c r="A56" s="48" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="45" t="s">
+        <v>738</v>
+      </c>
+      <c r="D56" s="46" t="s">
         <v>739</v>
-      </c>
-      <c r="D56" s="46" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="306" x14ac:dyDescent="0.2">
       <c r="A57" s="48" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="45" t="s">
+        <v>741</v>
+      </c>
+      <c r="D57" s="46" t="s">
         <v>742</v>
-      </c>
-      <c r="D57" s="46" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="204" x14ac:dyDescent="0.2">
       <c r="A58" s="48" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="45" t="s">
+        <v>744</v>
+      </c>
+      <c r="D58" s="46" t="s">
         <v>745</v>
-      </c>
-      <c r="D58" s="46" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A59" s="48" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="45" t="s">
+        <v>747</v>
+      </c>
+      <c r="D59" s="46" t="s">
         <v>748</v>
-      </c>
-      <c r="D59" s="46" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A60" s="48" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="45" t="s">
+        <v>750</v>
+      </c>
+      <c r="D60" s="46" t="s">
         <v>751</v>
-      </c>
-      <c r="D60" s="46" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A61" s="48" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B61" s="11"/>
       <c r="C61" s="45" t="s">
+        <v>753</v>
+      </c>
+      <c r="D61" s="46" t="s">
         <v>754</v>
-      </c>
-      <c r="D61" s="46" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A62" s="48" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B62" s="11"/>
       <c r="C62" s="45" t="s">
+        <v>756</v>
+      </c>
+      <c r="D62" s="46" t="s">
         <v>757</v>
-      </c>
-      <c r="D62" s="46" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -10627,44 +10627,44 @@
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="46" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D63" s="13"/>
     </row>
     <row r="64" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A64" s="48" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B64" s="11"/>
       <c r="C64" s="45" t="s">
+        <v>760</v>
+      </c>
+      <c r="D64" s="46" t="s">
         <v>761</v>
-      </c>
-      <c r="D64" s="46" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A65" s="48" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B65" s="11"/>
       <c r="C65" s="45" t="s">
+        <v>763</v>
+      </c>
+      <c r="D65" s="46" t="s">
         <v>764</v>
-      </c>
-      <c r="D65" s="46" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="48" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B66" s="11"/>
       <c r="C66" s="45" t="s">
+        <v>766</v>
+      </c>
+      <c r="D66" s="46" t="s">
         <v>767</v>
-      </c>
-      <c r="D66" s="46" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
@@ -10673,130 +10673,130 @@
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="45" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D67" s="46" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="48" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B68" s="11"/>
       <c r="C68" s="45" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D68" s="46" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="48" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B69" s="11"/>
       <c r="C69" s="45" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D69" s="46" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="48" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B70" s="11"/>
       <c r="C70" s="45" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D70" s="46" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="48" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B71" s="11"/>
       <c r="C71" s="45" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D71" s="46" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="48" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B72" s="11"/>
       <c r="C72" s="45" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D72" s="46" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="48" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="45" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D73" s="46" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="48" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B74" s="11"/>
       <c r="C74" s="45" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D74" s="46" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="48" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B75" s="11"/>
       <c r="C75" s="45" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D75" s="46" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="48" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="45" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D76" s="46" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="48" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B77" s="11"/>
       <c r="C77" s="45" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D77" s="46" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
   </sheetData>
@@ -10929,7 +10929,7 @@
         <v>269</v>
       </c>
       <c r="F3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -10961,144 +10961,144 @@
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>536</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="52" t="s">
         <v>421</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="50" t="s">
         <v>528</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>529</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="50" t="s">
         <v>530</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="52" t="s">
         <v>439</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -11190,11 +11190,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:F4"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -11202,6 +11197,11 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11342,13 +11342,13 @@
         <v>328</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>329</v>
@@ -11362,13 +11362,13 @@
         <v>435</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>329</v>
@@ -11382,13 +11382,13 @@
         <v>436</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>429</v>
@@ -11402,10 +11402,10 @@
         <v>548</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>544</v>
@@ -11419,13 +11419,13 @@
         <v>549</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -11436,10 +11436,10 @@
         <v>550</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>545</v>
@@ -11453,10 +11453,10 @@
         <v>551</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>546</v>
@@ -11470,10 +11470,10 @@
         <v>552</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>547</v>
@@ -11487,10 +11487,10 @@
         <v>438</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>553</v>
@@ -11504,10 +11504,10 @@
         <v>228</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>554</v>
@@ -11521,10 +11521,10 @@
         <v>229</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>555</v>
@@ -11538,13 +11538,13 @@
         <v>230</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -11555,10 +11555,10 @@
         <v>231</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>562</v>
@@ -11572,13 +11572,13 @@
         <v>232</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -11589,10 +11589,10 @@
         <v>233</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>563</v>
@@ -11606,13 +11606,13 @@
         <v>564</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="153" x14ac:dyDescent="0.2">
@@ -11623,13 +11623,13 @@
         <v>556</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="153" x14ac:dyDescent="0.2">
@@ -11643,7 +11643,7 @@
         <v>585</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>565</v>
@@ -11660,7 +11660,7 @@
         <v>586</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>566</v>
@@ -11677,7 +11677,7 @@
         <v>587</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>567</v>
@@ -11694,7 +11694,7 @@
         <v>588</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>568</v>
@@ -11711,7 +11711,7 @@
         <v>589</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>569</v>
@@ -11728,7 +11728,7 @@
         <v>590</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>571</v>
@@ -11745,7 +11745,7 @@
         <v>591</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>570</v>
@@ -11762,7 +11762,7 @@
         <v>592</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>576</v>
@@ -11779,7 +11779,7 @@
         <v>593</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>577</v>
@@ -11796,10 +11796,10 @@
         <v>594</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="372" x14ac:dyDescent="0.2">
@@ -11813,10 +11813,10 @@
         <v>595</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -11830,7 +11830,7 @@
         <v>596</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>581</v>
@@ -11847,13 +11847,13 @@
         <v>597</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="F31" s="13" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>437</v>
       </c>
@@ -11864,10 +11864,10 @@
         <v>598</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
   </sheetData>
@@ -14630,6 +14630,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -14830,27 +14850,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14867,29 +14892,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Addition of DM BCs
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BD3412-97EA-1045-93F4-CD596DF41C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5597532C-E3A2-0D4E-A049-4C48A73BE06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" firstSheet="16" activeTab="24" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="9440" yWindow="500" windowWidth="48740" windowHeight="27240" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="875">
   <si>
     <t>Screening</t>
   </si>
@@ -4787,12 +4787,15 @@
 &lt;p&gt;For each instrument, each assessment is to be performed by the same trained health care professional. If circumstances preclude meeting this requirement, the situation is to be documented on the Clinical Report Form (CRF), and the CRO research physician is to be notified.&lt;/p&gt;
 &lt;p&gt;In addition to the efficacy measures noted above, a survey form will be used to collect information from the caregiver on TTS acceptability (Attachment LZZT.9).&lt;/p&gt;</t>
   </si>
+  <si>
+    <t>BC: Sex, BC: Race, BC: Date of Birth</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4854,8 +4857,15 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4874,6 +4884,11 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4884,10 +4899,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5029,16 +5045,23 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7812,7 +7835,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7869,19 +7892,19 @@
       <c r="A3" s="3" t="s">
         <v>868</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="53" t="s">
         <v>870</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="53" t="s">
         <v>869</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="54" t="s">
         <v>871</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="53" t="s">
         <v>299</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="53" t="s">
         <v>872</v>
       </c>
     </row>
@@ -9879,7 +9902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="C28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -10243,7 +10266,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="48" t="s">
         <v>669</v>
       </c>
@@ -10255,7 +10278,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="48" t="s">
         <v>671</v>
       </c>
@@ -10267,7 +10290,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A33" s="48" t="s">
         <v>674</v>
       </c>
@@ -10291,7 +10314,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="255" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="238" x14ac:dyDescent="0.2">
       <c r="A35" s="48" t="s">
         <v>680</v>
       </c>
@@ -10303,7 +10326,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A36" s="48" t="s">
         <v>683</v>
       </c>
@@ -10315,7 +10338,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A37" s="48" t="s">
         <v>685</v>
       </c>
@@ -10327,7 +10350,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="48" t="s">
         <v>687</v>
       </c>
@@ -10339,7 +10362,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="204" x14ac:dyDescent="0.2">
       <c r="A39" s="48" t="s">
         <v>690</v>
       </c>
@@ -10667,7 +10690,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A67" s="47">
         <v>6</v>
       </c>
@@ -10961,144 +10984,144 @@
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>536</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="50" t="s">
         <v>421</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="51" t="s">
         <v>528</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>529</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="51" t="s">
         <v>530</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="50" t="s">
         <v>439</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -11190,6 +11213,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:F4"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -11197,11 +11225,6 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12087,8 +12110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12691,12 +12714,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="54" t="s">
+        <v>874</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
@@ -14630,26 +14655,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -14850,32 +14855,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14892,4 +14892,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add main timeline colour
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290F3814-0830-E143-BAC6-3165E6983F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BC9A68-A313-E146-B07F-FD3860E5D663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38620" yWindow="500" windowWidth="56420" windowHeight="27240" firstSheet="4" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="38620" yWindow="500" windowWidth="56420" windowHeight="27240" firstSheet="4" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -4801,7 +4801,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4870,8 +4870,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4895,6 +4902,11 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4905,11 +4917,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5069,9 +5082,22 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -11346,7 +11372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1EE44-0F6C-474B-8770-DA2A14736511}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -12140,8 +12166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12195,25 +12221,25 @@
       <c r="J1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="59" t="s">
         <v>360</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="59" t="s">
         <v>361</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="59" t="s">
         <v>362</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="59" t="s">
         <v>366</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -12254,25 +12280,25 @@
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="60" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="60" t="s">
         <v>17</v>
       </c>
       <c r="R2" s="2" t="s">
@@ -12313,25 +12339,25 @@
       <c r="J3" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="60" t="s">
         <v>363</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="60" t="s">
         <v>364</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="60" t="s">
         <v>365</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="60" t="s">
         <v>367</v>
       </c>
       <c r="R3" s="2" t="s">
@@ -12368,25 +12394,25 @@
       <c r="J4" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="60" t="s">
         <v>310</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="60" t="s">
         <v>310</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="60" t="s">
         <v>310</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="60" t="s">
         <v>310</v>
       </c>
       <c r="R4" s="2" t="s">
@@ -12423,25 +12449,25 @@
       <c r="J5" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="59" t="s">
         <v>305</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="59" t="s">
         <v>306</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="59" t="s">
         <v>307</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="59" t="s">
         <v>308</v>
       </c>
       <c r="R5" s="9" t="s">
@@ -12457,6 +12483,10 @@
       <c r="C6" s="14" t="s">
         <v>296</v>
       </c>
+      <c r="K6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="Q6" s="59"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
@@ -12485,25 +12515,25 @@
       <c r="J7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="59" t="s">
         <v>154</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="59" t="s">
         <v>154</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="59" t="s">
         <v>154</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="59" t="s">
         <v>154</v>
       </c>
       <c r="R7" s="1" t="s">
@@ -12540,25 +12570,25 @@
       <c r="J8" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="59" t="s">
         <v>106</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="59" t="s">
         <v>107</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="59" t="s">
         <v>108</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="59" t="s">
         <v>110</v>
       </c>
       <c r="R8" s="1" t="s">
@@ -12578,6 +12608,10 @@
       <c r="C9" s="16" t="s">
         <v>92</v>
       </c>
+      <c r="K9" s="59"/>
+      <c r="M9" s="59"/>
+      <c r="O9" s="59"/>
+      <c r="Q9" s="59"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -12606,25 +12640,25 @@
       <c r="J10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="60" t="s">
         <v>17</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="Q10" s="60" t="s">
         <v>17</v>
       </c>
       <c r="R10" s="2" t="s">
@@ -12661,25 +12695,25 @@
       <c r="J11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="25" t="s">
+      <c r="K11" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="25" t="s">
+      <c r="M11" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="25" t="s">
+      <c r="O11" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="Q11" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R11" s="25" t="s">
@@ -12716,25 +12750,25 @@
       <c r="J12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="60" t="s">
         <v>17</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="60" t="s">
         <v>17</v>
       </c>
       <c r="R12" s="2" t="s">
@@ -12773,25 +12807,25 @@
       <c r="J13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="25" t="s">
+      <c r="K13" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="25" t="s">
+      <c r="M13" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O13" s="25" t="s">
+      <c r="O13" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q13" s="25" t="s">
+      <c r="Q13" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R13" s="25" t="s">
@@ -12828,25 +12862,25 @@
       <c r="J14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="25" t="s">
+      <c r="K14" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="25" t="s">
+      <c r="M14" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="25" t="s">
+      <c r="O14" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q14" s="25" t="s">
+      <c r="Q14" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R14" s="2" t="s">
@@ -12883,25 +12917,25 @@
       <c r="J15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="25" t="s">
+      <c r="K15" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="25" t="s">
+      <c r="M15" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O15" s="25" t="s">
+      <c r="O15" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q15" s="25" t="s">
+      <c r="Q15" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -12938,25 +12972,25 @@
       <c r="J16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="25" t="s">
+      <c r="K16" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="25" t="s">
+      <c r="M16" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O16" s="25" t="s">
+      <c r="O16" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q16" s="25" t="s">
+      <c r="Q16" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R16" s="2" t="s">
@@ -12993,25 +13027,25 @@
       <c r="J17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="O17" s="60" t="s">
         <v>17</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="Q17" s="60" t="s">
         <v>17</v>
       </c>
       <c r="R17" s="2" t="s">
@@ -13048,25 +13082,25 @@
       <c r="J18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="O18" s="60" t="s">
         <v>17</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="Q18" s="60" t="s">
         <v>17</v>
       </c>
       <c r="R18" s="2" t="s">
@@ -13103,25 +13137,25 @@
       <c r="J19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="O19" s="60" t="s">
         <v>17</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="Q19" s="60" t="s">
         <v>17</v>
       </c>
       <c r="R19" s="2" t="s">
@@ -13158,25 +13192,25 @@
       <c r="J20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M20" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="O20" s="60" t="s">
         <v>17</v>
       </c>
       <c r="P20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="Q20" s="60" t="s">
         <v>17</v>
       </c>
       <c r="R20" s="2" t="s">
@@ -13213,25 +13247,25 @@
       <c r="J21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="O21" s="60" t="s">
         <v>17</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="Q21" s="60" t="s">
         <v>17</v>
       </c>
       <c r="R21" s="2" t="s">
@@ -13270,25 +13304,25 @@
       <c r="J22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K22" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="M22" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="O22" s="60" t="s">
         <v>17</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="Q22" s="60" t="s">
         <v>17</v>
       </c>
       <c r="R22" s="2" t="s">
@@ -13325,25 +13359,25 @@
       <c r="J23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K23" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="M23" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="O23" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="Q23" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R23" s="25" t="s">
@@ -13380,25 +13414,25 @@
       <c r="J24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K24" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M24" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="O24" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="Q24" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R24" s="25" t="s">
@@ -13435,25 +13469,25 @@
       <c r="J25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K25" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="M25" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="O25" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q25" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R25" s="2" t="s">
@@ -13490,25 +13524,25 @@
       <c r="J26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="K26" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="M26" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="O26" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="Q26" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R26" s="1" t="s">
@@ -13547,25 +13581,25 @@
       <c r="J27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="K27" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="M27" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="O27" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="Q27" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R27" s="1" t="s">
@@ -13602,25 +13636,25 @@
       <c r="J28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="K28" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="M28" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="O28" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="Q28" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R28" s="2" t="s">
@@ -13657,25 +13691,25 @@
       <c r="J29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="K29" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="M29" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O29" s="1" t="s">
+      <c r="O29" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="Q29" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R29" s="2" t="s">
@@ -13714,25 +13748,25 @@
       <c r="J30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="K30" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="M30" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="O30" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="Q30" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R30" s="2" t="s">
@@ -13769,25 +13803,25 @@
       <c r="J31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="K31" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="M31" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="O31" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="Q31" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R31" s="2" t="s">
@@ -13824,25 +13858,25 @@
       <c r="J32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="K32" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="M32" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="O32" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="Q32" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R32" s="2" t="s">
@@ -13881,25 +13915,25 @@
       <c r="J33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="K33" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="M33" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="O33" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P33" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="25" t="s">
+      <c r="Q33" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R33" s="2" t="s">
@@ -13936,25 +13970,25 @@
       <c r="J34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="K34" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="M34" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="O34" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="Q34" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R34" s="2" t="s">
@@ -13991,25 +14025,25 @@
       <c r="J35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="K35" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M35" s="2" t="s">
+      <c r="M35" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O35" s="2" t="s">
+      <c r="O35" s="60" t="s">
         <v>17</v>
       </c>
       <c r="P35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="2" t="s">
+      <c r="Q35" s="60" t="s">
         <v>17</v>
       </c>
       <c r="R35" s="2" t="s">
@@ -14048,25 +14082,25 @@
       <c r="J36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="K36" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="M36" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N36" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="O36" s="25" t="s">
+      <c r="O36" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P36" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="25" t="s">
+      <c r="Q36" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R36" s="2" t="s">
@@ -14103,25 +14137,25 @@
       <c r="J37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K37" s="25" t="s">
+      <c r="K37" s="59" t="s">
         <v>17</v>
       </c>
       <c r="L37" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M37" s="25" t="s">
+      <c r="M37" s="59" t="s">
         <v>17</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O37" s="25" t="s">
+      <c r="O37" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="25" t="s">
+      <c r="Q37" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R37" s="2" t="s">
@@ -14158,25 +14192,25 @@
       <c r="J38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="K38" s="60" t="s">
         <v>17</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="M38" s="60" t="s">
         <v>17</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O38" s="25" t="s">
+      <c r="O38" s="59" t="s">
         <v>17</v>
       </c>
       <c r="P38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q38" s="25" t="s">
+      <c r="Q38" s="59" t="s">
         <v>17</v>
       </c>
       <c r="R38" s="2" t="s">
@@ -14187,57 +14221,57 @@
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
-      <c r="B39" s="3" t="s">
+      <c r="A39" s="57"/>
+      <c r="B39" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="1" t="s">
+      <c r="C39" s="57"/>
+      <c r="D39" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" s="1" t="s">
+      <c r="E39" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="K39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="L39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="M39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="N39" s="2" t="s">
+      <c r="N39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="O39" s="2" t="s">
+      <c r="O39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="P39" s="2" t="s">
+      <c r="P39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="Q39" s="2" t="s">
+      <c r="Q39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="R39" s="2" t="s">
+      <c r="R39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="S39" s="25" t="s">
+      <c r="S39" s="59" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add PHUSE US exercises
</commit_message>
<xml_diff>
--- a/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BC9A68-A313-E146-B07F-FD3860E5D663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489D5E6C-7E45-084B-8B5D-4A99440C88D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38620" yWindow="500" windowWidth="56420" windowHeight="27240" firstSheet="4" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="44980" yWindow="500" windowWidth="56420" windowHeight="27240" activeTab="13" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -4922,7 +4922,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5063,15 +5063,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5093,6 +5084,27 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7164,7 +7176,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A19" sqref="A19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7678,27 +7690,29 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="58" t="s">
         <v>324</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="59" t="s">
         <v>416</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="59" t="s">
         <v>416</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="60" t="s">
         <v>288</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="60" t="s">
         <v>417</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="60" t="s">
         <v>417</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="60" t="s">
         <v>289</v>
       </c>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
@@ -7870,8 +7884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8C14B1-8C62-2C45-8CB1-1E9EDDA367B1}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7925,22 +7939,22 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="50" t="s">
         <v>867</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="50" t="s">
         <v>869</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="50" t="s">
         <v>868</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="51" t="s">
         <v>870</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="50" t="s">
         <v>299</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="50" t="s">
         <v>871</v>
       </c>
     </row>
@@ -9819,7 +9833,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9930,19 +9944,19 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="56"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56" t="s">
+      <c r="A6" s="53"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53" t="s">
         <v>875</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="53" t="s">
         <v>310</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="53" t="s">
         <v>434</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="53" t="s">
         <v>241</v>
       </c>
     </row>
@@ -11022,7 +11036,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B12" sqref="B12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11037,144 +11051,144 @@
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="63" t="s">
         <v>536</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
     </row>
     <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="61" t="s">
         <v>421</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="62" t="s">
         <v>528</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>529</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="62" t="s">
         <v>530</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="64" t="s">
         <v>439</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -11373,7 +11387,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11483,10 +11497,10 @@
       <c r="E5" s="13" t="s">
         <v>810</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="52" t="s">
         <v>874</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="53" t="s">
         <v>429</v>
       </c>
     </row>
@@ -12166,8 +12180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12221,25 +12235,25 @@
       <c r="J1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="56" t="s">
         <v>360</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="56" t="s">
         <v>361</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="O1" s="59" t="s">
+      <c r="O1" s="56" t="s">
         <v>362</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="56" t="s">
         <v>366</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -12280,25 +12294,25 @@
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="60" t="s">
+      <c r="K2" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="60" t="s">
+      <c r="M2" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="60" t="s">
+      <c r="O2" s="57" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="60" t="s">
+      <c r="Q2" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R2" s="2" t="s">
@@ -12339,25 +12353,25 @@
       <c r="J3" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="K3" s="60" t="s">
+      <c r="K3" s="57" t="s">
         <v>363</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="M3" s="60" t="s">
+      <c r="M3" s="57" t="s">
         <v>364</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="O3" s="60" t="s">
+      <c r="O3" s="57" t="s">
         <v>365</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="Q3" s="60" t="s">
+      <c r="Q3" s="57" t="s">
         <v>367</v>
       </c>
       <c r="R3" s="2" t="s">
@@ -12394,25 +12408,25 @@
       <c r="J4" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="K4" s="60" t="s">
+      <c r="K4" s="57" t="s">
         <v>310</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="M4" s="60" t="s">
+      <c r="M4" s="57" t="s">
         <v>310</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="O4" s="60" t="s">
+      <c r="O4" s="57" t="s">
         <v>310</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="Q4" s="60" t="s">
+      <c r="Q4" s="57" t="s">
         <v>310</v>
       </c>
       <c r="R4" s="2" t="s">
@@ -12449,25 +12463,25 @@
       <c r="J5" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="56" t="s">
         <v>305</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="M5" s="59" t="s">
+      <c r="M5" s="56" t="s">
         <v>306</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="56" t="s">
         <v>307</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="Q5" s="59" t="s">
+      <c r="Q5" s="56" t="s">
         <v>308</v>
       </c>
       <c r="R5" s="9" t="s">
@@ -12483,10 +12497,10 @@
       <c r="C6" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="K6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="Q6" s="59"/>
+      <c r="K6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="Q6" s="56"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
@@ -12515,25 +12529,25 @@
       <c r="J7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="K7" s="59" t="s">
+      <c r="K7" s="56" t="s">
         <v>154</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="M7" s="59" t="s">
+      <c r="M7" s="56" t="s">
         <v>154</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="O7" s="59" t="s">
+      <c r="O7" s="56" t="s">
         <v>154</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="Q7" s="59" t="s">
+      <c r="Q7" s="56" t="s">
         <v>154</v>
       </c>
       <c r="R7" s="1" t="s">
@@ -12570,25 +12584,25 @@
       <c r="J8" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="59" t="s">
+      <c r="K8" s="56" t="s">
         <v>106</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="M8" s="59" t="s">
+      <c r="M8" s="56" t="s">
         <v>107</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O8" s="59" t="s">
+      <c r="O8" s="56" t="s">
         <v>108</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="Q8" s="59" t="s">
+      <c r="Q8" s="56" t="s">
         <v>110</v>
       </c>
       <c r="R8" s="1" t="s">
@@ -12608,10 +12622,10 @@
       <c r="C9" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="K9" s="59"/>
-      <c r="M9" s="59"/>
-      <c r="O9" s="59"/>
-      <c r="Q9" s="59"/>
+      <c r="K9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="Q9" s="56"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -12640,25 +12654,25 @@
       <c r="J10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="60" t="s">
+      <c r="K10" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="60" t="s">
+      <c r="M10" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O10" s="60" t="s">
+      <c r="O10" s="57" t="s">
         <v>17</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q10" s="60" t="s">
+      <c r="Q10" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R10" s="2" t="s">
@@ -12695,25 +12709,25 @@
       <c r="J11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="59" t="s">
+      <c r="K11" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="59" t="s">
+      <c r="M11" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="59" t="s">
+      <c r="O11" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q11" s="59" t="s">
+      <c r="Q11" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R11" s="25" t="s">
@@ -12750,25 +12764,25 @@
       <c r="J12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="60" t="s">
+      <c r="K12" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="60" t="s">
+      <c r="M12" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O12" s="60" t="s">
+      <c r="O12" s="57" t="s">
         <v>17</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q12" s="60" t="s">
+      <c r="Q12" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R12" s="2" t="s">
@@ -12783,7 +12797,7 @@
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="51" t="s">
         <v>873</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -12807,25 +12821,25 @@
       <c r="J13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="59" t="s">
+      <c r="K13" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="59" t="s">
+      <c r="M13" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O13" s="59" t="s">
+      <c r="O13" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q13" s="59" t="s">
+      <c r="Q13" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R13" s="25" t="s">
@@ -12862,25 +12876,25 @@
       <c r="J14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="59" t="s">
+      <c r="K14" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="59" t="s">
+      <c r="M14" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="59" t="s">
+      <c r="O14" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q14" s="59" t="s">
+      <c r="Q14" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R14" s="2" t="s">
@@ -12917,25 +12931,25 @@
       <c r="J15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="59" t="s">
+      <c r="K15" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="59" t="s">
+      <c r="M15" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O15" s="59" t="s">
+      <c r="O15" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q15" s="59" t="s">
+      <c r="Q15" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -12972,25 +12986,25 @@
       <c r="J16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="59" t="s">
+      <c r="K16" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="59" t="s">
+      <c r="M16" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="O16" s="59" t="s">
+      <c r="O16" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q16" s="59" t="s">
+      <c r="Q16" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R16" s="2" t="s">
@@ -13027,25 +13041,25 @@
       <c r="J17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="60" t="s">
+      <c r="K17" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="60" t="s">
+      <c r="M17" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O17" s="60" t="s">
+      <c r="O17" s="57" t="s">
         <v>17</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q17" s="60" t="s">
+      <c r="Q17" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R17" s="2" t="s">
@@ -13082,25 +13096,25 @@
       <c r="J18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="60" t="s">
+      <c r="K18" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M18" s="60" t="s">
+      <c r="M18" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="60" t="s">
+      <c r="O18" s="57" t="s">
         <v>17</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q18" s="60" t="s">
+      <c r="Q18" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R18" s="2" t="s">
@@ -13137,25 +13151,25 @@
       <c r="J19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="60" t="s">
+      <c r="K19" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M19" s="60" t="s">
+      <c r="M19" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O19" s="60" t="s">
+      <c r="O19" s="57" t="s">
         <v>17</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q19" s="60" t="s">
+      <c r="Q19" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R19" s="2" t="s">
@@ -13192,25 +13206,25 @@
       <c r="J20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="60" t="s">
+      <c r="K20" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M20" s="60" t="s">
+      <c r="M20" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O20" s="60" t="s">
+      <c r="O20" s="57" t="s">
         <v>17</v>
       </c>
       <c r="P20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q20" s="60" t="s">
+      <c r="Q20" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R20" s="2" t="s">
@@ -13247,25 +13261,25 @@
       <c r="J21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="60" t="s">
+      <c r="K21" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M21" s="60" t="s">
+      <c r="M21" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O21" s="60" t="s">
+      <c r="O21" s="57" t="s">
         <v>17</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q21" s="60" t="s">
+      <c r="Q21" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R21" s="2" t="s">
@@ -13304,25 +13318,25 @@
       <c r="J22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="60" t="s">
+      <c r="K22" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M22" s="60" t="s">
+      <c r="M22" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O22" s="60" t="s">
+      <c r="O22" s="57" t="s">
         <v>17</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q22" s="60" t="s">
+      <c r="Q22" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R22" s="2" t="s">
@@ -13359,25 +13373,25 @@
       <c r="J23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="59" t="s">
+      <c r="K23" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M23" s="59" t="s">
+      <c r="M23" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O23" s="59" t="s">
+      <c r="O23" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="59" t="s">
+      <c r="Q23" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R23" s="25" t="s">
@@ -13414,25 +13428,25 @@
       <c r="J24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="59" t="s">
+      <c r="K24" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M24" s="59" t="s">
+      <c r="M24" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O24" s="59" t="s">
+      <c r="O24" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="59" t="s">
+      <c r="Q24" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R24" s="25" t="s">
@@ -13469,25 +13483,25 @@
       <c r="J25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K25" s="59" t="s">
+      <c r="K25" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M25" s="59" t="s">
+      <c r="M25" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O25" s="59" t="s">
+      <c r="O25" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q25" s="59" t="s">
+      <c r="Q25" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R25" s="2" t="s">
@@ -13524,25 +13538,25 @@
       <c r="J26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="59" t="s">
+      <c r="K26" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M26" s="59" t="s">
+      <c r="M26" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O26" s="59" t="s">
+      <c r="O26" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="59" t="s">
+      <c r="Q26" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R26" s="1" t="s">
@@ -13581,25 +13595,25 @@
       <c r="J27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="59" t="s">
+      <c r="K27" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M27" s="59" t="s">
+      <c r="M27" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O27" s="59" t="s">
+      <c r="O27" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="59" t="s">
+      <c r="Q27" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R27" s="1" t="s">
@@ -13636,25 +13650,25 @@
       <c r="J28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K28" s="59" t="s">
+      <c r="K28" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M28" s="59" t="s">
+      <c r="M28" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O28" s="59" t="s">
+      <c r="O28" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q28" s="59" t="s">
+      <c r="Q28" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R28" s="2" t="s">
@@ -13691,25 +13705,25 @@
       <c r="J29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K29" s="59" t="s">
+      <c r="K29" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M29" s="59" t="s">
+      <c r="M29" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O29" s="59" t="s">
+      <c r="O29" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q29" s="59" t="s">
+      <c r="Q29" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R29" s="2" t="s">
@@ -13748,25 +13762,25 @@
       <c r="J30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K30" s="59" t="s">
+      <c r="K30" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M30" s="59" t="s">
+      <c r="M30" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O30" s="59" t="s">
+      <c r="O30" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q30" s="59" t="s">
+      <c r="Q30" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R30" s="2" t="s">
@@ -13803,25 +13817,25 @@
       <c r="J31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K31" s="59" t="s">
+      <c r="K31" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M31" s="59" t="s">
+      <c r="M31" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O31" s="59" t="s">
+      <c r="O31" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="59" t="s">
+      <c r="Q31" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R31" s="2" t="s">
@@ -13858,25 +13872,25 @@
       <c r="J32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="59" t="s">
+      <c r="K32" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M32" s="59" t="s">
+      <c r="M32" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O32" s="59" t="s">
+      <c r="O32" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q32" s="59" t="s">
+      <c r="Q32" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R32" s="2" t="s">
@@ -13915,25 +13929,25 @@
       <c r="J33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K33" s="59" t="s">
+      <c r="K33" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M33" s="59" t="s">
+      <c r="M33" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O33" s="59" t="s">
+      <c r="O33" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P33" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="59" t="s">
+      <c r="Q33" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R33" s="2" t="s">
@@ -13970,25 +13984,25 @@
       <c r="J34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K34" s="59" t="s">
+      <c r="K34" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M34" s="59" t="s">
+      <c r="M34" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O34" s="59" t="s">
+      <c r="O34" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q34" s="59" t="s">
+      <c r="Q34" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R34" s="2" t="s">
@@ -14025,25 +14039,25 @@
       <c r="J35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K35" s="60" t="s">
+      <c r="K35" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M35" s="60" t="s">
+      <c r="M35" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O35" s="60" t="s">
+      <c r="O35" s="57" t="s">
         <v>17</v>
       </c>
       <c r="P35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="60" t="s">
+      <c r="Q35" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R35" s="2" t="s">
@@ -14082,25 +14096,25 @@
       <c r="J36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K36" s="60" t="s">
+      <c r="K36" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M36" s="60" t="s">
+      <c r="M36" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N36" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="O36" s="59" t="s">
+      <c r="O36" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P36" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="59" t="s">
+      <c r="Q36" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R36" s="2" t="s">
@@ -14137,25 +14151,25 @@
       <c r="J37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K37" s="59" t="s">
+      <c r="K37" s="56" t="s">
         <v>17</v>
       </c>
       <c r="L37" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M37" s="59" t="s">
+      <c r="M37" s="56" t="s">
         <v>17</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O37" s="59" t="s">
+      <c r="O37" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="59" t="s">
+      <c r="Q37" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R37" s="2" t="s">
@@ -14192,25 +14206,25 @@
       <c r="J38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K38" s="60" t="s">
+      <c r="K38" s="57" t="s">
         <v>17</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M38" s="60" t="s">
+      <c r="M38" s="57" t="s">
         <v>17</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O38" s="59" t="s">
+      <c r="O38" s="56" t="s">
         <v>17</v>
       </c>
       <c r="P38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q38" s="59" t="s">
+      <c r="Q38" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R38" s="2" t="s">
@@ -14221,57 +14235,57 @@
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="57"/>
-      <c r="B39" s="58" t="s">
+      <c r="A39" s="54"/>
+      <c r="B39" s="55" t="s">
         <v>171</v>
       </c>
-      <c r="C39" s="57"/>
-      <c r="D39" s="59" t="s">
+      <c r="C39" s="54"/>
+      <c r="D39" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" s="59" t="s">
+      <c r="E39" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="G39" s="60" t="s">
+      <c r="G39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="60" t="s">
+      <c r="H39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="I39" s="60" t="s">
+      <c r="I39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="J39" s="60" t="s">
+      <c r="J39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="K39" s="60" t="s">
+      <c r="K39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="L39" s="60" t="s">
+      <c r="L39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="M39" s="60" t="s">
+      <c r="M39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="N39" s="60" t="s">
+      <c r="N39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="O39" s="60" t="s">
+      <c r="O39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="P39" s="60" t="s">
+      <c r="P39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="Q39" s="60" t="s">
+      <c r="Q39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="R39" s="60" t="s">
+      <c r="R39" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="S39" s="59" t="s">
+      <c r="S39" s="56" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>